<commit_message>
/home/ofenloch/workspaces/COVID19/rki-data-evaluation/getRKIData.sh: add data automatically downloaded at 2021-04-06--20-21-33
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Klinische-Aspekte.xlsx
+++ b/rki-data/RKI-Klinische-Aspekte.xlsx
@@ -1,19 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Wissdaten\RKI_nCoV-Lage\3.Kommunikation\3.7.Lageberichte\2021-03-30\Webmaster_Tabellen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB86D14-DF6A-4948-B9DA-DFA5950DEC03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1151A2C-946E-4FDA-8B34-C4568813227A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="1" xr2:uid="{7A96F809-61A3-46BE-921C-258450650152}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6225" xr2:uid="{DB775562-523C-43F7-B3D3-B72E2874F045}"/>
   </bookViews>
   <sheets>
-    <sheet name="Klinische Aspekte" sheetId="1" r:id="rId1"/>
+    <sheet name="Klinischer Aspekte" sheetId="1" r:id="rId1"/>
     <sheet name="Fälle_Hospitalisierung_Alter" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
   <si>
     <t>Meldejahr</t>
   </si>
@@ -67,6 +62,108 @@
     <t>Anteil Verstorben</t>
   </si>
   <si>
+    <t>Die dem RKI übermittelte COVID-19-Fälle nach Meldewoche und  Geschlecht sowie Anteile mit für COVID-19 relevanten Symptomen, Anteile Hospitalisierter und Verstorbener für die Meldewochen KW 10 – 53/2020 und KW 01 - 12/2021</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Meldewoche</t>
+  </si>
+  <si>
     <t>0 - 4 Jährige</t>
   </si>
   <si>
@@ -83,105 +180,6 @@
   </si>
   <si>
     <t>80+ Jährige</t>
-  </si>
-  <si>
-    <t>Meldewoche</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>Die dem RKI übermittelte COVID-19-Fälle nach Meldewoche und  Geschlecht sowie Anteile mit für COVID-19 relevanten Symptomen, Anteile Hospitalisierter und Verstorbener für die Meldewochen KW 10 – 53/2020 und KW 01 - 12/2021</t>
-  </si>
-  <si>
-    <t>12</t>
   </si>
 </sst>
 </file>
@@ -361,7 +359,9 @@
     <xf numFmtId="10" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -675,18 +675,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B954E3B8-F82B-4D64-BB14-6BD6AE52A778}">
-  <dimension ref="A1:M58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED98BD9-4AB5-4844-ABD1-68F2C3D62B46}">
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:M58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -738,16 +738,16 @@
         <v>10</v>
       </c>
       <c r="C3" s="5">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="D3" s="5">
         <v>43</v>
       </c>
       <c r="E3" s="6">
-        <v>0.53072625698324027</v>
+        <v>0.52954292084726873</v>
       </c>
       <c r="F3" s="6">
-        <v>0.46927374301675978</v>
+        <v>0.47045707915273133</v>
       </c>
       <c r="G3" s="7">
         <v>836</v>
@@ -756,19 +756,19 @@
         <v>8.3732057416267949E-2</v>
       </c>
       <c r="I3" s="5">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="J3" s="9">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="K3" s="6">
-        <v>0.20074349442379183</v>
+        <v>0.20395550061804696</v>
       </c>
       <c r="L3" s="9">
         <v>12</v>
       </c>
       <c r="M3" s="10">
-        <v>1.3407821219999999E-2</v>
+        <v>1.337792642E-2</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -779,37 +779,37 @@
         <v>11</v>
       </c>
       <c r="C4" s="12">
-        <v>6431</v>
+        <v>6434</v>
       </c>
       <c r="D4" s="13">
         <v>45</v>
       </c>
       <c r="E4" s="14">
-        <v>0.56276248250116656</v>
+        <v>0.56281094527363185</v>
       </c>
       <c r="F4" s="14">
-        <v>0.43723751749883338</v>
+        <v>0.43718905472636815</v>
       </c>
       <c r="G4" s="12">
-        <v>5771</v>
+        <v>5770</v>
       </c>
       <c r="H4" s="15">
-        <v>5.3023739386588116E-2</v>
+        <v>5.3206239168110916E-2</v>
       </c>
       <c r="I4" s="12">
-        <v>5631</v>
+        <v>5636</v>
       </c>
       <c r="J4" s="13">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="K4" s="14">
-        <v>9.394423725803587E-2</v>
+        <v>9.4570617459190917E-2</v>
       </c>
       <c r="L4" s="13">
         <v>85</v>
       </c>
       <c r="M4" s="16">
-        <v>1.321722904E-2</v>
+        <v>1.3211066210000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -820,37 +820,37 @@
         <v>12</v>
       </c>
       <c r="C5" s="7">
-        <v>22440</v>
+        <v>22447</v>
       </c>
       <c r="D5" s="5">
         <v>45</v>
       </c>
       <c r="E5" s="6">
-        <v>0.54993757802746568</v>
+        <v>0.54998885669712505</v>
       </c>
       <c r="F5" s="6">
-        <v>0.45006242197253432</v>
+        <v>0.45001114330287495</v>
       </c>
       <c r="G5" s="7">
-        <v>20197</v>
+        <v>20191</v>
       </c>
       <c r="H5" s="8">
-        <v>3.8966183096499483E-2</v>
+        <v>3.8928235352384724E-2</v>
       </c>
       <c r="I5" s="7">
-        <v>19396</v>
+        <v>19407</v>
       </c>
       <c r="J5" s="7">
-        <v>2218</v>
+        <v>2232</v>
       </c>
       <c r="K5" s="6">
-        <v>0.11435347494328728</v>
+        <v>0.1150100479208533</v>
       </c>
       <c r="L5" s="5">
         <v>478</v>
       </c>
       <c r="M5" s="10">
-        <v>2.130124777E-2</v>
+        <v>2.1294605059999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -861,37 +861,37 @@
         <v>13</v>
       </c>
       <c r="C6" s="12">
-        <v>33999</v>
+        <v>33993</v>
       </c>
       <c r="D6" s="13">
         <v>48</v>
       </c>
       <c r="E6" s="14">
-        <v>0.49501133119463164</v>
+        <v>0.49501015631899675</v>
       </c>
       <c r="F6" s="14">
-        <v>0.5049886688053683</v>
+        <v>0.5049898436810033</v>
       </c>
       <c r="G6" s="12">
-        <v>30856</v>
+        <v>30845</v>
       </c>
       <c r="H6" s="15">
-        <v>3.2927145449831476E-2</v>
+        <v>3.2938887988328738E-2</v>
       </c>
       <c r="I6" s="12">
-        <v>29541</v>
+        <v>29538</v>
       </c>
       <c r="J6" s="12">
-        <v>5137</v>
+        <v>5148</v>
       </c>
       <c r="K6" s="14">
-        <v>0.1738939101587624</v>
+        <v>0.17428397318708105</v>
       </c>
       <c r="L6" s="12">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="M6" s="16">
-        <v>4.3118915260000001E-2</v>
+        <v>4.3097108219999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -902,37 +902,37 @@
         <v>14</v>
       </c>
       <c r="C7" s="7">
-        <v>36083</v>
+        <v>36080</v>
       </c>
       <c r="D7" s="5">
         <v>51</v>
       </c>
       <c r="E7" s="6">
-        <v>0.45070031895714879</v>
+        <v>0.45065461000776658</v>
       </c>
       <c r="F7" s="6">
-        <v>0.54929968104285121</v>
+        <v>0.54934538999223348</v>
       </c>
       <c r="G7" s="7">
-        <v>32068</v>
+        <v>32056</v>
       </c>
       <c r="H7" s="8">
-        <v>5.5475863789447424E-2</v>
+        <v>5.5496630895932118E-2</v>
       </c>
       <c r="I7" s="7">
-        <v>31637</v>
+        <v>31636</v>
       </c>
       <c r="J7" s="7">
-        <v>6086</v>
+        <v>6094</v>
       </c>
       <c r="K7" s="6">
-        <v>0.19236969371305748</v>
+        <v>0.19262865090403339</v>
       </c>
       <c r="L7" s="7">
-        <v>2258</v>
+        <v>2259</v>
       </c>
       <c r="M7" s="10">
-        <v>6.2577945290000006E-2</v>
+        <v>6.2610864739999994E-2</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -943,37 +943,37 @@
         <v>15</v>
       </c>
       <c r="C8" s="12">
-        <v>27181</v>
+        <v>27185</v>
       </c>
       <c r="D8" s="13">
         <v>52</v>
       </c>
       <c r="E8" s="14">
-        <v>0.43494916752615292</v>
+        <v>0.43488509133765468</v>
       </c>
       <c r="F8" s="14">
-        <v>0.56505083247384702</v>
+        <v>0.56511490866234526</v>
       </c>
       <c r="G8" s="12">
-        <v>23607</v>
+        <v>23603</v>
       </c>
       <c r="H8" s="15">
-        <v>8.4593552759774648E-2</v>
+        <v>8.4607888827691394E-2</v>
       </c>
       <c r="I8" s="12">
-        <v>24163</v>
+        <v>24170</v>
       </c>
       <c r="J8" s="12">
-        <v>4726</v>
+        <v>4735</v>
       </c>
       <c r="K8" s="14">
-        <v>0.19558829615527873</v>
+        <v>0.19590401323955317</v>
       </c>
       <c r="L8" s="12">
-        <v>1879</v>
+        <v>1880</v>
       </c>
       <c r="M8" s="16">
-        <v>6.9129171109999998E-2</v>
+        <v>6.9155784430000006E-2</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -984,37 +984,37 @@
         <v>16</v>
       </c>
       <c r="C9" s="7">
-        <v>17365</v>
+        <v>17360</v>
       </c>
       <c r="D9" s="5">
         <v>51</v>
       </c>
       <c r="E9" s="6">
-        <v>0.44719243629655253</v>
+        <v>0.44732137708321318</v>
       </c>
       <c r="F9" s="6">
-        <v>0.55280756370344752</v>
+        <v>0.55267862291678682</v>
       </c>
       <c r="G9" s="7">
-        <v>14890</v>
+        <v>14884</v>
       </c>
       <c r="H9" s="8">
-        <v>0.1145063801208865</v>
+        <v>0.11455253963988175</v>
       </c>
       <c r="I9" s="7">
         <v>15541</v>
       </c>
       <c r="J9" s="7">
-        <v>3374</v>
+        <v>3381</v>
       </c>
       <c r="K9" s="6">
-        <v>0.21710314651566823</v>
+        <v>0.21755356798146838</v>
       </c>
       <c r="L9" s="7">
         <v>1217</v>
       </c>
       <c r="M9" s="10">
-        <v>7.0083501290000003E-2</v>
+        <v>7.0103686629999995E-2</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1025,37 +1025,37 @@
         <v>17</v>
       </c>
       <c r="C10" s="12">
-        <v>12375</v>
+        <v>12379</v>
       </c>
       <c r="D10" s="13">
         <v>50</v>
       </c>
       <c r="E10" s="14">
-        <v>0.44966823110535686</v>
+        <v>0.44968451706843554</v>
       </c>
       <c r="F10" s="14">
-        <v>0.55033176889464319</v>
+        <v>0.55031548293156451</v>
       </c>
       <c r="G10" s="12">
-        <v>10284</v>
+        <v>10282</v>
       </c>
       <c r="H10" s="15">
-        <v>0.13905095293660055</v>
+        <v>0.13907800038902937</v>
       </c>
       <c r="I10" s="12">
-        <v>10993</v>
+        <v>10998</v>
       </c>
       <c r="J10" s="12">
-        <v>2235</v>
+        <v>2241</v>
       </c>
       <c r="K10" s="14">
-        <v>0.20331119803511324</v>
+        <v>0.20376432078559739</v>
       </c>
       <c r="L10" s="13">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="M10" s="16">
-        <v>5.8181818179999997E-2</v>
+        <v>5.8243799979999997E-2</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1066,37 +1066,37 @@
         <v>18</v>
       </c>
       <c r="C11" s="7">
-        <v>7444</v>
+        <v>7441</v>
       </c>
       <c r="D11" s="5">
         <v>48</v>
       </c>
       <c r="E11" s="6">
-        <v>0.47761795940314561</v>
+        <v>0.47767616998386231</v>
       </c>
       <c r="F11" s="6">
-        <v>0.52238204059685445</v>
+        <v>0.52232383001613769</v>
       </c>
       <c r="G11" s="7">
-        <v>6259</v>
+        <v>6258</v>
       </c>
       <c r="H11" s="8">
-        <v>0.17558715449752357</v>
+        <v>0.17561521252796419</v>
       </c>
       <c r="I11" s="7">
-        <v>6612</v>
+        <v>6611</v>
       </c>
       <c r="J11" s="7">
-        <v>1362</v>
+        <v>1365</v>
       </c>
       <c r="K11" s="6">
-        <v>0.20598911070780399</v>
+        <v>0.20647405838753594</v>
       </c>
       <c r="L11" s="5">
         <v>386</v>
       </c>
       <c r="M11" s="10">
-        <v>5.1853842019999999E-2</v>
+        <v>5.1874748009999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1107,37 +1107,37 @@
         <v>19</v>
       </c>
       <c r="C12" s="12">
-        <v>6239</v>
+        <v>6240</v>
       </c>
       <c r="D12" s="13">
         <v>47</v>
       </c>
       <c r="E12" s="14">
-        <v>0.48002566982191563</v>
+        <v>0.48010907924286172</v>
       </c>
       <c r="F12" s="14">
-        <v>0.51997433017808437</v>
+        <v>0.51989092075713828</v>
       </c>
       <c r="G12" s="12">
-        <v>5248</v>
+        <v>5249</v>
       </c>
       <c r="H12" s="15">
-        <v>0.19645579268292682</v>
+        <v>0.19603734044579921</v>
       </c>
       <c r="I12" s="12">
-        <v>5632</v>
+        <v>5633</v>
       </c>
       <c r="J12" s="12">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="K12" s="14">
-        <v>0.19176136363636365</v>
+        <v>0.19208237173797266</v>
       </c>
       <c r="L12" s="13">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M12" s="16">
-        <v>4.1032216699999999E-2</v>
+        <v>4.118589743E-2</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1148,37 +1148,37 @@
         <v>20</v>
       </c>
       <c r="C13" s="7">
-        <v>4758</v>
+        <v>4768</v>
       </c>
       <c r="D13" s="5">
         <v>45</v>
       </c>
       <c r="E13" s="6">
-        <v>0.49452861952861954</v>
+        <v>0.49475010499790006</v>
       </c>
       <c r="F13" s="6">
-        <v>0.50547138047138052</v>
+        <v>0.50524989500209994</v>
       </c>
       <c r="G13" s="7">
-        <v>3953</v>
+        <v>3952</v>
       </c>
       <c r="H13" s="8">
-        <v>0.23096382494308121</v>
+        <v>0.23102226720647773</v>
       </c>
       <c r="I13" s="7">
-        <v>4235</v>
+        <v>4250</v>
       </c>
       <c r="J13" s="5">
-        <v>750</v>
+        <v>766</v>
       </c>
       <c r="K13" s="6">
-        <v>0.17709563164108619</v>
+        <v>0.18023529411764705</v>
       </c>
       <c r="L13" s="5">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M13" s="10">
-        <v>3.4258091630000001E-2</v>
+        <v>3.4395973150000002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1189,37 +1189,37 @@
         <v>21</v>
       </c>
       <c r="C14" s="12">
-        <v>3621</v>
+        <v>3613</v>
       </c>
       <c r="D14" s="13">
         <v>43</v>
       </c>
       <c r="E14" s="14">
-        <v>0.50277161862527719</v>
+        <v>0.50277623542476402</v>
       </c>
       <c r="F14" s="14">
-        <v>0.49722838137472286</v>
+        <v>0.49722376457523598</v>
       </c>
       <c r="G14" s="12">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="H14" s="15">
-        <v>0.26313932980599647</v>
+        <v>0.26323218066337334</v>
       </c>
       <c r="I14" s="12">
         <v>3122</v>
       </c>
       <c r="J14" s="13">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="K14" s="14">
-        <v>0.16463805253042921</v>
+        <v>0.16495836002562461</v>
       </c>
       <c r="L14" s="13">
         <v>113</v>
       </c>
       <c r="M14" s="16">
-        <v>3.1206848929999999E-2</v>
+        <v>3.1275947960000001E-2</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1230,37 +1230,37 @@
         <v>22</v>
       </c>
       <c r="C15" s="7">
-        <v>3205</v>
+        <v>3204</v>
       </c>
       <c r="D15" s="5">
         <v>42</v>
       </c>
       <c r="E15" s="6">
-        <v>0.51581584716567497</v>
+        <v>0.51566416040100249</v>
       </c>
       <c r="F15" s="6">
-        <v>0.48418415283432509</v>
+        <v>0.48433583959899751</v>
       </c>
       <c r="G15" s="7">
-        <v>2547</v>
+        <v>2545</v>
       </c>
       <c r="H15" s="8">
-        <v>0.23164507263447193</v>
+        <v>0.23182711198428291</v>
       </c>
       <c r="I15" s="7">
-        <v>2769</v>
+        <v>2768</v>
       </c>
       <c r="J15" s="5">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="K15" s="6">
-        <v>0.15131816540267246</v>
+        <v>0.15209537572254336</v>
       </c>
       <c r="L15" s="5">
         <v>65</v>
       </c>
       <c r="M15" s="10">
-        <v>2.0280811230000001E-2</v>
+        <v>2.028714107E-2</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1476,16 +1476,16 @@
         <v>28</v>
       </c>
       <c r="C21" s="7">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="D21" s="5">
         <v>36</v>
       </c>
       <c r="E21" s="6">
-        <v>0.55963681386710684</v>
+        <v>0.5590421139554087</v>
       </c>
       <c r="F21" s="6">
-        <v>0.4403631861328931</v>
+        <v>0.44095788604459124</v>
       </c>
       <c r="G21" s="7">
         <v>1934</v>
@@ -1494,19 +1494,19 @@
         <v>0.23888314374353672</v>
       </c>
       <c r="I21" s="7">
-        <v>2195</v>
+        <v>2193</v>
       </c>
       <c r="J21" s="5">
         <v>256</v>
       </c>
       <c r="K21" s="6">
-        <v>0.11662870159453304</v>
+        <v>0.11673506611947104</v>
       </c>
       <c r="L21" s="5">
         <v>25</v>
       </c>
       <c r="M21" s="10">
-        <v>1.029654036E-2</v>
+        <v>1.0300782850000001E-2</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1517,16 +1517,16 @@
         <v>29</v>
       </c>
       <c r="C22" s="12">
-        <v>3015</v>
+        <v>3016</v>
       </c>
       <c r="D22" s="13">
         <v>36</v>
       </c>
       <c r="E22" s="14">
-        <v>0.52493351063829785</v>
+        <v>0.52509139248919912</v>
       </c>
       <c r="F22" s="14">
-        <v>0.47506648936170215</v>
+        <v>0.47490860751080094</v>
       </c>
       <c r="G22" s="12">
         <v>2358</v>
@@ -1535,19 +1535,19 @@
         <v>0.22943172179813401</v>
       </c>
       <c r="I22" s="12">
-        <v>2646</v>
+        <v>2647</v>
       </c>
       <c r="J22" s="13">
         <v>318</v>
       </c>
       <c r="K22" s="14">
-        <v>0.12018140589569161</v>
+        <v>0.12013600302228938</v>
       </c>
       <c r="L22" s="13">
         <v>30</v>
       </c>
       <c r="M22" s="16">
-        <v>9.9502487499999997E-3</v>
+        <v>9.9469495999999994E-3</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1558,22 +1558,22 @@
         <v>30</v>
       </c>
       <c r="C23" s="7">
-        <v>3929</v>
+        <v>3928</v>
       </c>
       <c r="D23" s="5">
         <v>36</v>
       </c>
       <c r="E23" s="6">
-        <v>0.52334779280428678</v>
+        <v>0.52322613578356303</v>
       </c>
       <c r="F23" s="6">
-        <v>0.47665220719571322</v>
+        <v>0.47677386421643697</v>
       </c>
       <c r="G23" s="7">
         <v>3182</v>
       </c>
       <c r="H23" s="8">
-        <v>0.27435575109993715</v>
+        <v>0.27372721558768071</v>
       </c>
       <c r="I23" s="7">
         <v>3477</v>
@@ -1588,7 +1588,7 @@
         <v>33</v>
       </c>
       <c r="M23" s="10">
-        <v>8.3990837299999996E-3</v>
+        <v>8.4012219900000008E-3</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1599,37 +1599,37 @@
         <v>31</v>
       </c>
       <c r="C24" s="12">
-        <v>4817</v>
+        <v>4822</v>
       </c>
       <c r="D24" s="13">
         <v>36</v>
       </c>
       <c r="E24" s="14">
-        <v>0.50270382695507487</v>
+        <v>0.5021815915229586</v>
       </c>
       <c r="F24" s="14">
-        <v>0.49729617304492513</v>
+        <v>0.49781840847704134</v>
       </c>
       <c r="G24" s="12">
-        <v>3705</v>
+        <v>3713</v>
       </c>
       <c r="H24" s="15">
-        <v>0.24561403508771928</v>
+        <v>0.24562348505251819</v>
       </c>
       <c r="I24" s="12">
-        <v>4166</v>
+        <v>4175</v>
       </c>
       <c r="J24" s="13">
         <v>389</v>
       </c>
       <c r="K24" s="14">
-        <v>9.3374939990398462E-2</v>
+        <v>9.3173652694610781E-2</v>
       </c>
       <c r="L24" s="13">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M24" s="16">
-        <v>6.4355407900000003E-3</v>
+        <v>6.6362505100000004E-3</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1640,37 +1640,37 @@
         <v>32</v>
       </c>
       <c r="C25" s="7">
-        <v>6056</v>
+        <v>6057</v>
       </c>
       <c r="D25" s="5">
         <v>34</v>
       </c>
       <c r="E25" s="6">
-        <v>0.53671849156467089</v>
+        <v>0.53662973375227385</v>
       </c>
       <c r="F25" s="6">
-        <v>0.46328150843532917</v>
+        <v>0.46337026624772615</v>
       </c>
       <c r="G25" s="7">
-        <v>4549</v>
+        <v>4552</v>
       </c>
       <c r="H25" s="8">
-        <v>0.29984612002637945</v>
+        <v>0.30008787346221444</v>
       </c>
       <c r="I25" s="7">
-        <v>5283</v>
+        <v>5286</v>
       </c>
       <c r="J25" s="5">
         <v>399</v>
       </c>
       <c r="K25" s="6">
-        <v>7.5525269733106193E-2</v>
+        <v>7.5482406356413165E-2</v>
       </c>
       <c r="L25" s="5">
         <v>31</v>
       </c>
       <c r="M25" s="10">
-        <v>5.1188903500000004E-3</v>
+        <v>5.1180452299999998E-3</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1687,25 +1687,25 @@
         <v>32</v>
       </c>
       <c r="E26" s="14">
-        <v>0.5339720156309089</v>
+        <v>0.53409807134753562</v>
       </c>
       <c r="F26" s="14">
-        <v>0.46602798436909115</v>
+        <v>0.46590192865246438</v>
       </c>
       <c r="G26" s="12">
-        <v>5851</v>
+        <v>5854</v>
       </c>
       <c r="H26" s="15">
-        <v>0.33242180823790807</v>
+        <v>0.33259309873590709</v>
       </c>
       <c r="I26" s="12">
-        <v>7007</v>
+        <v>7009</v>
       </c>
       <c r="J26" s="13">
         <v>438</v>
       </c>
       <c r="K26" s="14">
-        <v>6.2508919651776795E-2</v>
+        <v>6.2491082893422742E-2</v>
       </c>
       <c r="L26" s="13">
         <v>30</v>
@@ -1734,19 +1734,19 @@
         <v>0.45270553691275167</v>
       </c>
       <c r="G27" s="7">
-        <v>7202</v>
+        <v>7203</v>
       </c>
       <c r="H27" s="8">
-        <v>0.34559844487642322</v>
+        <v>0.34555046508399279</v>
       </c>
       <c r="I27" s="7">
-        <v>8307</v>
+        <v>8309</v>
       </c>
       <c r="J27" s="5">
         <v>434</v>
       </c>
       <c r="K27" s="6">
-        <v>5.2245094498615627E-2</v>
+        <v>5.2232518955349617E-2</v>
       </c>
       <c r="L27" s="5">
         <v>30</v>
@@ -1763,37 +1763,37 @@
         <v>35</v>
       </c>
       <c r="C28" s="12">
-        <v>8821</v>
+        <v>8820</v>
       </c>
       <c r="D28" s="13">
         <v>32</v>
       </c>
       <c r="E28" s="14">
-        <v>0.53074027603513174</v>
+        <v>0.53102897558749718</v>
       </c>
       <c r="F28" s="14">
-        <v>0.46925972396486826</v>
+        <v>0.46897102441250288</v>
       </c>
       <c r="G28" s="12">
-        <v>6872</v>
+        <v>6874</v>
       </c>
       <c r="H28" s="15">
-        <v>0.30733410942956929</v>
+        <v>0.30724469013674716</v>
       </c>
       <c r="I28" s="12">
-        <v>7425</v>
+        <v>7427</v>
       </c>
       <c r="J28" s="13">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K28" s="14">
-        <v>4.9427609427609424E-2</v>
+        <v>4.9279655311700553E-2</v>
       </c>
       <c r="L28" s="13">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M28" s="16">
-        <v>2.1539507899999998E-3</v>
+        <v>2.04081632E-3</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1804,37 +1804,37 @@
         <v>36</v>
       </c>
       <c r="C29" s="7">
-        <v>8619</v>
+        <v>8620</v>
       </c>
       <c r="D29" s="5">
         <v>33</v>
       </c>
       <c r="E29" s="6">
-        <v>0.53650571495218102</v>
+        <v>0.53655976676384842</v>
       </c>
       <c r="F29" s="6">
-        <v>0.46349428504781898</v>
+        <v>0.46344023323615158</v>
       </c>
       <c r="G29" s="7">
-        <v>6656</v>
+        <v>6657</v>
       </c>
       <c r="H29" s="8">
-        <v>0.27178485576923078</v>
+        <v>0.27174402884182064</v>
       </c>
       <c r="I29" s="7">
-        <v>7085</v>
+        <v>7086</v>
       </c>
       <c r="J29" s="5">
         <v>397</v>
       </c>
       <c r="K29" s="6">
-        <v>5.6033874382498239E-2</v>
+        <v>5.6025966694891335E-2</v>
       </c>
       <c r="L29" s="5">
         <v>36</v>
       </c>
       <c r="M29" s="10">
-        <v>4.1768186499999997E-3</v>
+        <v>4.1763340999999999E-3</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1845,16 +1845,16 @@
         <v>37</v>
       </c>
       <c r="C30" s="12">
-        <v>9773</v>
+        <v>9771</v>
       </c>
       <c r="D30" s="13">
         <v>35</v>
       </c>
       <c r="E30" s="14">
-        <v>0.5182556824025506</v>
+        <v>0.51795082810410453</v>
       </c>
       <c r="F30" s="14">
-        <v>0.48174431759744935</v>
+        <v>0.48204917189589547</v>
       </c>
       <c r="G30" s="12">
         <v>7606</v>
@@ -1863,19 +1863,19 @@
         <v>0.20496976071522482</v>
       </c>
       <c r="I30" s="12">
-        <v>8035</v>
+        <v>8037</v>
       </c>
       <c r="J30" s="13">
         <v>464</v>
       </c>
       <c r="K30" s="14">
-        <v>5.7747355320472933E-2</v>
+        <v>5.7732984944631083E-2</v>
       </c>
       <c r="L30" s="13">
         <v>66</v>
       </c>
       <c r="M30" s="16">
-        <v>6.7532998999999998E-3</v>
+        <v>6.7546822199999997E-3</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1886,37 +1886,37 @@
         <v>38</v>
       </c>
       <c r="C31" s="7">
-        <v>12294</v>
+        <v>12296</v>
       </c>
       <c r="D31" s="5">
         <v>36</v>
       </c>
       <c r="E31" s="6">
-        <v>0.51214128035320083</v>
+        <v>0.51222104144527103</v>
       </c>
       <c r="F31" s="6">
-        <v>0.48785871964679911</v>
+        <v>0.48777895855472903</v>
       </c>
       <c r="G31" s="7">
-        <v>9765</v>
+        <v>9768</v>
       </c>
       <c r="H31" s="8">
-        <v>0.18689196108550948</v>
+        <v>0.18693693693693694</v>
       </c>
       <c r="I31" s="7">
-        <v>10062</v>
+        <v>10069</v>
       </c>
       <c r="J31" s="5">
         <v>674</v>
       </c>
       <c r="K31" s="6">
-        <v>6.6984694891671637E-2</v>
+        <v>6.6938126924222865E-2</v>
       </c>
       <c r="L31" s="5">
         <v>79</v>
       </c>
       <c r="M31" s="10">
-        <v>6.4258988100000004E-3</v>
+        <v>6.4248536099999996E-3</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1933,25 +1933,25 @@
         <v>37</v>
       </c>
       <c r="E32" s="14">
-        <v>0.51634741133933382</v>
+        <v>0.51642434033387186</v>
       </c>
       <c r="F32" s="14">
-        <v>0.48365258866066618</v>
+        <v>0.48357565966612814</v>
       </c>
       <c r="G32" s="12">
-        <v>10359</v>
+        <v>10361</v>
       </c>
       <c r="H32" s="15">
-        <v>0.18196737136789265</v>
+        <v>0.18193224592220827</v>
       </c>
       <c r="I32" s="12">
-        <v>10849</v>
+        <v>10852</v>
       </c>
       <c r="J32" s="13">
         <v>771</v>
       </c>
       <c r="K32" s="14">
-        <v>7.1066457738040378E-2</v>
+        <v>7.1046811647622554E-2</v>
       </c>
       <c r="L32" s="13">
         <v>107</v>
@@ -1968,37 +1968,37 @@
         <v>40</v>
       </c>
       <c r="C33" s="7">
-        <v>15930</v>
+        <v>15932</v>
       </c>
       <c r="D33" s="5">
         <v>38</v>
       </c>
       <c r="E33" s="6">
-        <v>0.51942572885838423</v>
+        <v>0.51936032235723728</v>
       </c>
       <c r="F33" s="6">
-        <v>0.48057427114161577</v>
+        <v>0.48063967764276272</v>
       </c>
       <c r="G33" s="7">
-        <v>12605</v>
+        <v>12610</v>
       </c>
       <c r="H33" s="8">
-        <v>0.17564458548195161</v>
+        <v>0.17573354480570974</v>
       </c>
       <c r="I33" s="7">
-        <v>13474</v>
+        <v>13480</v>
       </c>
       <c r="J33" s="5">
         <v>873</v>
       </c>
       <c r="K33" s="6">
-        <v>6.4791450200385931E-2</v>
+        <v>6.4762611275964388E-2</v>
       </c>
       <c r="L33" s="5">
         <v>121</v>
       </c>
       <c r="M33" s="10">
-        <v>7.5957313200000001E-3</v>
+        <v>7.5947777999999999E-3</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2009,37 +2009,37 @@
         <v>41</v>
       </c>
       <c r="C34" s="19">
-        <v>26126</v>
+        <v>26128</v>
       </c>
       <c r="D34" s="20">
         <v>39</v>
       </c>
       <c r="E34" s="21">
-        <v>0.51037264694583173</v>
+        <v>0.51044867854947762</v>
       </c>
       <c r="F34" s="21">
-        <v>0.48962735305416827</v>
+        <v>0.48955132145052244</v>
       </c>
       <c r="G34" s="19">
-        <v>20089</v>
+        <v>20102</v>
       </c>
       <c r="H34" s="22">
-        <v>0.16616058539499229</v>
+        <v>0.16635160680529301</v>
       </c>
       <c r="I34" s="19">
-        <v>21537</v>
+        <v>21545</v>
       </c>
       <c r="J34" s="20">
         <v>1586</v>
       </c>
       <c r="K34" s="21">
-        <v>7.364071133398338E-2</v>
+        <v>7.3613367370619631E-2</v>
       </c>
       <c r="L34" s="20">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M34" s="23">
-        <v>9.1479751899999993E-3</v>
+        <v>9.1090018299999995E-3</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2050,37 +2050,37 @@
         <v>42</v>
       </c>
       <c r="C35" s="7">
-        <v>42087</v>
+        <v>42089</v>
       </c>
       <c r="D35" s="5">
         <v>39</v>
       </c>
       <c r="E35" s="6">
-        <v>0.50856242088418635</v>
+        <v>0.50853812901530893</v>
       </c>
       <c r="F35" s="6">
-        <v>0.49143757911581359</v>
+        <v>0.49146187098469107</v>
       </c>
       <c r="G35" s="7">
-        <v>30857</v>
+        <v>30878</v>
       </c>
       <c r="H35" s="8">
-        <v>0.15970444307612536</v>
+        <v>0.15988729840015545</v>
       </c>
       <c r="I35" s="7">
-        <v>33681</v>
+        <v>33704</v>
       </c>
       <c r="J35" s="5">
-        <v>2324</v>
+        <v>2325</v>
       </c>
       <c r="K35" s="6">
-        <v>6.9000326593628453E-2</v>
+        <v>6.89829100403513E-2</v>
       </c>
       <c r="L35" s="5">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="M35" s="10">
-        <v>1.0810939239999999E-2</v>
+        <v>1.0834184700000001E-2</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2091,37 +2091,37 @@
         <v>43</v>
       </c>
       <c r="C36" s="12">
-        <v>74828</v>
+        <v>74836</v>
       </c>
       <c r="D36" s="13">
         <v>40</v>
       </c>
       <c r="E36" s="14">
-        <v>0.50165180489901162</v>
+        <v>0.50151057401812693</v>
       </c>
       <c r="F36" s="14">
-        <v>0.49834819510098838</v>
+        <v>0.49848942598187312</v>
       </c>
       <c r="G36" s="12">
-        <v>52372</v>
+        <v>52398</v>
       </c>
       <c r="H36" s="15">
-        <v>0.1548537386389674</v>
+        <v>0.15481506927745334</v>
       </c>
       <c r="I36" s="12">
-        <v>58082</v>
+        <v>58129</v>
       </c>
       <c r="J36" s="13">
-        <v>4096</v>
+        <v>4098</v>
       </c>
       <c r="K36" s="14">
-        <v>7.0520987569298574E-2</v>
+        <v>7.0498374305424147E-2</v>
       </c>
       <c r="L36" s="13">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="M36" s="16">
-        <v>1.3176885649999999E-2</v>
+        <v>1.3202202140000001E-2</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2132,37 +2132,37 @@
         <v>44</v>
       </c>
       <c r="C37" s="7">
-        <v>111096</v>
+        <v>111099</v>
       </c>
       <c r="D37" s="5">
         <v>41</v>
       </c>
       <c r="E37" s="6">
-        <v>0.49730199543693188</v>
+        <v>0.4972793858021059</v>
       </c>
       <c r="F37" s="6">
-        <v>0.50269800456306812</v>
+        <v>0.50272061419789416</v>
       </c>
       <c r="G37" s="7">
-        <v>75593</v>
+        <v>75603</v>
       </c>
       <c r="H37" s="8">
-        <v>0.15772624449353775</v>
+        <v>0.15775829001494648</v>
       </c>
       <c r="I37" s="7">
-        <v>83889</v>
+        <v>83921</v>
       </c>
       <c r="J37" s="5">
-        <v>5902</v>
+        <v>5904</v>
       </c>
       <c r="K37" s="6">
-        <v>7.0354873702154042E-2</v>
+        <v>7.0351878552448135E-2</v>
       </c>
       <c r="L37" s="5">
-        <v>1579</v>
+        <v>1581</v>
       </c>
       <c r="M37" s="10">
-        <v>1.421293295E-2</v>
+        <v>1.423055113E-2</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2173,37 +2173,37 @@
         <v>45</v>
       </c>
       <c r="C38" s="19">
-        <v>125805</v>
+        <v>125818</v>
       </c>
       <c r="D38" s="20">
         <v>41</v>
       </c>
       <c r="E38" s="21">
-        <v>0.4912811886739557</v>
+        <v>0.4912579991510288</v>
       </c>
       <c r="F38" s="21">
-        <v>0.50871881132604424</v>
+        <v>0.50874200084897125</v>
       </c>
       <c r="G38" s="19">
-        <v>84713</v>
+        <v>84884</v>
       </c>
       <c r="H38" s="22">
-        <v>0.15264481248450651</v>
+        <v>0.15260826539748362</v>
       </c>
       <c r="I38" s="19">
-        <v>92597</v>
+        <v>92666</v>
       </c>
       <c r="J38" s="20">
-        <v>6820</v>
+        <v>6826</v>
       </c>
       <c r="K38" s="21">
-        <v>7.3652494141278876E-2</v>
+        <v>7.3662400448924095E-2</v>
       </c>
       <c r="L38" s="20">
-        <v>1847</v>
+        <v>1849</v>
       </c>
       <c r="M38" s="23">
-        <v>1.4681451450000001E-2</v>
+        <v>1.469583048E-2</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2214,37 +2214,37 @@
         <v>46</v>
       </c>
       <c r="C39" s="7">
-        <v>127868</v>
+        <v>127869</v>
       </c>
       <c r="D39" s="5">
         <v>42</v>
       </c>
       <c r="E39" s="6">
-        <v>0.48458733841564466</v>
+        <v>0.4845717983522207</v>
       </c>
       <c r="F39" s="6">
-        <v>0.51541266158435528</v>
+        <v>0.51542820164777925</v>
       </c>
       <c r="G39" s="7">
-        <v>85460</v>
+        <v>85572</v>
       </c>
       <c r="H39" s="8">
-        <v>0.14871284811607768</v>
+        <v>0.14857663721778153</v>
       </c>
       <c r="I39" s="7">
-        <v>94318</v>
+        <v>94413</v>
       </c>
       <c r="J39" s="5">
-        <v>7462</v>
+        <v>7467</v>
       </c>
       <c r="K39" s="6">
-        <v>7.9115333234377319E-2</v>
+        <v>7.9088684820946262E-2</v>
       </c>
       <c r="L39" s="5">
-        <v>2449</v>
+        <v>2452</v>
       </c>
       <c r="M39" s="10">
-        <v>1.915256358E-2</v>
+        <v>1.9175875299999999E-2</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2255,37 +2255,37 @@
         <v>47</v>
       </c>
       <c r="C40" s="19">
-        <v>128476</v>
+        <v>128469</v>
       </c>
       <c r="D40" s="20">
         <v>43</v>
       </c>
       <c r="E40" s="21">
-        <v>0.47446840195317702</v>
+        <v>0.47446308198777237</v>
       </c>
       <c r="F40" s="21">
-        <v>0.52553159804682292</v>
+        <v>0.52553691801222757</v>
       </c>
       <c r="G40" s="19">
-        <v>86020</v>
+        <v>86334</v>
       </c>
       <c r="H40" s="22">
-        <v>0.1485119739595443</v>
+        <v>0.14809924247689207</v>
       </c>
       <c r="I40" s="19">
-        <v>93881</v>
+        <v>93919</v>
       </c>
       <c r="J40" s="20">
         <v>8003</v>
       </c>
       <c r="K40" s="21">
-        <v>8.5246215954239937E-2</v>
+        <v>8.5211724997071941E-2</v>
       </c>
       <c r="L40" s="20">
-        <v>3124</v>
+        <v>3128</v>
       </c>
       <c r="M40" s="23">
-        <v>2.4315825520000001E-2</v>
+        <v>2.4348286350000001E-2</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2296,37 +2296,37 @@
         <v>48</v>
       </c>
       <c r="C41" s="7">
-        <v>123287</v>
+        <v>123291</v>
       </c>
       <c r="D41" s="5">
         <v>44</v>
       </c>
       <c r="E41" s="6">
-        <v>0.46551667836792004</v>
+        <v>0.4655227304266904</v>
       </c>
       <c r="F41" s="6">
-        <v>0.5344833216320799</v>
+        <v>0.53447726957330965</v>
       </c>
       <c r="G41" s="7">
-        <v>82179</v>
+        <v>82267</v>
       </c>
       <c r="H41" s="8">
-        <v>0.15480840604047263</v>
+        <v>0.1547035871005385</v>
       </c>
       <c r="I41" s="7">
-        <v>89610</v>
+        <v>89665</v>
       </c>
       <c r="J41" s="5">
-        <v>8234</v>
+        <v>8246</v>
       </c>
       <c r="K41" s="6">
-        <v>9.188706617565004E-2</v>
+        <v>9.1964534656778008E-2</v>
       </c>
       <c r="L41" s="5">
-        <v>3485</v>
+        <v>3490</v>
       </c>
       <c r="M41" s="10">
-        <v>2.826737612E-2</v>
+        <v>2.830701348E-2</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2337,37 +2337,37 @@
         <v>49</v>
       </c>
       <c r="C42" s="19">
-        <v>128502</v>
+        <v>128510</v>
       </c>
       <c r="D42" s="20">
         <v>45</v>
       </c>
       <c r="E42" s="21">
-        <v>0.45912615346018454</v>
+        <v>0.45909800017246649</v>
       </c>
       <c r="F42" s="21">
-        <v>0.54087384653981541</v>
+        <v>0.54090199982753351</v>
       </c>
       <c r="G42" s="19">
-        <v>87039</v>
+        <v>87102</v>
       </c>
       <c r="H42" s="22">
-        <v>0.14176403681108468</v>
+        <v>0.14174186585841886</v>
       </c>
       <c r="I42" s="19">
-        <v>93652</v>
+        <v>93712</v>
       </c>
       <c r="J42" s="20">
-        <v>9071</v>
+        <v>9077</v>
       </c>
       <c r="K42" s="21">
-        <v>9.6858582838593943E-2</v>
+        <v>9.6860594160833188E-2</v>
       </c>
       <c r="L42" s="20">
-        <v>4346</v>
+        <v>4352</v>
       </c>
       <c r="M42" s="23">
-        <v>3.382048528E-2</v>
+        <v>3.386506886E-2</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2378,37 +2378,37 @@
         <v>50</v>
       </c>
       <c r="C43" s="7">
-        <v>156533</v>
+        <v>156531</v>
       </c>
       <c r="D43" s="5">
         <v>46</v>
       </c>
       <c r="E43" s="6">
-        <v>0.45386421381018238</v>
+        <v>0.45381859349169901</v>
       </c>
       <c r="F43" s="6">
-        <v>0.54613578618981762</v>
+        <v>0.54618140650830105</v>
       </c>
       <c r="G43" s="7">
-        <v>106251</v>
+        <v>106534</v>
       </c>
       <c r="H43" s="8">
-        <v>0.14459158031453823</v>
+        <v>0.14520247057277488</v>
       </c>
       <c r="I43" s="7">
-        <v>113575</v>
+        <v>113744</v>
       </c>
       <c r="J43" s="5">
-        <v>11079</v>
+        <v>11099</v>
       </c>
       <c r="K43" s="6">
-        <v>9.7547875852960597E-2</v>
+        <v>9.757877338584893E-2</v>
       </c>
       <c r="L43" s="5">
-        <v>5570</v>
+        <v>5575</v>
       </c>
       <c r="M43" s="10">
-        <v>3.5583551069999997E-2</v>
+        <v>3.5615948270000003E-2</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2419,37 +2419,37 @@
         <v>51</v>
       </c>
       <c r="C44" s="19">
-        <v>174930</v>
+        <v>174934</v>
       </c>
       <c r="D44" s="20">
         <v>46</v>
       </c>
       <c r="E44" s="21">
-        <v>0.4518118069708798</v>
+        <v>0.4518307426597582</v>
       </c>
       <c r="F44" s="21">
-        <v>0.54818819302912014</v>
+        <v>0.5481692573402418</v>
       </c>
       <c r="G44" s="19">
-        <v>117184</v>
+        <v>117292</v>
       </c>
       <c r="H44" s="22">
-        <v>0.14391043145821955</v>
+        <v>0.14393138491968763</v>
       </c>
       <c r="I44" s="19">
-        <v>125367</v>
+        <v>125468</v>
       </c>
       <c r="J44" s="20">
-        <v>12313</v>
+        <v>12330</v>
       </c>
       <c r="K44" s="21">
-        <v>9.8215638884235887E-2</v>
+        <v>9.8272069372270218E-2</v>
       </c>
       <c r="L44" s="20">
-        <v>6233</v>
+        <v>6242</v>
       </c>
       <c r="M44" s="23">
-        <v>3.5631395410000002E-2</v>
+        <v>3.5682028650000003E-2</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2460,37 +2460,37 @@
         <v>52</v>
       </c>
       <c r="C45" s="7">
-        <v>139245</v>
+        <v>139232</v>
       </c>
       <c r="D45" s="5">
         <v>48</v>
       </c>
       <c r="E45" s="6">
-        <v>0.44491556082948641</v>
+        <v>0.44490191680113461</v>
       </c>
       <c r="F45" s="6">
-        <v>0.55508443917051353</v>
+        <v>0.55509808319886544</v>
       </c>
       <c r="G45" s="7">
-        <v>90749</v>
+        <v>90899</v>
       </c>
       <c r="H45" s="8">
-        <v>0.15729098943239045</v>
+        <v>0.15731746223830845</v>
       </c>
       <c r="I45" s="7">
-        <v>99133</v>
+        <v>99297</v>
       </c>
       <c r="J45" s="5">
-        <v>10884</v>
+        <v>10905</v>
       </c>
       <c r="K45" s="6">
-        <v>0.10979189573603139</v>
+        <v>0.10982204900450164</v>
       </c>
       <c r="L45" s="5">
-        <v>5534</v>
+        <v>5542</v>
       </c>
       <c r="M45" s="10">
-        <v>3.9742899200000001E-2</v>
+        <v>3.980406803E-2</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2501,37 +2501,37 @@
         <v>53</v>
       </c>
       <c r="C46" s="19">
-        <v>123184</v>
+        <v>123201</v>
       </c>
       <c r="D46" s="20">
         <v>49</v>
       </c>
       <c r="E46" s="21">
-        <v>0.44120946150634122</v>
+        <v>0.44120897562892436</v>
       </c>
       <c r="F46" s="21">
-        <v>0.55879053849365878</v>
+        <v>0.55879102437107564</v>
       </c>
       <c r="G46" s="19">
-        <v>83366</v>
+        <v>83749</v>
       </c>
       <c r="H46" s="22">
-        <v>0.13420339227023007</v>
+        <v>0.13421055773800283</v>
       </c>
       <c r="I46" s="19">
-        <v>89375</v>
+        <v>89737</v>
       </c>
       <c r="J46" s="20">
-        <v>10700</v>
+        <v>10731</v>
       </c>
       <c r="K46" s="21">
-        <v>0.11972027972027972</v>
+        <v>0.11958278079276106</v>
       </c>
       <c r="L46" s="20">
-        <v>5496</v>
+        <v>5504</v>
       </c>
       <c r="M46" s="23">
-        <v>4.4616183910000003E-2</v>
+        <v>4.4674962050000003E-2</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2542,37 +2542,37 @@
         <v>1</v>
       </c>
       <c r="C47" s="27">
-        <v>145482</v>
+        <v>145488</v>
       </c>
       <c r="D47" s="28">
         <v>48</v>
       </c>
       <c r="E47" s="29">
-        <v>0.45082410721718141</v>
+        <v>0.45085486388070056</v>
       </c>
       <c r="F47" s="29">
-        <v>0.54917589278281864</v>
+        <v>0.54914513611929949</v>
       </c>
       <c r="G47" s="27">
-        <v>100238</v>
+        <v>100576</v>
       </c>
       <c r="H47" s="30">
-        <v>0.13192601608172549</v>
+        <v>0.1320295100222717</v>
       </c>
       <c r="I47" s="27">
-        <v>105494</v>
+        <v>105973</v>
       </c>
       <c r="J47" s="28">
-        <v>10737</v>
+        <v>10748</v>
       </c>
       <c r="K47" s="29">
-        <v>0.10177830018768839</v>
+        <v>0.10142206033612335</v>
       </c>
       <c r="L47" s="28">
-        <v>5474</v>
+        <v>5482</v>
       </c>
       <c r="M47" s="31">
-        <v>3.7626647970000003E-2</v>
+        <v>3.7680083580000003E-2</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2583,37 +2583,37 @@
         <v>2</v>
       </c>
       <c r="C48" s="19">
-        <v>118986</v>
+        <v>119010</v>
       </c>
       <c r="D48" s="20">
         <v>48</v>
       </c>
       <c r="E48" s="21">
-        <v>0.45434710631542308</v>
+        <v>0.45432710669031717</v>
       </c>
       <c r="F48" s="21">
-        <v>0.54565289368457692</v>
+        <v>0.54567289330968283</v>
       </c>
       <c r="G48" s="19">
-        <v>80139</v>
+        <v>80434</v>
       </c>
       <c r="H48" s="22">
-        <v>0.15757621133280925</v>
+        <v>0.15749558644354378</v>
       </c>
       <c r="I48" s="19">
-        <v>86517</v>
+        <v>86920</v>
       </c>
       <c r="J48" s="20">
-        <v>9499</v>
+        <v>9509</v>
       </c>
       <c r="K48" s="21">
-        <v>0.10979345099806974</v>
+        <v>0.10939944776806258</v>
       </c>
       <c r="L48" s="20">
-        <v>4856</v>
+        <v>4874</v>
       </c>
       <c r="M48" s="23">
-        <v>4.0811524039999998E-2</v>
+        <v>4.0954541630000001E-2</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2624,37 +2624,37 @@
         <v>3</v>
       </c>
       <c r="C49" s="7">
-        <v>95584</v>
+        <v>95585</v>
       </c>
       <c r="D49" s="5">
         <v>48</v>
       </c>
       <c r="E49" s="6">
-        <v>0.4581236084290945</v>
+        <v>0.45818956875903477</v>
       </c>
       <c r="F49" s="6">
-        <v>0.5418763915709055</v>
+        <v>0.54181043124096528</v>
       </c>
       <c r="G49" s="7">
-        <v>66118</v>
+        <v>66266</v>
       </c>
       <c r="H49" s="8">
-        <v>0.15693154662875466</v>
+        <v>0.15683759393957686</v>
       </c>
       <c r="I49" s="7">
-        <v>72063</v>
+        <v>72208</v>
       </c>
       <c r="J49" s="5">
-        <v>8471</v>
+        <v>8485</v>
       </c>
       <c r="K49" s="6">
-        <v>0.11754992159638095</v>
+        <v>0.11750775537336583</v>
       </c>
       <c r="L49" s="5">
-        <v>3864</v>
+        <v>3877</v>
       </c>
       <c r="M49" s="10">
-        <v>4.0425175760000001E-2</v>
+        <v>4.0560757439999998E-2</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2665,37 +2665,37 @@
         <v>4</v>
       </c>
       <c r="C50" s="19">
-        <v>78253</v>
+        <v>78245</v>
       </c>
       <c r="D50" s="20">
         <v>48</v>
       </c>
       <c r="E50" s="21">
-        <v>0.46321690939554067</v>
+        <v>0.46311977213264766</v>
       </c>
       <c r="F50" s="21">
-        <v>0.53678309060445939</v>
+        <v>0.53688022786735234</v>
       </c>
       <c r="G50" s="19">
-        <v>54595</v>
+        <v>54758</v>
       </c>
       <c r="H50" s="22">
-        <v>0.15876911805110358</v>
+        <v>0.15917308886372766</v>
       </c>
       <c r="I50" s="19">
-        <v>60457</v>
+        <v>60745</v>
       </c>
       <c r="J50" s="20">
-        <v>7135</v>
+        <v>7152</v>
       </c>
       <c r="K50" s="21">
-        <v>0.11801776469226062</v>
+        <v>0.11773808543913079</v>
       </c>
       <c r="L50" s="20">
-        <v>2905</v>
+        <v>2924</v>
       </c>
       <c r="M50" s="23">
-        <v>3.7123177379999997E-2</v>
+        <v>3.736979998E-2</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2706,37 +2706,37 @@
         <v>5</v>
       </c>
       <c r="C51" s="7">
-        <v>64648</v>
+        <v>64672</v>
       </c>
       <c r="D51" s="5">
         <v>46</v>
       </c>
       <c r="E51" s="6">
-        <v>0.47373598575934545</v>
+        <v>0.47374664419054752</v>
       </c>
       <c r="F51" s="6">
-        <v>0.52626401424065461</v>
+        <v>0.52625335580945243</v>
       </c>
       <c r="G51" s="7">
-        <v>45783</v>
+        <v>46123</v>
       </c>
       <c r="H51" s="8">
-        <v>0.15955704082301292</v>
+        <v>0.15985516987186435</v>
       </c>
       <c r="I51" s="7">
-        <v>50559</v>
+        <v>50868</v>
       </c>
       <c r="J51" s="5">
-        <v>6088</v>
+        <v>6114</v>
       </c>
       <c r="K51" s="6">
-        <v>0.12041377400660615</v>
+        <v>0.12019344184949281</v>
       </c>
       <c r="L51" s="5">
-        <v>2071</v>
+        <v>2081</v>
       </c>
       <c r="M51" s="10">
-        <v>3.2035020409999997E-2</v>
+        <v>3.2177758530000003E-2</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2747,37 +2747,37 @@
         <v>6</v>
       </c>
       <c r="C52" s="19">
-        <v>50865</v>
+        <v>50869</v>
       </c>
       <c r="D52" s="20">
         <v>45</v>
       </c>
       <c r="E52" s="21">
-        <v>0.48387416496521102</v>
+        <v>0.48379744326627688</v>
       </c>
       <c r="F52" s="21">
-        <v>0.51612583503478904</v>
+        <v>0.51620255673372317</v>
       </c>
       <c r="G52" s="19">
-        <v>36694</v>
+        <v>36861</v>
       </c>
       <c r="H52" s="22">
-        <v>0.16405951926745516</v>
+        <v>0.1638859499199696</v>
       </c>
       <c r="I52" s="19">
-        <v>40016</v>
+        <v>40213</v>
       </c>
       <c r="J52" s="20">
-        <v>4858</v>
+        <v>4883</v>
       </c>
       <c r="K52" s="21">
-        <v>0.1214014394242303</v>
+        <v>0.12142839380299902</v>
       </c>
       <c r="L52" s="20">
-        <v>1531</v>
+        <v>1544</v>
       </c>
       <c r="M52" s="23">
-        <v>3.0099282410000001E-2</v>
+        <v>3.0352474000000001E-2</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2788,37 +2788,37 @@
         <v>7</v>
       </c>
       <c r="C53" s="7">
-        <v>52506</v>
+        <v>52517</v>
       </c>
       <c r="D53" s="5">
         <v>44</v>
       </c>
       <c r="E53" s="6">
-        <v>0.49183818310858762</v>
+        <v>0.49180296435487891</v>
       </c>
       <c r="F53" s="6">
-        <v>0.50816181689141238</v>
+        <v>0.50819703564512109</v>
       </c>
       <c r="G53" s="7">
-        <v>38264</v>
+        <v>38440</v>
       </c>
       <c r="H53" s="8">
-        <v>0.16294689525402467</v>
+        <v>0.16298126951092612</v>
       </c>
       <c r="I53" s="7">
-        <v>41751</v>
+        <v>41997</v>
       </c>
       <c r="J53" s="5">
-        <v>4804</v>
+        <v>4825</v>
       </c>
       <c r="K53" s="6">
-        <v>0.11506311226078417</v>
+        <v>0.11488915874943448</v>
       </c>
       <c r="L53" s="5">
-        <v>1288</v>
+        <v>1316</v>
       </c>
       <c r="M53" s="10">
-        <v>2.4530529839999999E-2</v>
+        <v>2.5058552460000001E-2</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2829,37 +2829,37 @@
         <v>8</v>
       </c>
       <c r="C54" s="19">
-        <v>56480</v>
+        <v>56498</v>
       </c>
       <c r="D54" s="20">
         <v>42</v>
       </c>
       <c r="E54" s="21">
-        <v>0.49720431639303392</v>
+        <v>0.49716096189103076</v>
       </c>
       <c r="F54" s="21">
-        <v>0.50279568360696603</v>
+        <v>0.50283903810896924</v>
       </c>
       <c r="G54" s="19">
-        <v>41042</v>
+        <v>41261</v>
       </c>
       <c r="H54" s="22">
-        <v>0.15791140782612934</v>
+        <v>0.15767916434405371</v>
       </c>
       <c r="I54" s="19">
-        <v>44398</v>
+        <v>44722</v>
       </c>
       <c r="J54" s="20">
-        <v>4430</v>
+        <v>4466</v>
       </c>
       <c r="K54" s="21">
-        <v>9.9779269336456602E-2</v>
+        <v>9.9861365770761587E-2</v>
       </c>
       <c r="L54" s="20">
-        <v>998</v>
+        <v>1037</v>
       </c>
       <c r="M54" s="23">
-        <v>1.766997167E-2</v>
+        <v>1.8354632020000001E-2</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2870,37 +2870,37 @@
         <v>9</v>
       </c>
       <c r="C55" s="7">
-        <v>58492</v>
+        <v>58514</v>
       </c>
       <c r="D55" s="5">
         <v>40</v>
       </c>
       <c r="E55" s="6">
-        <v>0.50715612743411542</v>
+        <v>0.50708439369970426</v>
       </c>
       <c r="F55" s="6">
-        <v>0.49284387256588452</v>
+        <v>0.49291560630029574</v>
       </c>
       <c r="G55" s="7">
-        <v>42256</v>
+        <v>42599</v>
       </c>
       <c r="H55" s="8">
-        <v>0.15453426732298373</v>
+        <v>0.15436982088781426</v>
       </c>
       <c r="I55" s="7">
-        <v>45447</v>
+        <v>45855</v>
       </c>
       <c r="J55" s="5">
-        <v>3922</v>
+        <v>3972</v>
       </c>
       <c r="K55" s="6">
-        <v>8.6298325522036659E-2</v>
+        <v>8.6620870134118413E-2</v>
       </c>
       <c r="L55" s="5">
-        <v>732</v>
+        <v>799</v>
       </c>
       <c r="M55" s="10">
-        <v>1.25145319E-2</v>
+        <v>1.365485183E-2</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2911,78 +2911,78 @@
         <v>10</v>
       </c>
       <c r="C56" s="19">
-        <v>71416</v>
+        <v>71459</v>
       </c>
       <c r="D56" s="20">
         <v>39</v>
       </c>
       <c r="E56" s="21">
-        <v>0.50273008169081645</v>
+        <v>0.50277707293693086</v>
       </c>
       <c r="F56" s="21">
-        <v>0.49726991830918349</v>
+        <v>0.49722292706306914</v>
       </c>
       <c r="G56" s="19">
-        <v>49323</v>
+        <v>50410</v>
       </c>
       <c r="H56" s="22">
-        <v>0.15443099568152788</v>
+        <v>0.15423527077960722</v>
       </c>
       <c r="I56" s="19">
-        <v>52938</v>
-      </c>
-      <c r="J56" s="20">
-        <v>4140</v>
+        <v>53905</v>
+      </c>
+      <c r="J56" s="32">
+        <v>4312</v>
       </c>
       <c r="K56" s="21">
-        <v>7.8204692281536897E-2</v>
-      </c>
-      <c r="L56" s="20">
-        <v>607</v>
+        <v>7.9992579538076244E-2</v>
+      </c>
+      <c r="L56" s="32">
+        <v>740</v>
       </c>
       <c r="M56" s="23">
-        <v>8.49949591E-3</v>
+        <v>1.0355588509999999E-2</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="17">
+      <c r="A57" s="25">
         <v>2021</v>
       </c>
-      <c r="B57" s="17">
+      <c r="B57" s="25">
         <v>11</v>
       </c>
-      <c r="C57" s="7">
-        <v>92574</v>
-      </c>
-      <c r="D57" s="5">
+      <c r="C57" s="27">
+        <v>92782</v>
+      </c>
+      <c r="D57" s="28">
         <v>39</v>
       </c>
-      <c r="E57" s="6">
-        <v>0.50411084043848964</v>
-      </c>
-      <c r="F57" s="6">
-        <v>0.49588915956151036</v>
-      </c>
-      <c r="G57" s="7">
-        <v>61469</v>
-      </c>
-      <c r="H57" s="8">
-        <v>0.15323171029299321</v>
-      </c>
-      <c r="I57" s="7">
-        <v>66438</v>
-      </c>
-      <c r="J57" s="5">
-        <v>4262</v>
-      </c>
-      <c r="K57" s="6">
-        <v>6.4150034618742288E-2</v>
-      </c>
-      <c r="L57" s="5">
-        <v>372</v>
-      </c>
-      <c r="M57" s="10">
-        <v>4.0184068900000003E-3</v>
+      <c r="E57" s="29">
+        <v>0.50402906566888994</v>
+      </c>
+      <c r="F57" s="29">
+        <v>0.49597093433111</v>
+      </c>
+      <c r="G57" s="27">
+        <v>63393</v>
+      </c>
+      <c r="H57" s="30">
+        <v>0.15194106604830188</v>
+      </c>
+      <c r="I57" s="27">
+        <v>68072</v>
+      </c>
+      <c r="J57" s="28">
+        <v>4692</v>
+      </c>
+      <c r="K57" s="29">
+        <v>6.8927018451051827E-2</v>
+      </c>
+      <c r="L57" s="28">
+        <v>593</v>
+      </c>
+      <c r="M57" s="31">
+        <v>6.3913258999999997E-3</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2993,50 +2993,92 @@
         <v>12</v>
       </c>
       <c r="C58" s="19">
-        <v>114770</v>
+        <v>116633</v>
       </c>
       <c r="D58" s="20">
         <v>38</v>
       </c>
       <c r="E58" s="21">
-        <v>0.50760349197409182</v>
+        <v>0.50785213610945457</v>
       </c>
       <c r="F58" s="21">
-        <v>0.49239650802590818</v>
+        <v>0.49214786389054543</v>
       </c>
       <c r="G58" s="19">
-        <v>62803</v>
+        <v>73049</v>
       </c>
       <c r="H58" s="22">
-        <v>0.16226931834466507</v>
+        <v>0.15496447589973852</v>
       </c>
       <c r="I58" s="19">
-        <v>74207</v>
+        <v>82254</v>
       </c>
       <c r="J58" s="20">
-        <v>3627</v>
+        <v>4805</v>
       </c>
       <c r="K58" s="21">
-        <v>4.8876790599269609E-2</v>
+        <v>5.8416611958081066E-2</v>
       </c>
       <c r="L58" s="20">
-        <v>142</v>
+        <v>397</v>
       </c>
       <c r="M58" s="23">
-        <v>1.23725712E-3</v>
+        <v>3.4038393899999998E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="25">
+        <v>2023</v>
+      </c>
+      <c r="B59" s="25">
+        <v>13</v>
+      </c>
+      <c r="C59" s="27">
+        <v>108738</v>
+      </c>
+      <c r="D59" s="28">
+        <v>39</v>
+      </c>
+      <c r="E59" s="29">
+        <v>0.51304388205247276</v>
+      </c>
+      <c r="F59" s="29">
+        <v>0.4869561179475273</v>
+      </c>
+      <c r="G59" s="27">
+        <v>54108</v>
+      </c>
+      <c r="H59" s="30">
+        <v>0.15583647519775265</v>
+      </c>
+      <c r="I59" s="27">
+        <v>65352</v>
+      </c>
+      <c r="J59" s="28">
+        <v>3246</v>
+      </c>
+      <c r="K59" s="29">
+        <v>4.9669482188762396E-2</v>
+      </c>
+      <c r="L59" s="28">
+        <v>129</v>
+      </c>
+      <c r="M59" s="31">
+        <v>1.1863378E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2B208C-555F-44C6-980F-40400D13B2EF}">
-  <dimension ref="A1:H30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E6585B-9715-4742-AD54-D5D5F0340D3B}">
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3046,33 +3088,33 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -3095,10 +3137,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -3121,10 +3163,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>9</v>
@@ -3147,10 +3189,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>15</v>
@@ -3173,10 +3215,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
       </c>
       <c r="C6">
         <v>21</v>
@@ -3199,10 +3241,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>24</v>
@@ -3220,15 +3262,15 @@
         <v>780</v>
       </c>
       <c r="H7">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>50</v>
@@ -3240,7 +3282,7 @@
         <v>428</v>
       </c>
       <c r="F8">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="G8">
         <v>1411</v>
@@ -3251,10 +3293,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>64</v>
@@ -3269,18 +3311,18 @@
         <v>1490</v>
       </c>
       <c r="G9">
-        <v>2074</v>
+        <v>2075</v>
       </c>
       <c r="H9">
-        <v>1681</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>65</v>
@@ -3289,27 +3331,27 @@
         <v>58</v>
       </c>
       <c r="E10">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="F10">
         <v>1680</v>
       </c>
       <c r="G10">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="H10">
-        <v>2040</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C11">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D11">
         <v>68</v>
@@ -3318,27 +3360,27 @@
         <v>569</v>
       </c>
       <c r="F11">
-        <v>1704</v>
+        <v>1706</v>
       </c>
       <c r="G11">
         <v>2558</v>
       </c>
       <c r="H11">
-        <v>2489</v>
+        <v>2491</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>54</v>
       </c>
       <c r="D12">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E12">
         <v>597</v>
@@ -3347,18 +3389,18 @@
         <v>1654</v>
       </c>
       <c r="G12">
-        <v>2837</v>
+        <v>2835</v>
       </c>
       <c r="H12">
-        <v>2802</v>
+        <v>2803</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C13">
         <v>63</v>
@@ -3367,24 +3409,24 @@
         <v>68</v>
       </c>
       <c r="E13">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="F13">
-        <v>1670</v>
+        <v>1673</v>
       </c>
       <c r="G13">
-        <v>2840</v>
+        <v>2843</v>
       </c>
       <c r="H13">
-        <v>3032</v>
+        <v>3037</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>57</v>
@@ -3393,24 +3435,24 @@
         <v>58</v>
       </c>
       <c r="E14">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="F14">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="G14">
         <v>3140</v>
       </c>
       <c r="H14">
-        <v>3572</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <v>70</v>
@@ -3419,24 +3461,24 @@
         <v>66</v>
       </c>
       <c r="E15">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="F15">
-        <v>1928</v>
+        <v>1930</v>
       </c>
       <c r="G15">
-        <v>3879</v>
+        <v>3889</v>
       </c>
       <c r="H15">
-        <v>4463</v>
+        <v>4470</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>78</v>
@@ -3445,24 +3487,24 @@
         <v>83</v>
       </c>
       <c r="E16">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="F16">
-        <v>2142</v>
+        <v>2145</v>
       </c>
       <c r="G16">
-        <v>4301</v>
+        <v>4305</v>
       </c>
       <c r="H16">
-        <v>5009</v>
+        <v>5017</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C17">
         <v>53</v>
@@ -3474,21 +3516,21 @@
         <v>594</v>
       </c>
       <c r="F17">
-        <v>1821</v>
+        <v>1828</v>
       </c>
       <c r="G17">
-        <v>3831</v>
+        <v>3839</v>
       </c>
       <c r="H17">
-        <v>4520</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C18">
         <v>74</v>
@@ -3497,24 +3539,24 @@
         <v>51</v>
       </c>
       <c r="E18">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="F18">
-        <v>1847</v>
+        <v>1851</v>
       </c>
       <c r="G18">
-        <v>3752</v>
+        <v>3766</v>
       </c>
       <c r="H18">
-        <v>4361</v>
+        <v>4372</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C19">
         <v>61</v>
@@ -3526,47 +3568,47 @@
         <v>560</v>
       </c>
       <c r="F19">
-        <v>1727</v>
+        <v>1731</v>
       </c>
       <c r="G19">
-        <v>3823</v>
+        <v>3828</v>
       </c>
       <c r="H19">
-        <v>4532</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C20">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D20">
         <v>46</v>
       </c>
       <c r="E20">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="F20">
         <v>1540</v>
       </c>
       <c r="G20">
-        <v>3263</v>
+        <v>3267</v>
       </c>
       <c r="H20">
-        <v>4085</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C21">
         <v>39</v>
@@ -3578,24 +3620,24 @@
         <v>385</v>
       </c>
       <c r="F21">
-        <v>1405</v>
+        <v>1408</v>
       </c>
       <c r="G21">
-        <v>3044</v>
+        <v>3048</v>
       </c>
       <c r="H21">
-        <v>3559</v>
+        <v>3566</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C22">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22">
         <v>30</v>
@@ -3604,21 +3646,21 @@
         <v>385</v>
       </c>
       <c r="F22">
-        <v>1169</v>
+        <v>1171</v>
       </c>
       <c r="G22">
-        <v>2651</v>
+        <v>2662</v>
       </c>
       <c r="H22">
-        <v>2864</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C23">
         <v>42</v>
@@ -3630,21 +3672,21 @@
         <v>338</v>
       </c>
       <c r="F23">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="G23">
-        <v>2224</v>
+        <v>2230</v>
       </c>
       <c r="H23">
-        <v>2373</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C24">
         <v>36</v>
@@ -3653,24 +3695,24 @@
         <v>22</v>
       </c>
       <c r="E24">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F24">
-        <v>913</v>
+        <v>920</v>
       </c>
       <c r="G24">
-        <v>1823</v>
+        <v>1829</v>
       </c>
       <c r="H24">
-        <v>1785</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C25">
         <v>35</v>
@@ -3679,24 +3721,24 @@
         <v>22</v>
       </c>
       <c r="E25">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F25">
-        <v>979</v>
+        <v>984</v>
       </c>
       <c r="G25">
-        <v>1882</v>
+        <v>1889</v>
       </c>
       <c r="H25">
-        <v>1584</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C26">
         <v>43</v>
@@ -3705,24 +3747,24 @@
         <v>31</v>
       </c>
       <c r="E26">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="F26">
-        <v>996</v>
+        <v>1004</v>
       </c>
       <c r="G26">
-        <v>1660</v>
+        <v>1674</v>
       </c>
       <c r="H26">
-        <v>1402</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C27">
         <v>49</v>
@@ -3731,94 +3773,120 @@
         <v>28</v>
       </c>
       <c r="E27">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="F27">
-        <v>921</v>
+        <v>937</v>
       </c>
       <c r="G27">
-        <v>1474</v>
+        <v>1495</v>
       </c>
       <c r="H27">
-        <v>1145</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28">
         <v>49</v>
       </c>
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28">
-        <v>47</v>
-      </c>
       <c r="D28">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E28">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="F28">
-        <v>1128</v>
+        <v>1189</v>
       </c>
       <c r="G28">
-        <v>1468</v>
+        <v>1532</v>
       </c>
       <c r="H28">
-        <v>1107</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C29">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D29">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E29">
-        <v>378</v>
+        <v>404</v>
       </c>
       <c r="F29">
-        <v>1173</v>
+        <v>1308</v>
       </c>
       <c r="G29">
-        <v>1536</v>
+        <v>1729</v>
       </c>
       <c r="H29">
-        <v>1045</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="32">
-        <v>2021</v>
+      <c r="A30" t="s">
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C30">
+        <v>70</v>
+      </c>
+      <c r="D30">
+        <v>72</v>
+      </c>
+      <c r="E30">
+        <v>471</v>
+      </c>
+      <c r="F30">
+        <v>1337</v>
+      </c>
+      <c r="G30">
+        <v>1707</v>
+      </c>
+      <c r="H30">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31">
         <v>63</v>
       </c>
-      <c r="D30">
-        <v>60</v>
-      </c>
-      <c r="E30">
-        <v>369</v>
-      </c>
-      <c r="F30">
-        <v>952</v>
-      </c>
-      <c r="G30">
-        <v>1253</v>
-      </c>
-      <c r="H30">
-        <v>925</v>
+      <c r="D31">
+        <v>73</v>
+      </c>
+      <c r="E31">
+        <v>331</v>
+      </c>
+      <c r="F31">
+        <v>839</v>
+      </c>
+      <c r="G31">
+        <v>1160</v>
+      </c>
+      <c r="H31">
+        <v>778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
/home/ofenloch/workspaces/COVID19/rki-data-evaluation/getRKIData.sh: add data automatically downloaded at 2021-04-09--05-03-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Klinische-Aspekte.xlsx
+++ b/rki-data/RKI-Klinische-Aspekte.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1151A2C-946E-4FDA-8B34-C4568813227A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92CE1CA-87CB-4F5D-AE05-A5DF90924F7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6225" xr2:uid="{DB775562-523C-43F7-B3D3-B72E2874F045}"/>
   </bookViews>
@@ -678,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED98BD9-4AB5-4844-ABD1-68F2C3D62B46}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2987,7 +2987,7 @@
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="18">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B58" s="18">
         <v>12</v>
@@ -3028,7 +3028,7 @@
     </row>
     <row r="59" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="25">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B59" s="25">
         <v>13</v>

</xml_diff>

<commit_message>
/home/ofenloch/workspaces/COVID19/rki-data-evaluation/getRKIData.sh: add data automatically downloaded at 2021-04-28--05-03-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Klinische-Aspekte.xlsx
+++ b/rki-data/RKI-Klinische-Aspekte.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82730AD2-C0F1-4A91-9B17-F2E3063BB02E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949AEF4E-AF57-43B6-8A97-49DBCC66A3C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{3677AF26-2CAB-4FDE-A93C-D8C0E4111944}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{3677AF26-2CAB-4FDE-A93C-D8C0E4111944}"/>
   </bookViews>
   <sheets>
     <sheet name="Klinische_Aspekte" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Meldejahr</t>
   </si>
@@ -65,207 +65,102 @@
     <t>A80+</t>
   </si>
   <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
     <t>2020-KW37</t>
   </si>
   <si>
-    <t>38</t>
-  </si>
-  <si>
     <t>2020-KW38</t>
   </si>
   <si>
-    <t>39</t>
-  </si>
-  <si>
     <t>2020-KW39</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>2020-KW40</t>
   </si>
   <si>
-    <t>41</t>
-  </si>
-  <si>
     <t>2020-KW41</t>
   </si>
   <si>
-    <t>42</t>
-  </si>
-  <si>
     <t>2020-KW42</t>
   </si>
   <si>
-    <t>43</t>
-  </si>
-  <si>
     <t>2020-KW43</t>
   </si>
   <si>
-    <t>44</t>
-  </si>
-  <si>
     <t>2020-KW44</t>
   </si>
   <si>
-    <t>45</t>
-  </si>
-  <si>
     <t>2020-KW45</t>
   </si>
   <si>
-    <t>46</t>
-  </si>
-  <si>
     <t>2020-KW46</t>
   </si>
   <si>
-    <t>47</t>
-  </si>
-  <si>
     <t>2020-KW47</t>
   </si>
   <si>
-    <t>48</t>
-  </si>
-  <si>
     <t>2020-KW48</t>
   </si>
   <si>
-    <t>49</t>
-  </si>
-  <si>
     <t>2020-KW49</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
     <t>2020-KW50</t>
   </si>
   <si>
-    <t>51</t>
-  </si>
-  <si>
     <t>2020-KW51</t>
   </si>
   <si>
-    <t>52</t>
-  </si>
-  <si>
     <t>2020-KW52</t>
   </si>
   <si>
-    <t>53</t>
-  </si>
-  <si>
     <t>2020-KW53</t>
   </si>
   <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
     <t>2021-KW01</t>
   </si>
   <si>
-    <t>02</t>
-  </si>
-  <si>
     <t>2021-KW02</t>
   </si>
   <si>
-    <t>03</t>
-  </si>
-  <si>
     <t>2021-KW03</t>
   </si>
   <si>
-    <t>04</t>
-  </si>
-  <si>
     <t>2021-KW04</t>
   </si>
   <si>
-    <t>05</t>
-  </si>
-  <si>
     <t>2021-KW05</t>
   </si>
   <si>
-    <t>06</t>
-  </si>
-  <si>
     <t>2021-KW06</t>
   </si>
   <si>
-    <t>07</t>
-  </si>
-  <si>
     <t>2021-KW07</t>
   </si>
   <si>
-    <t>08</t>
-  </si>
-  <si>
     <t>2021-KW08</t>
   </si>
   <si>
-    <t>09</t>
-  </si>
-  <si>
     <t>2021-KW09</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>2021-KW10</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>2021-KW11</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>2021-KW12</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>2021-KW13</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>2021-KW14</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>2021-KW15</t>
   </si>
   <si>
-    <t>Die dem RKI übermittelten COVID-19-Fälle nach Meldewoche und  Geschlecht sowie Anteile mit für COVID-19 relevanten Symptomen, Anteile Hospitalisierter und Verstorbener für die Meldewochen KW 10 – 53/2020 und KW 01 - 15/2021</t>
-  </si>
-  <si>
     <t>MW</t>
   </si>
   <si>
@@ -300,6 +195,12 @@
   </si>
   <si>
     <t>Anteil Verstorben</t>
+  </si>
+  <si>
+    <t>Die dem RKI übermittelten COVID-19-Fälle nach Meldewoche und  Geschlecht sowie Anteile mit für COVID-19 relevanten Symptomen, Anteile Hospitalisierter und Verstorbener für die Meldewochen KW 10 – 53/2020 und KW 01 - 16/2021</t>
+  </si>
+  <si>
+    <t>2021-KW16</t>
   </si>
 </sst>
 </file>
@@ -384,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -482,6 +383,11 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -796,17 +702,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872BAA18-906B-41C7-A8B5-537096EA6980}">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -814,40 +720,40 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -926,10 +832,10 @@
         <v>9.4654590658852775E-2</v>
       </c>
       <c r="L4" s="13">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M4" s="16">
-        <v>1.3221340789999999E-2</v>
+        <v>1.306579561E-2</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -940,37 +846,37 @@
         <v>12</v>
       </c>
       <c r="C5" s="7">
-        <v>22415</v>
+        <v>22410</v>
       </c>
       <c r="D5" s="5">
         <v>45</v>
       </c>
       <c r="E5" s="6">
-        <v>0.54992634914966743</v>
+        <v>0.5499151709974105</v>
       </c>
       <c r="F5" s="6">
-        <v>0.45007365085033252</v>
+        <v>0.4500848290025895</v>
       </c>
       <c r="G5" s="7">
-        <v>20159</v>
+        <v>20156</v>
       </c>
       <c r="H5" s="8">
-        <v>3.8940423632124611E-2</v>
+        <v>3.8896606469537603E-2</v>
       </c>
       <c r="I5" s="7">
-        <v>19381</v>
+        <v>19377</v>
       </c>
       <c r="J5" s="7">
-        <v>2229</v>
+        <v>2230</v>
       </c>
       <c r="K5" s="6">
-        <v>0.11500954543109231</v>
+        <v>0.1150848944625071</v>
       </c>
       <c r="L5" s="5">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="M5" s="10">
-        <v>2.132500557E-2</v>
+        <v>2.1195894680000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -981,37 +887,37 @@
         <v>13</v>
       </c>
       <c r="C6" s="12">
-        <v>33971</v>
+        <v>33970</v>
       </c>
       <c r="D6" s="13">
         <v>48</v>
       </c>
       <c r="E6" s="14">
-        <v>0.49488909181960117</v>
+        <v>0.49490367053555645</v>
       </c>
       <c r="F6" s="14">
-        <v>0.50511090818039883</v>
+        <v>0.50509632946444349</v>
       </c>
       <c r="G6" s="12">
         <v>30824</v>
       </c>
       <c r="H6" s="15">
-        <v>3.2928886581884247E-2</v>
+        <v>3.2961328834674279E-2</v>
       </c>
       <c r="I6" s="12">
-        <v>29520</v>
+        <v>29519</v>
       </c>
       <c r="J6" s="12">
-        <v>5143</v>
+        <v>5144</v>
       </c>
       <c r="K6" s="14">
-        <v>0.17422086720867208</v>
+        <v>0.17426064568582947</v>
       </c>
       <c r="L6" s="12">
         <v>1463</v>
       </c>
       <c r="M6" s="16">
-        <v>4.3066144649999999E-2</v>
+        <v>4.3067412419999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1022,37 +928,37 @@
         <v>14</v>
       </c>
       <c r="C7" s="7">
-        <v>36058</v>
+        <v>36053</v>
       </c>
       <c r="D7" s="5">
         <v>51</v>
       </c>
       <c r="E7" s="6">
-        <v>0.45076325284485153</v>
+        <v>0.45079805690492714</v>
       </c>
       <c r="F7" s="6">
-        <v>0.54923674715514847</v>
+        <v>0.54920194309507286</v>
       </c>
       <c r="G7" s="7">
-        <v>32041</v>
+        <v>32038</v>
       </c>
       <c r="H7" s="8">
-        <v>5.5522611653818547E-2</v>
+        <v>5.5527810724764343E-2</v>
       </c>
       <c r="I7" s="7">
-        <v>31619</v>
+        <v>31615</v>
       </c>
       <c r="J7" s="7">
-        <v>6091</v>
+        <v>6092</v>
       </c>
       <c r="K7" s="6">
-        <v>0.19263733830924445</v>
+        <v>0.19269334176814804</v>
       </c>
       <c r="L7" s="7">
-        <v>2260</v>
+        <v>2261</v>
       </c>
       <c r="M7" s="10">
-        <v>6.2676798490000005E-2</v>
+        <v>6.2713227740000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1063,37 +969,37 @@
         <v>15</v>
       </c>
       <c r="C8" s="12">
-        <v>27160</v>
+        <v>27158</v>
       </c>
       <c r="D8" s="13">
         <v>52</v>
       </c>
       <c r="E8" s="14">
-        <v>0.43469605927673538</v>
+        <v>0.43469124423963135</v>
       </c>
       <c r="F8" s="14">
-        <v>0.56530394072326462</v>
+        <v>0.56530875576036865</v>
       </c>
       <c r="G8" s="12">
-        <v>23583</v>
+        <v>23580</v>
       </c>
       <c r="H8" s="15">
-        <v>8.4637238688886063E-2</v>
+        <v>8.4605597964376597E-2</v>
       </c>
       <c r="I8" s="12">
-        <v>24152</v>
+        <v>24151</v>
       </c>
       <c r="J8" s="12">
-        <v>4730</v>
+        <v>4731</v>
       </c>
       <c r="K8" s="14">
-        <v>0.19584299436899635</v>
+        <v>0.19589250962693056</v>
       </c>
       <c r="L8" s="12">
-        <v>1878</v>
+        <v>1876</v>
       </c>
       <c r="M8" s="16">
-        <v>6.9145802650000004E-2</v>
+        <v>6.9077251630000003E-2</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1104,37 +1010,37 @@
         <v>16</v>
       </c>
       <c r="C9" s="7">
-        <v>17345</v>
+        <v>17342</v>
       </c>
       <c r="D9" s="5">
         <v>51</v>
       </c>
       <c r="E9" s="6">
-        <v>0.44724691215514256</v>
+        <v>0.44720891300583038</v>
       </c>
       <c r="F9" s="6">
-        <v>0.55275308784485744</v>
+        <v>0.55279108699416957</v>
       </c>
       <c r="G9" s="7">
         <v>14877</v>
       </c>
       <c r="H9" s="8">
-        <v>0.11467365732338509</v>
+        <v>0.11474087517644686</v>
       </c>
       <c r="I9" s="7">
-        <v>15530</v>
+        <v>15528</v>
       </c>
       <c r="J9" s="7">
-        <v>3379</v>
+        <v>3378</v>
       </c>
       <c r="K9" s="6">
-        <v>0.2175788795878944</v>
+        <v>0.21754250386398763</v>
       </c>
       <c r="L9" s="7">
         <v>1217</v>
       </c>
       <c r="M9" s="10">
-        <v>7.0164312480000005E-2</v>
+        <v>7.0176450230000006E-2</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1145,37 +1051,37 @@
         <v>17</v>
       </c>
       <c r="C10" s="12">
-        <v>12360</v>
+        <v>12362</v>
       </c>
       <c r="D10" s="13">
         <v>50</v>
       </c>
       <c r="E10" s="14">
-        <v>0.44980960868508468</v>
+        <v>0.44981773997569868</v>
       </c>
       <c r="F10" s="14">
-        <v>0.55019039131491532</v>
+        <v>0.55018226002430137</v>
       </c>
       <c r="G10" s="12">
         <v>10270</v>
       </c>
       <c r="H10" s="15">
-        <v>0.13924050632911392</v>
+        <v>0.139143135345667</v>
       </c>
       <c r="I10" s="12">
-        <v>10983</v>
+        <v>10984</v>
       </c>
       <c r="J10" s="12">
         <v>2240</v>
       </c>
       <c r="K10" s="14">
-        <v>0.20395156150414276</v>
+        <v>0.20393299344501092</v>
       </c>
       <c r="L10" s="13">
         <v>721</v>
       </c>
       <c r="M10" s="16">
-        <v>5.8333333330000001E-2</v>
+        <v>5.8323895799999997E-2</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1192,25 +1098,25 @@
         <v>48</v>
       </c>
       <c r="E11" s="6">
-        <v>0.47779870828848225</v>
+        <v>0.47806781485468247</v>
       </c>
       <c r="F11" s="6">
-        <v>0.52220129171151775</v>
+        <v>0.52193218514531758</v>
       </c>
       <c r="G11" s="7">
         <v>6257</v>
       </c>
       <c r="H11" s="8">
-        <v>0.17564327952692985</v>
+        <v>0.1758031005274093</v>
       </c>
       <c r="I11" s="7">
         <v>6609</v>
       </c>
       <c r="J11" s="7">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="K11" s="6">
-        <v>0.20653654108034497</v>
+        <v>0.20638523225904071</v>
       </c>
       <c r="L11" s="5">
         <v>386</v>
@@ -1227,37 +1133,37 @@
         <v>19</v>
       </c>
       <c r="C12" s="12">
-        <v>6237</v>
+        <v>6238</v>
       </c>
       <c r="D12" s="13">
         <v>47</v>
       </c>
       <c r="E12" s="14">
-        <v>0.48017974642914463</v>
+        <v>0.48026315789473684</v>
       </c>
       <c r="F12" s="14">
-        <v>0.51982025357085537</v>
+        <v>0.51973684210526316</v>
       </c>
       <c r="G12" s="12">
-        <v>5252</v>
+        <v>5253</v>
       </c>
       <c r="H12" s="15">
-        <v>0.1966869763899467</v>
+        <v>0.19683990100894727</v>
       </c>
       <c r="I12" s="12">
-        <v>5630</v>
+        <v>5631</v>
       </c>
       <c r="J12" s="12">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="K12" s="14">
-        <v>0.19200710479573713</v>
+        <v>0.19215059492097319</v>
       </c>
       <c r="L12" s="13">
         <v>257</v>
       </c>
       <c r="M12" s="16">
-        <v>4.1205707869999997E-2</v>
+        <v>4.1199102270000003E-2</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1268,16 +1174,16 @@
         <v>20</v>
       </c>
       <c r="C13" s="7">
-        <v>4762</v>
+        <v>4761</v>
       </c>
       <c r="D13" s="5">
         <v>45</v>
       </c>
       <c r="E13" s="6">
-        <v>0.49537426408746849</v>
+        <v>0.4952681388012618</v>
       </c>
       <c r="F13" s="6">
-        <v>0.50462573591253157</v>
+        <v>0.50473186119873814</v>
       </c>
       <c r="G13" s="7">
         <v>3946</v>
@@ -1286,19 +1192,19 @@
         <v>0.23162696401419158</v>
       </c>
       <c r="I13" s="7">
-        <v>4244</v>
+        <v>4243</v>
       </c>
       <c r="J13" s="5">
         <v>763</v>
       </c>
       <c r="K13" s="6">
-        <v>0.17978322337417529</v>
+        <v>0.17982559509780816</v>
       </c>
       <c r="L13" s="5">
         <v>164</v>
       </c>
       <c r="M13" s="10">
-        <v>3.4439311209999997E-2</v>
+        <v>3.4446544840000003E-2</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1309,16 +1215,16 @@
         <v>21</v>
       </c>
       <c r="C14" s="12">
-        <v>3609</v>
+        <v>3608</v>
       </c>
       <c r="D14" s="13">
         <v>43</v>
       </c>
       <c r="E14" s="14">
-        <v>0.50305725403001667</v>
+        <v>0.50319710870169587</v>
       </c>
       <c r="F14" s="14">
-        <v>0.49694274596998333</v>
+        <v>0.49680289129830413</v>
       </c>
       <c r="G14" s="12">
         <v>2837</v>
@@ -1339,7 +1245,7 @@
         <v>113</v>
       </c>
       <c r="M14" s="16">
-        <v>3.1310612350000003E-2</v>
+        <v>3.1319290460000003E-2</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1350,16 +1256,16 @@
         <v>22</v>
       </c>
       <c r="C15" s="7">
-        <v>3204</v>
+        <v>3205</v>
       </c>
       <c r="D15" s="5">
         <v>42</v>
       </c>
       <c r="E15" s="6">
-        <v>0.51566416040100249</v>
+        <v>0.51581584716567497</v>
       </c>
       <c r="F15" s="6">
-        <v>0.48433583959899751</v>
+        <v>0.48418415283432509</v>
       </c>
       <c r="G15" s="7">
         <v>2548</v>
@@ -1380,7 +1286,7 @@
         <v>65</v>
       </c>
       <c r="M15" s="10">
-        <v>2.028714107E-2</v>
+        <v>2.0280811230000001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1479,10 +1385,10 @@
         <v>36</v>
       </c>
       <c r="E18" s="14">
-        <v>0.58814958717824184</v>
+        <v>0.58790675084992716</v>
       </c>
       <c r="F18" s="14">
-        <v>0.41185041282175816</v>
+        <v>0.41209324915007284</v>
       </c>
       <c r="G18" s="12">
         <v>2937</v>
@@ -1596,37 +1502,37 @@
         <v>28</v>
       </c>
       <c r="C21" s="7">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="D21" s="5">
         <v>36</v>
       </c>
       <c r="E21" s="6">
-        <v>0.5590421139554087</v>
+        <v>0.55885997521685249</v>
       </c>
       <c r="F21" s="6">
-        <v>0.44095788604459124</v>
+        <v>0.44114002478314746</v>
       </c>
       <c r="G21" s="7">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="H21" s="8">
-        <v>0.23875968992248062</v>
+        <v>0.23940020682523269</v>
       </c>
       <c r="I21" s="7">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="J21" s="5">
         <v>256</v>
       </c>
       <c r="K21" s="6">
-        <v>0.11673506611947104</v>
+        <v>0.11678832116788321</v>
       </c>
       <c r="L21" s="5">
         <v>25</v>
       </c>
       <c r="M21" s="10">
-        <v>1.0300782850000001E-2</v>
+        <v>1.030502885E-2</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1637,37 +1543,37 @@
         <v>29</v>
       </c>
       <c r="C22" s="12">
-        <v>3014</v>
+        <v>3015</v>
       </c>
       <c r="D22" s="13">
         <v>36</v>
       </c>
       <c r="E22" s="14">
-        <v>0.52477552377785164</v>
+        <v>0.52460106382978722</v>
       </c>
       <c r="F22" s="14">
-        <v>0.47522447622214831</v>
+        <v>0.47539893617021278</v>
       </c>
       <c r="G22" s="12">
-        <v>2359</v>
+        <v>2360</v>
       </c>
       <c r="H22" s="15">
-        <v>0.22975837219160661</v>
+        <v>0.22966101694915253</v>
       </c>
       <c r="I22" s="12">
-        <v>2645</v>
+        <v>2646</v>
       </c>
       <c r="J22" s="13">
         <v>317</v>
       </c>
       <c r="K22" s="14">
-        <v>0.11984877126654064</v>
+        <v>0.11980347694633409</v>
       </c>
       <c r="L22" s="13">
         <v>30</v>
       </c>
       <c r="M22" s="16">
-        <v>9.9535500900000008E-3</v>
+        <v>9.9502487499999997E-3</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1719,16 +1625,16 @@
         <v>31</v>
       </c>
       <c r="C24" s="12">
-        <v>4822</v>
+        <v>4823</v>
       </c>
       <c r="D24" s="13">
         <v>36</v>
       </c>
       <c r="E24" s="14">
-        <v>0.5021815915229586</v>
+        <v>0.50207727461570417</v>
       </c>
       <c r="F24" s="14">
-        <v>0.49781840847704134</v>
+        <v>0.49792272538429583</v>
       </c>
       <c r="G24" s="12">
         <v>3715</v>
@@ -1749,7 +1655,7 @@
         <v>32</v>
       </c>
       <c r="M24" s="16">
-        <v>6.6362505100000004E-3</v>
+        <v>6.6348745500000002E-3</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1760,16 +1666,16 @@
         <v>32</v>
       </c>
       <c r="C25" s="7">
-        <v>6058</v>
+        <v>6057</v>
       </c>
       <c r="D25" s="5">
         <v>34</v>
       </c>
       <c r="E25" s="6">
-        <v>0.53670634920634919</v>
+        <v>0.53679510501074912</v>
       </c>
       <c r="F25" s="6">
-        <v>0.46329365079365081</v>
+        <v>0.46320489498925088</v>
       </c>
       <c r="G25" s="7">
         <v>4556</v>
@@ -1790,7 +1696,7 @@
         <v>31</v>
       </c>
       <c r="M25" s="10">
-        <v>5.1172003899999999E-3</v>
+        <v>5.1180452299999998E-3</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1842,16 +1748,16 @@
         <v>34</v>
       </c>
       <c r="C27" s="7">
-        <v>9591</v>
+        <v>9590</v>
       </c>
       <c r="D27" s="5">
         <v>32</v>
       </c>
       <c r="E27" s="6">
-        <v>0.54729446308724827</v>
+        <v>0.54735186156266391</v>
       </c>
       <c r="F27" s="6">
-        <v>0.45270553691275167</v>
+        <v>0.45264813843733614</v>
       </c>
       <c r="G27" s="7">
         <v>7211</v>
@@ -1860,19 +1766,19 @@
         <v>0.34530578283178476</v>
       </c>
       <c r="I27" s="7">
-        <v>8310</v>
+        <v>8309</v>
       </c>
       <c r="J27" s="5">
         <v>434</v>
       </c>
       <c r="K27" s="6">
-        <v>5.2226233453670279E-2</v>
+        <v>5.2232518955349617E-2</v>
       </c>
       <c r="L27" s="5">
         <v>30</v>
       </c>
       <c r="M27" s="10">
-        <v>3.12793243E-3</v>
+        <v>3.1282585999999999E-3</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1883,37 +1789,37 @@
         <v>35</v>
       </c>
       <c r="C28" s="12">
-        <v>8823</v>
+        <v>8821</v>
       </c>
       <c r="D28" s="13">
         <v>32</v>
       </c>
       <c r="E28" s="14">
-        <v>0.53118941726536661</v>
+        <v>0.53119653245123755</v>
       </c>
       <c r="F28" s="14">
-        <v>0.46881058273463339</v>
+        <v>0.4688034675487624</v>
       </c>
       <c r="G28" s="12">
         <v>6878</v>
       </c>
       <c r="H28" s="15">
-        <v>0.3073567897644664</v>
+        <v>0.30750218086653097</v>
       </c>
       <c r="I28" s="12">
-        <v>7429</v>
+        <v>7428</v>
       </c>
       <c r="J28" s="13">
         <v>366</v>
       </c>
       <c r="K28" s="14">
-        <v>4.9266388477587832E-2</v>
+        <v>4.9273021001615507E-2</v>
       </c>
       <c r="L28" s="13">
         <v>18</v>
       </c>
       <c r="M28" s="16">
-        <v>2.0401223999999998E-3</v>
+        <v>2.0405849599999999E-3</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1924,16 +1830,16 @@
         <v>36</v>
       </c>
       <c r="C29" s="7">
-        <v>8614</v>
+        <v>8615</v>
       </c>
       <c r="D29" s="5">
         <v>33</v>
       </c>
       <c r="E29" s="6">
-        <v>0.53670206558524913</v>
+        <v>0.53675612602100353</v>
       </c>
       <c r="F29" s="6">
-        <v>0.46329793441475087</v>
+        <v>0.46324387397899652</v>
       </c>
       <c r="G29" s="7">
         <v>6656</v>
@@ -1954,7 +1860,7 @@
         <v>36</v>
       </c>
       <c r="M29" s="10">
-        <v>4.1792430899999997E-3</v>
+        <v>4.1787579800000004E-3</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1965,37 +1871,37 @@
         <v>37</v>
       </c>
       <c r="C30" s="12">
-        <v>9769</v>
+        <v>9770</v>
       </c>
       <c r="D30" s="13">
         <v>35</v>
       </c>
       <c r="E30" s="14">
-        <v>0.51785163082621666</v>
+        <v>0.51779835390946505</v>
       </c>
       <c r="F30" s="14">
-        <v>0.48214836917378329</v>
+        <v>0.48220164609053495</v>
       </c>
       <c r="G30" s="12">
-        <v>7605</v>
+        <v>7613</v>
       </c>
       <c r="H30" s="15">
-        <v>0.20499671268902039</v>
+        <v>0.20517535794036518</v>
       </c>
       <c r="I30" s="12">
-        <v>8037</v>
+        <v>8038</v>
       </c>
       <c r="J30" s="13">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="K30" s="14">
-        <v>5.7857409481149681E-2</v>
+        <v>5.7974620552376212E-2</v>
       </c>
       <c r="L30" s="13">
         <v>66</v>
       </c>
       <c r="M30" s="16">
-        <v>6.7560650999999999E-3</v>
+        <v>6.7553735899999997E-3</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2018,19 +1924,19 @@
         <v>0.48794245074797676</v>
       </c>
       <c r="G31" s="7">
-        <v>9768</v>
+        <v>9770</v>
       </c>
       <c r="H31" s="8">
-        <v>0.18673218673218672</v>
+        <v>0.18669396110542477</v>
       </c>
       <c r="I31" s="7">
-        <v>10067</v>
+        <v>10068</v>
       </c>
       <c r="J31" s="5">
         <v>674</v>
       </c>
       <c r="K31" s="6">
-        <v>6.6951425449488428E-2</v>
+        <v>6.6944775526420336E-2</v>
       </c>
       <c r="L31" s="5">
         <v>79</v>
@@ -2059,19 +1965,19 @@
         <v>0.48365258866066618</v>
       </c>
       <c r="G32" s="12">
-        <v>10361</v>
+        <v>10369</v>
       </c>
       <c r="H32" s="15">
-        <v>0.18193224592220827</v>
+        <v>0.18188832095669785</v>
       </c>
       <c r="I32" s="12">
-        <v>10853</v>
+        <v>10856</v>
       </c>
       <c r="J32" s="13">
         <v>771</v>
       </c>
       <c r="K32" s="14">
-        <v>7.1040265364415364E-2</v>
+        <v>7.1020633750921144E-2</v>
       </c>
       <c r="L32" s="13">
         <v>107</v>
@@ -2088,37 +1994,37 @@
         <v>40</v>
       </c>
       <c r="C33" s="7">
-        <v>15932</v>
+        <v>15928</v>
       </c>
       <c r="D33" s="5">
         <v>38</v>
       </c>
       <c r="E33" s="6">
-        <v>0.51929736195932763</v>
+        <v>0.51923924680395495</v>
       </c>
       <c r="F33" s="6">
-        <v>0.48070263804067243</v>
+        <v>0.48076075319604511</v>
       </c>
       <c r="G33" s="7">
-        <v>12613</v>
+        <v>12616</v>
       </c>
       <c r="H33" s="8">
-        <v>0.17545389677317053</v>
+        <v>0.17541217501585288</v>
       </c>
       <c r="I33" s="7">
         <v>13481</v>
       </c>
       <c r="J33" s="5">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="K33" s="6">
-        <v>6.4906164231140123E-2</v>
+        <v>6.4831985757733107E-2</v>
       </c>
       <c r="L33" s="5">
         <v>121</v>
       </c>
       <c r="M33" s="10">
-        <v>7.5947777999999999E-3</v>
+        <v>7.5966850800000003E-3</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2129,37 +2035,37 @@
         <v>41</v>
       </c>
       <c r="C34" s="19">
-        <v>26126</v>
+        <v>26127</v>
       </c>
       <c r="D34" s="20">
         <v>39</v>
       </c>
       <c r="E34" s="21">
-        <v>0.51035304060543196</v>
+        <v>0.51029502151198525</v>
       </c>
       <c r="F34" s="21">
-        <v>0.48964695939456804</v>
+        <v>0.48970497848801475</v>
       </c>
       <c r="G34" s="19">
-        <v>20100</v>
+        <v>20102</v>
       </c>
       <c r="H34" s="22">
-        <v>0.16626865671641791</v>
+        <v>0.16625211421749081</v>
       </c>
       <c r="I34" s="19">
-        <v>21546</v>
+        <v>21549</v>
       </c>
       <c r="J34" s="20">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="K34" s="21">
-        <v>7.3609950802933255E-2</v>
+        <v>7.3646108868160934E-2</v>
       </c>
       <c r="L34" s="20">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M34" s="23">
-        <v>9.1096991499999991E-3</v>
+        <v>9.1476250599999993E-3</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2170,37 +2076,37 @@
         <v>42</v>
       </c>
       <c r="C35" s="7">
-        <v>42087</v>
+        <v>42086</v>
       </c>
       <c r="D35" s="5">
         <v>39</v>
       </c>
       <c r="E35" s="6">
-        <v>0.50856242088418635</v>
+        <v>0.50857456768892706</v>
       </c>
       <c r="F35" s="6">
-        <v>0.49143757911581359</v>
+        <v>0.49142543231107289</v>
       </c>
       <c r="G35" s="7">
-        <v>30879</v>
+        <v>30890</v>
       </c>
       <c r="H35" s="8">
-        <v>0.15984973606658245</v>
+        <v>0.15995467788928455</v>
       </c>
       <c r="I35" s="7">
-        <v>33703</v>
+        <v>33713</v>
       </c>
       <c r="J35" s="5">
-        <v>2325</v>
+        <v>2327</v>
       </c>
       <c r="K35" s="6">
-        <v>6.8984956828768956E-2</v>
+        <v>6.9023818704950612E-2</v>
       </c>
       <c r="L35" s="5">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="M35" s="10">
-        <v>1.0882220160000001E-2</v>
+        <v>1.0930000469999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2211,37 +2117,37 @@
         <v>43</v>
       </c>
       <c r="C36" s="12">
-        <v>74824</v>
+        <v>74817</v>
       </c>
       <c r="D36" s="13">
         <v>40</v>
       </c>
       <c r="E36" s="14">
-        <v>0.50150408250966905</v>
+        <v>0.50149750862914166</v>
       </c>
       <c r="F36" s="14">
-        <v>0.4984959174903309</v>
+        <v>0.49850249137085834</v>
       </c>
       <c r="G36" s="12">
-        <v>52396</v>
+        <v>52413</v>
       </c>
       <c r="H36" s="15">
-        <v>0.15476372242155889</v>
+        <v>0.15486615915898727</v>
       </c>
       <c r="I36" s="12">
-        <v>58134</v>
+        <v>58145</v>
       </c>
       <c r="J36" s="13">
         <v>4101</v>
       </c>
       <c r="K36" s="14">
-        <v>7.0543915780782326E-2</v>
+        <v>7.0530570126408121E-2</v>
       </c>
       <c r="L36" s="13">
         <v>991</v>
       </c>
       <c r="M36" s="16">
-        <v>1.324441355E-2</v>
+        <v>1.3245652720000001E-2</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2252,37 +2158,37 @@
         <v>44</v>
       </c>
       <c r="C37" s="7">
-        <v>111090</v>
+        <v>111077</v>
       </c>
       <c r="D37" s="5">
         <v>41</v>
       </c>
       <c r="E37" s="6">
-        <v>0.49726558255767628</v>
+        <v>0.49726078255593892</v>
       </c>
       <c r="F37" s="6">
-        <v>0.50273441744232372</v>
+        <v>0.50273921744406114</v>
       </c>
       <c r="G37" s="7">
-        <v>75617</v>
+        <v>75643</v>
       </c>
       <c r="H37" s="8">
-        <v>0.15770263300580556</v>
+        <v>0.15774096743915497</v>
       </c>
       <c r="I37" s="7">
-        <v>83939</v>
+        <v>83954</v>
       </c>
       <c r="J37" s="5">
-        <v>5907</v>
+        <v>5915</v>
       </c>
       <c r="K37" s="6">
-        <v>7.0372532434267748E-2</v>
+        <v>7.0455249303189846E-2</v>
       </c>
       <c r="L37" s="5">
-        <v>1586</v>
+        <v>1592</v>
       </c>
       <c r="M37" s="10">
-        <v>1.4276712570000001E-2</v>
+        <v>1.433240004E-2</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2293,37 +2199,37 @@
         <v>45</v>
       </c>
       <c r="C38" s="19">
-        <v>125803</v>
+        <v>125799</v>
       </c>
       <c r="D38" s="20">
         <v>41</v>
       </c>
       <c r="E38" s="21">
-        <v>0.49126095384566093</v>
+        <v>0.49125266345183355</v>
       </c>
       <c r="F38" s="21">
-        <v>0.50873904615433907</v>
+        <v>0.5087473365481664</v>
       </c>
       <c r="G38" s="19">
-        <v>85213</v>
+        <v>85229</v>
       </c>
       <c r="H38" s="22">
-        <v>0.15217161700679474</v>
+        <v>0.15217824918748313</v>
       </c>
       <c r="I38" s="19">
-        <v>92744</v>
+        <v>92757</v>
       </c>
       <c r="J38" s="20">
-        <v>6828</v>
+        <v>6834</v>
       </c>
       <c r="K38" s="21">
-        <v>7.3622013283878199E-2</v>
+        <v>7.3676380219282647E-2</v>
       </c>
       <c r="L38" s="20">
-        <v>1849</v>
+        <v>1856</v>
       </c>
       <c r="M38" s="23">
-        <v>1.469758272E-2</v>
+        <v>1.475369438E-2</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2340,31 +2246,31 @@
         <v>42</v>
       </c>
       <c r="E39" s="6">
-        <v>0.48455764540596857</v>
+        <v>0.48458181071972595</v>
       </c>
       <c r="F39" s="6">
-        <v>0.51544235459403143</v>
+        <v>0.51541818928027405</v>
       </c>
       <c r="G39" s="7">
-        <v>85770</v>
+        <v>85802</v>
       </c>
       <c r="H39" s="8">
-        <v>0.14843185262912439</v>
+        <v>0.14842311368033378</v>
       </c>
       <c r="I39" s="7">
-        <v>94452</v>
+        <v>94482</v>
       </c>
       <c r="J39" s="5">
-        <v>7470</v>
+        <v>7475</v>
       </c>
       <c r="K39" s="6">
-        <v>7.9087790623808912E-2</v>
+        <v>7.911559873838403E-2</v>
       </c>
       <c r="L39" s="5">
-        <v>2457</v>
+        <v>2468</v>
       </c>
       <c r="M39" s="10">
-        <v>1.9218434669999999E-2</v>
+        <v>1.930447569E-2</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2375,37 +2281,37 @@
         <v>47</v>
       </c>
       <c r="C40" s="19">
-        <v>128465</v>
+        <v>128456</v>
       </c>
       <c r="D40" s="20">
         <v>43</v>
       </c>
       <c r="E40" s="21">
-        <v>0.4744436867558649</v>
+        <v>0.47442268800852838</v>
       </c>
       <c r="F40" s="21">
-        <v>0.5255563132441351</v>
+        <v>0.52557731199147162</v>
       </c>
       <c r="G40" s="19">
-        <v>86386</v>
+        <v>86420</v>
       </c>
       <c r="H40" s="22">
-        <v>0.1480911258768782</v>
+        <v>0.14810229113631104</v>
       </c>
       <c r="I40" s="19">
-        <v>93960</v>
+        <v>93995</v>
       </c>
       <c r="J40" s="20">
-        <v>8011</v>
+        <v>8019</v>
       </c>
       <c r="K40" s="21">
-        <v>8.525968497232865E-2</v>
+        <v>8.5313048566413113E-2</v>
       </c>
       <c r="L40" s="20">
-        <v>3140</v>
+        <v>3149</v>
       </c>
       <c r="M40" s="23">
-        <v>2.444245514E-2</v>
+        <v>2.4514230549999998E-2</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2416,37 +2322,37 @@
         <v>48</v>
       </c>
       <c r="C41" s="7">
-        <v>123294</v>
+        <v>123290</v>
       </c>
       <c r="D41" s="5">
         <v>44</v>
       </c>
       <c r="E41" s="6">
-        <v>0.46552821902600688</v>
+        <v>0.46549936737276032</v>
       </c>
       <c r="F41" s="6">
-        <v>0.53447178097399306</v>
+        <v>0.53450063262723968</v>
       </c>
       <c r="G41" s="7">
-        <v>82373</v>
+        <v>82441</v>
       </c>
       <c r="H41" s="8">
-        <v>0.15466232867565829</v>
+        <v>0.15459540762484686</v>
       </c>
       <c r="I41" s="7">
-        <v>89759</v>
+        <v>89846</v>
       </c>
       <c r="J41" s="5">
-        <v>8250</v>
+        <v>8251</v>
       </c>
       <c r="K41" s="6">
-        <v>9.1912788689713573E-2</v>
+        <v>9.1834917525543708E-2</v>
       </c>
       <c r="L41" s="5">
-        <v>3496</v>
+        <v>3505</v>
       </c>
       <c r="M41" s="10">
-        <v>2.8354988880000001E-2</v>
+        <v>2.8428907449999999E-2</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2457,37 +2363,37 @@
         <v>49</v>
       </c>
       <c r="C42" s="19">
-        <v>128507</v>
+        <v>128506</v>
       </c>
       <c r="D42" s="20">
         <v>45</v>
       </c>
       <c r="E42" s="21">
-        <v>0.45915119779254987</v>
+        <v>0.45916687570550607</v>
       </c>
       <c r="F42" s="21">
-        <v>0.54084880220745013</v>
+        <v>0.54083312429449393</v>
       </c>
       <c r="G42" s="19">
-        <v>87341</v>
+        <v>87469</v>
       </c>
       <c r="H42" s="22">
-        <v>0.14206386462257131</v>
+        <v>0.14207319164503995</v>
       </c>
       <c r="I42" s="19">
-        <v>94106</v>
+        <v>94164</v>
       </c>
       <c r="J42" s="20">
-        <v>9083</v>
+        <v>9088</v>
       </c>
       <c r="K42" s="21">
-        <v>9.6518819203876477E-2</v>
+        <v>9.6512467609702224E-2</v>
       </c>
       <c r="L42" s="20">
-        <v>4357</v>
+        <v>4370</v>
       </c>
       <c r="M42" s="23">
-        <v>3.3904767830000002E-2</v>
+        <v>3.4006194259999997E-2</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2498,37 +2404,37 @@
         <v>50</v>
       </c>
       <c r="C43" s="7">
-        <v>156524</v>
+        <v>156512</v>
       </c>
       <c r="D43" s="5">
         <v>46</v>
       </c>
       <c r="E43" s="6">
-        <v>0.45385021097046413</v>
+        <v>0.45384491686231626</v>
       </c>
       <c r="F43" s="6">
-        <v>0.54614978902953581</v>
+        <v>0.54615508313768368</v>
       </c>
       <c r="G43" s="7">
-        <v>107266</v>
+        <v>107365</v>
       </c>
       <c r="H43" s="8">
-        <v>0.14648630507336902</v>
+        <v>0.14663065244725934</v>
       </c>
       <c r="I43" s="7">
-        <v>114606</v>
+        <v>114700</v>
       </c>
       <c r="J43" s="5">
-        <v>11140</v>
+        <v>11157</v>
       </c>
       <c r="K43" s="6">
-        <v>9.7202589742247353E-2</v>
+        <v>9.7271142109851785E-2</v>
       </c>
       <c r="L43" s="5">
-        <v>5589</v>
+        <v>5598</v>
       </c>
       <c r="M43" s="10">
-        <v>3.5706984230000002E-2</v>
+        <v>3.576722551E-2</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2539,37 +2445,37 @@
         <v>51</v>
       </c>
       <c r="C44" s="19">
-        <v>174927</v>
+        <v>174930</v>
       </c>
       <c r="D44" s="20">
         <v>46</v>
       </c>
       <c r="E44" s="21">
-        <v>0.45182161997248432</v>
+        <v>0.45178930160539238</v>
       </c>
       <c r="F44" s="21">
-        <v>0.54817838002751573</v>
+        <v>0.54821069839460768</v>
       </c>
       <c r="G44" s="19">
-        <v>117823</v>
+        <v>118103</v>
       </c>
       <c r="H44" s="22">
-        <v>0.14392775604084093</v>
+        <v>0.1444586504999873</v>
       </c>
       <c r="I44" s="19">
-        <v>126199</v>
+        <v>126478</v>
       </c>
       <c r="J44" s="20">
-        <v>12344</v>
+        <v>12395</v>
       </c>
       <c r="K44" s="21">
-        <v>9.7813770315137202E-2</v>
+        <v>9.8001233416088171E-2</v>
       </c>
       <c r="L44" s="20">
-        <v>6257</v>
+        <v>6265</v>
       </c>
       <c r="M44" s="23">
-        <v>3.5769206579999997E-2</v>
+        <v>3.5814325729999999E-2</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2580,37 +2486,37 @@
         <v>52</v>
       </c>
       <c r="C45" s="7">
-        <v>139207</v>
+        <v>139212</v>
       </c>
       <c r="D45" s="5">
         <v>48</v>
       </c>
       <c r="E45" s="6">
-        <v>0.44492021930649384</v>
+        <v>0.44487921307681183</v>
       </c>
       <c r="F45" s="6">
-        <v>0.55507978069350616</v>
+        <v>0.55512078692318823</v>
       </c>
       <c r="G45" s="7">
-        <v>91190</v>
+        <v>91379</v>
       </c>
       <c r="H45" s="8">
-        <v>0.15760500054830573</v>
+        <v>0.15780430952407007</v>
       </c>
       <c r="I45" s="7">
-        <v>99767</v>
+        <v>99948</v>
       </c>
       <c r="J45" s="5">
-        <v>10900</v>
+        <v>10916</v>
       </c>
       <c r="K45" s="6">
-        <v>0.10925456313209779</v>
+        <v>0.10921679273222075</v>
       </c>
       <c r="L45" s="5">
-        <v>5557</v>
+        <v>5559</v>
       </c>
       <c r="M45" s="10">
-        <v>3.9918969589999999E-2</v>
+        <v>3.9931902419999998E-2</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2621,37 +2527,37 @@
         <v>53</v>
       </c>
       <c r="C46" s="19">
-        <v>123196</v>
+        <v>123193</v>
       </c>
       <c r="D46" s="20">
         <v>49</v>
       </c>
       <c r="E46" s="21">
-        <v>0.44123449715525359</v>
+        <v>0.44119814008317232</v>
       </c>
       <c r="F46" s="21">
-        <v>0.55876550284474646</v>
+        <v>0.55880185991682763</v>
       </c>
       <c r="G46" s="19">
-        <v>84149</v>
+        <v>84273</v>
       </c>
       <c r="H46" s="22">
-        <v>0.13408358982281429</v>
+        <v>0.13417108682496173</v>
       </c>
       <c r="I46" s="19">
-        <v>90207</v>
+        <v>90311</v>
       </c>
       <c r="J46" s="20">
-        <v>10775</v>
+        <v>10790</v>
       </c>
       <c r="K46" s="21">
-        <v>0.11944749298834902</v>
+        <v>0.11947603281992226</v>
       </c>
       <c r="L46" s="20">
-        <v>5530</v>
+        <v>5541</v>
       </c>
       <c r="M46" s="23">
-        <v>4.4887821029999997E-2</v>
+        <v>4.4978204930000001E-2</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2662,37 +2568,37 @@
         <v>1</v>
       </c>
       <c r="C47" s="27">
-        <v>145489</v>
+        <v>145482</v>
       </c>
       <c r="D47" s="28">
         <v>48</v>
       </c>
       <c r="E47" s="29">
-        <v>0.45085270027533308</v>
+        <v>0.45082876759830781</v>
       </c>
       <c r="F47" s="29">
-        <v>0.54914729972466692</v>
+        <v>0.54917123240169219</v>
       </c>
       <c r="G47" s="27">
-        <v>101341</v>
+        <v>101571</v>
       </c>
       <c r="H47" s="30">
-        <v>0.13199988158790618</v>
+        <v>0.13187819357887587</v>
       </c>
       <c r="I47" s="27">
-        <v>106583</v>
+        <v>106772</v>
       </c>
       <c r="J47" s="28">
-        <v>10811</v>
+        <v>10832</v>
       </c>
       <c r="K47" s="29">
-        <v>0.10143268626328776</v>
+        <v>0.10144981830442439</v>
       </c>
       <c r="L47" s="28">
-        <v>5521</v>
+        <v>5534</v>
       </c>
       <c r="M47" s="31">
-        <v>3.7947886090000001E-2</v>
+        <v>3.8039070119999997E-2</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2703,37 +2609,37 @@
         <v>2</v>
       </c>
       <c r="C48" s="19">
-        <v>119012</v>
+        <v>119004</v>
       </c>
       <c r="D48" s="20">
         <v>48</v>
       </c>
       <c r="E48" s="21">
-        <v>0.45429934143526379</v>
+        <v>0.45425150005516468</v>
       </c>
       <c r="F48" s="21">
-        <v>0.54570065856473626</v>
+        <v>0.54574849994483532</v>
       </c>
       <c r="G48" s="19">
-        <v>81045</v>
+        <v>81142</v>
       </c>
       <c r="H48" s="22">
-        <v>0.15738170152384479</v>
+        <v>0.15761258041458184</v>
       </c>
       <c r="I48" s="19">
-        <v>87211</v>
+        <v>87319</v>
       </c>
       <c r="J48" s="20">
-        <v>9547</v>
+        <v>9563</v>
       </c>
       <c r="K48" s="21">
-        <v>0.10947013564802605</v>
+        <v>0.10951797432403028</v>
       </c>
       <c r="L48" s="20">
-        <v>4912</v>
+        <v>4921</v>
       </c>
       <c r="M48" s="23">
-        <v>4.1273148920000002E-2</v>
+        <v>4.1351551200000003E-2</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2744,37 +2650,37 @@
         <v>3</v>
       </c>
       <c r="C49" s="7">
-        <v>95580</v>
+        <v>95576</v>
       </c>
       <c r="D49" s="5">
         <v>48</v>
       </c>
       <c r="E49" s="6">
-        <v>0.45819440341028994</v>
+        <v>0.45815396302861483</v>
       </c>
       <c r="F49" s="6">
-        <v>0.54180559658971006</v>
+        <v>0.54184603697138511</v>
       </c>
       <c r="G49" s="7">
-        <v>66628</v>
+        <v>66808</v>
       </c>
       <c r="H49" s="8">
-        <v>0.15652578495527406</v>
+        <v>0.15670279008501975</v>
       </c>
       <c r="I49" s="7">
-        <v>72401</v>
+        <v>72476</v>
       </c>
       <c r="J49" s="5">
-        <v>8501</v>
+        <v>8509</v>
       </c>
       <c r="K49" s="6">
-        <v>0.11741550531070012</v>
+        <v>0.11740438214029472</v>
       </c>
       <c r="L49" s="5">
-        <v>3909</v>
+        <v>3923</v>
       </c>
       <c r="M49" s="10">
-        <v>4.089767733E-2</v>
+        <v>4.1045869249999999E-2</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2785,37 +2691,37 @@
         <v>4</v>
       </c>
       <c r="C50" s="19">
-        <v>78248</v>
+        <v>78244</v>
       </c>
       <c r="D50" s="20">
         <v>48</v>
       </c>
       <c r="E50" s="21">
-        <v>0.46310376823547605</v>
+        <v>0.46313334364208031</v>
       </c>
       <c r="F50" s="21">
-        <v>0.53689623176452395</v>
+        <v>0.53686665635791975</v>
       </c>
       <c r="G50" s="19">
-        <v>55045</v>
+        <v>55387</v>
       </c>
       <c r="H50" s="22">
-        <v>0.15894268325915159</v>
+        <v>0.15942369147995017</v>
       </c>
       <c r="I50" s="19">
-        <v>60909</v>
+        <v>61176</v>
       </c>
       <c r="J50" s="20">
-        <v>7181</v>
+        <v>7219</v>
       </c>
       <c r="K50" s="21">
-        <v>0.11789719089132969</v>
+        <v>0.11800379233686413</v>
       </c>
       <c r="L50" s="20">
-        <v>2959</v>
+        <v>2974</v>
       </c>
       <c r="M50" s="23">
-        <v>3.7815663020000001E-2</v>
+        <v>3.8009304219999998E-2</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2826,37 +2732,37 @@
         <v>5</v>
       </c>
       <c r="C51" s="7">
-        <v>64679</v>
+        <v>64669</v>
       </c>
       <c r="D51" s="5">
         <v>46</v>
       </c>
       <c r="E51" s="6">
-        <v>0.47374662568071529</v>
+        <v>0.47373841400617922</v>
       </c>
       <c r="F51" s="6">
-        <v>0.52625337431928476</v>
+        <v>0.52626158599382078</v>
       </c>
       <c r="G51" s="7">
-        <v>46412</v>
+        <v>46542</v>
       </c>
       <c r="H51" s="8">
-        <v>0.15991553908471948</v>
+        <v>0.15979115637488719</v>
       </c>
       <c r="I51" s="7">
-        <v>51002</v>
+        <v>51107</v>
       </c>
       <c r="J51" s="5">
-        <v>6152</v>
+        <v>6173</v>
       </c>
       <c r="K51" s="6">
-        <v>0.12062272067762049</v>
+        <v>0.12078580233627488</v>
       </c>
       <c r="L51" s="5">
-        <v>2117</v>
+        <v>2130</v>
       </c>
       <c r="M51" s="10">
-        <v>3.2730870910000001E-2</v>
+        <v>3.293695588E-2</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2867,37 +2773,37 @@
         <v>6</v>
       </c>
       <c r="C52" s="19">
-        <v>50855</v>
+        <v>50848</v>
       </c>
       <c r="D52" s="20">
         <v>45</v>
       </c>
       <c r="E52" s="21">
-        <v>0.48378399809689954</v>
+        <v>0.48375394009079553</v>
       </c>
       <c r="F52" s="21">
-        <v>0.51621600190310046</v>
+        <v>0.51624605990920447</v>
       </c>
       <c r="G52" s="19">
-        <v>37285</v>
+        <v>37393</v>
       </c>
       <c r="H52" s="22">
-        <v>0.16363148719324125</v>
+        <v>0.16337282379054904</v>
       </c>
       <c r="I52" s="19">
-        <v>40423</v>
+        <v>40456</v>
       </c>
       <c r="J52" s="20">
-        <v>4942</v>
+        <v>4950</v>
       </c>
       <c r="K52" s="21">
-        <v>0.1222571308413527</v>
+        <v>0.12235515127545976</v>
       </c>
       <c r="L52" s="20">
-        <v>1589</v>
+        <v>1598</v>
       </c>
       <c r="M52" s="23">
-        <v>3.1245698549999999E-2</v>
+        <v>3.142699811E-2</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2908,37 +2814,37 @@
         <v>7</v>
       </c>
       <c r="C53" s="7">
-        <v>52500</v>
+        <v>52492</v>
       </c>
       <c r="D53" s="5">
         <v>44</v>
       </c>
       <c r="E53" s="6">
-        <v>0.4917812685808543</v>
+        <v>0.49179919046979609</v>
       </c>
       <c r="F53" s="6">
-        <v>0.50821873141914575</v>
+        <v>0.50820080953020397</v>
       </c>
       <c r="G53" s="7">
-        <v>38562</v>
+        <v>38691</v>
       </c>
       <c r="H53" s="8">
-        <v>0.16264716560344381</v>
+        <v>0.16233749450776666</v>
       </c>
       <c r="I53" s="7">
-        <v>42042</v>
+        <v>42067</v>
       </c>
       <c r="J53" s="5">
-        <v>4868</v>
+        <v>4882</v>
       </c>
       <c r="K53" s="6">
-        <v>0.11578897293183008</v>
+        <v>0.11605296313024462</v>
       </c>
       <c r="L53" s="5">
-        <v>1368</v>
+        <v>1387</v>
       </c>
       <c r="M53" s="10">
-        <v>2.6057142849999999E-2</v>
+        <v>2.642307399E-2</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2949,37 +2855,37 @@
         <v>8</v>
       </c>
       <c r="C54" s="19">
-        <v>56479</v>
+        <v>56460</v>
       </c>
       <c r="D54" s="20">
         <v>42</v>
       </c>
       <c r="E54" s="21">
-        <v>0.49713329297389697</v>
+        <v>0.49708779366973621</v>
       </c>
       <c r="F54" s="21">
-        <v>0.50286670702610303</v>
+        <v>0.50291220633026379</v>
       </c>
       <c r="G54" s="19">
-        <v>41513</v>
+        <v>41547</v>
       </c>
       <c r="H54" s="22">
-        <v>0.15734830053236334</v>
+        <v>0.15738801838881267</v>
       </c>
       <c r="I54" s="19">
-        <v>44859</v>
+        <v>44892</v>
       </c>
       <c r="J54" s="20">
-        <v>4519</v>
+        <v>4516</v>
       </c>
       <c r="K54" s="21">
-        <v>0.10073786754051584</v>
+        <v>0.10059698832754166</v>
       </c>
       <c r="L54" s="20">
-        <v>1112</v>
+        <v>1127</v>
       </c>
       <c r="M54" s="23">
-        <v>1.9688733860000002E-2</v>
+        <v>1.9961034360000001E-2</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2990,37 +2896,37 @@
         <v>9</v>
       </c>
       <c r="C55" s="7">
-        <v>58521</v>
+        <v>58502</v>
       </c>
       <c r="D55" s="5">
         <v>40</v>
       </c>
       <c r="E55" s="6">
-        <v>0.50704031634144242</v>
+        <v>0.50705097337827609</v>
       </c>
       <c r="F55" s="6">
-        <v>0.49295968365855758</v>
+        <v>0.49294902662172385</v>
       </c>
       <c r="G55" s="7">
-        <v>43157</v>
+        <v>43205</v>
       </c>
       <c r="H55" s="8">
-        <v>0.15478369673517622</v>
+        <v>0.15470431663001968</v>
       </c>
       <c r="I55" s="7">
-        <v>46156</v>
+        <v>46193</v>
       </c>
       <c r="J55" s="5">
-        <v>4059</v>
+        <v>4076</v>
       </c>
       <c r="K55" s="6">
-        <v>8.794089609151573E-2</v>
+        <v>8.8238477691425107E-2</v>
       </c>
       <c r="L55" s="5">
-        <v>908</v>
+        <v>939</v>
       </c>
       <c r="M55" s="10">
-        <v>1.551579774E-2</v>
+        <v>1.6050733300000002E-2</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3031,37 +2937,37 @@
         <v>10</v>
       </c>
       <c r="C56" s="19">
-        <v>71470</v>
+        <v>71452</v>
       </c>
       <c r="D56" s="20">
         <v>39</v>
       </c>
       <c r="E56" s="21">
-        <v>0.50271968885632157</v>
+        <v>0.50269904582035485</v>
       </c>
       <c r="F56" s="21">
-        <v>0.49728031114367849</v>
+        <v>0.49730095417964509</v>
       </c>
       <c r="G56" s="19">
-        <v>51926</v>
+        <v>52136</v>
       </c>
       <c r="H56" s="22">
-        <v>0.15547124754458266</v>
+        <v>0.15597667638483964</v>
       </c>
       <c r="I56" s="19">
-        <v>54983</v>
+        <v>55073</v>
       </c>
       <c r="J56" s="32">
-        <v>4492</v>
+        <v>4516</v>
       </c>
       <c r="K56" s="21">
-        <v>8.1697979375443319E-2</v>
+        <v>8.2000254208051127E-2</v>
       </c>
       <c r="L56" s="32">
-        <v>932</v>
+        <v>970</v>
       </c>
       <c r="M56" s="23">
-        <v>1.304043654E-2</v>
+        <v>1.3575547219999999E-2</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3072,37 +2978,37 @@
         <v>11</v>
       </c>
       <c r="C57" s="7">
-        <v>92815</v>
+        <v>92789</v>
       </c>
       <c r="D57" s="5">
         <v>39</v>
       </c>
       <c r="E57" s="6">
-        <v>0.50400494250008132</v>
+        <v>0.50402246508803883</v>
       </c>
       <c r="F57" s="6">
-        <v>0.49599505749991873</v>
+        <v>0.49597753491196112</v>
       </c>
       <c r="G57" s="7">
-        <v>65879</v>
+        <v>66913</v>
       </c>
       <c r="H57" s="8">
-        <v>0.15268902078052188</v>
+        <v>0.15363232854602243</v>
       </c>
       <c r="I57" s="7">
-        <v>70094</v>
+        <v>70649</v>
       </c>
       <c r="J57" s="5">
-        <v>5135</v>
+        <v>5228</v>
       </c>
       <c r="K57" s="6">
-        <v>7.3258766798870084E-2</v>
+        <v>7.3999631983467568E-2</v>
       </c>
       <c r="L57" s="5">
-        <v>994</v>
+        <v>1092</v>
       </c>
       <c r="M57" s="10">
-        <v>1.0709475830000001E-2</v>
+        <v>1.1768636359999999E-2</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3113,37 +3019,37 @@
         <v>12</v>
       </c>
       <c r="C58" s="19">
-        <v>116666</v>
+        <v>116631</v>
       </c>
       <c r="D58" s="20">
         <v>38</v>
       </c>
       <c r="E58" s="21">
-        <v>0.50792883471595174</v>
+        <v>0.50801229472811726</v>
       </c>
       <c r="F58" s="21">
-        <v>0.49207116528404826</v>
+        <v>0.49198770527188274</v>
       </c>
       <c r="G58" s="19">
-        <v>78845</v>
+        <v>80233</v>
       </c>
       <c r="H58" s="22">
-        <v>0.1552793455513983</v>
+        <v>0.15568407014570065</v>
       </c>
       <c r="I58" s="19">
-        <v>86285</v>
+        <v>87289</v>
       </c>
       <c r="J58" s="32">
-        <v>5908</v>
+        <v>6071</v>
       </c>
       <c r="K58" s="21">
-        <v>6.8470765486469257E-2</v>
+        <v>6.9550573382671357E-2</v>
       </c>
       <c r="L58" s="32">
-        <v>1032</v>
+        <v>1213</v>
       </c>
       <c r="M58" s="23">
-        <v>8.84576483E-3</v>
+        <v>1.040032238E-2</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3154,37 +3060,37 @@
         <v>13</v>
       </c>
       <c r="C59" s="7">
-        <v>110482</v>
+        <v>110441</v>
       </c>
       <c r="D59" s="5">
         <v>39</v>
       </c>
       <c r="E59" s="6">
-        <v>0.51245259626604434</v>
+        <v>0.51235389580788093</v>
       </c>
       <c r="F59" s="6">
-        <v>0.48754740373395566</v>
+        <v>0.48764610419211901</v>
       </c>
       <c r="G59" s="7">
-        <v>71816</v>
+        <v>73414</v>
       </c>
       <c r="H59" s="8">
-        <v>0.15166536704912553</v>
+        <v>0.15215081592066909</v>
       </c>
       <c r="I59" s="7">
-        <v>79097</v>
+        <v>80286</v>
       </c>
       <c r="J59" s="5">
-        <v>5611</v>
+        <v>5868</v>
       </c>
       <c r="K59" s="6">
-        <v>7.0938215102974822E-2</v>
+        <v>7.3088707869367012E-2</v>
       </c>
       <c r="L59" s="5">
-        <v>857</v>
+        <v>1113</v>
       </c>
       <c r="M59" s="10">
-        <v>7.7569196700000001E-3</v>
+        <v>1.007777908E-2</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3195,1072 +3101,1148 @@
         <v>14</v>
       </c>
       <c r="C60" s="19">
-        <v>118417</v>
+        <v>118588</v>
       </c>
       <c r="D60" s="20">
         <v>39</v>
       </c>
       <c r="E60" s="21">
-        <v>0.5078737143002986</v>
+        <v>0.50755633288617952</v>
       </c>
       <c r="F60" s="21">
-        <v>0.4921262856997014</v>
+        <v>0.49244366711382043</v>
       </c>
       <c r="G60" s="19">
-        <v>74603</v>
+        <v>77964</v>
       </c>
       <c r="H60" s="22">
-        <v>0.13738053429486749</v>
+        <v>0.1378071930634652</v>
       </c>
       <c r="I60" s="19">
-        <v>82456</v>
+        <v>85169</v>
       </c>
       <c r="J60" s="32">
-        <v>5424</v>
+        <v>6070</v>
       </c>
       <c r="K60" s="21">
-        <v>6.5780537498787234E-2</v>
+        <v>7.1270063051110152E-2</v>
       </c>
       <c r="L60" s="32">
-        <v>496</v>
+        <v>849</v>
       </c>
       <c r="M60" s="23">
-        <v>4.18858778E-3</v>
+        <v>7.1592403900000001E-3</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="18">
+      <c r="A61" s="17">
         <v>2021</v>
       </c>
-      <c r="B61" s="18">
+      <c r="B61" s="17">
         <v>15</v>
       </c>
-      <c r="C61" s="19">
-        <v>140789</v>
-      </c>
-      <c r="D61" s="20">
+      <c r="C61" s="7">
+        <v>142522</v>
+      </c>
+      <c r="D61" s="5">
         <v>38</v>
       </c>
-      <c r="E61" s="21">
-        <v>0.5102487705065154</v>
-      </c>
-      <c r="F61" s="21">
-        <v>0.4897512294934846</v>
-      </c>
-      <c r="G61" s="19">
-        <v>74445</v>
-      </c>
-      <c r="H61" s="22">
-        <v>0.15658539861642823</v>
-      </c>
-      <c r="I61" s="19">
-        <v>89745</v>
-      </c>
-      <c r="J61" s="32">
-        <v>3965</v>
-      </c>
-      <c r="K61" s="21">
-        <v>4.4180734302746674E-2</v>
-      </c>
-      <c r="L61" s="32">
-        <v>180</v>
-      </c>
-      <c r="M61" s="23">
-        <v>1.2785089700000001E-3</v>
+      <c r="E61" s="6">
+        <v>0.51026303678266716</v>
+      </c>
+      <c r="F61" s="6">
+        <v>0.48973696321733279</v>
+      </c>
+      <c r="G61" s="7">
+        <v>87364</v>
+      </c>
+      <c r="H61" s="8">
+        <v>0.15506387070189093</v>
+      </c>
+      <c r="I61" s="7">
+        <v>99114</v>
+      </c>
+      <c r="J61" s="5">
+        <v>5536</v>
+      </c>
+      <c r="K61" s="6">
+        <v>5.5854874185281594E-2</v>
+      </c>
+      <c r="L61" s="5">
+        <v>535</v>
+      </c>
+      <c r="M61" s="10">
+        <v>3.7538064200000002E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="18">
+        <v>2021</v>
+      </c>
+      <c r="B62" s="18">
+        <v>16</v>
+      </c>
+      <c r="C62" s="19">
+        <v>144068</v>
+      </c>
+      <c r="D62" s="20">
+        <v>37</v>
+      </c>
+      <c r="E62" s="21">
+        <v>0.51943199853926425</v>
+      </c>
+      <c r="F62" s="21">
+        <v>0.48056800146073569</v>
+      </c>
+      <c r="G62" s="19">
+        <v>75752</v>
+      </c>
+      <c r="H62" s="22">
+        <v>0.16787675572922167</v>
+      </c>
+      <c r="I62" s="19">
+        <v>92276</v>
+      </c>
+      <c r="J62" s="32">
+        <v>4004</v>
+      </c>
+      <c r="K62" s="21">
+        <v>4.3391564437123414E-2</v>
+      </c>
+      <c r="L62" s="32">
+        <v>161</v>
+      </c>
+      <c r="M62" s="23">
+        <v>1.11752783E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EE44EF-F204-44BC-9DFD-46318AB81991}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:I34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="33"/>
+    <col min="2" max="2" width="13.85546875" style="33" customWidth="1"/>
+    <col min="3" max="8" width="14.140625" style="33" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="33"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+      <c r="C1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="33" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="33" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B3" s="35">
+        <v>37</v>
+      </c>
+      <c r="C3" s="33">
+        <v>12</v>
+      </c>
+      <c r="D3" s="33">
+        <v>12</v>
+      </c>
+      <c r="E3" s="33">
+        <v>50</v>
+      </c>
+      <c r="F3" s="33">
+        <v>157</v>
+      </c>
+      <c r="G3" s="33">
+        <v>138</v>
+      </c>
+      <c r="H3" s="33">
+        <v>96</v>
+      </c>
+      <c r="I3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B4" s="35">
+        <v>38</v>
+      </c>
+      <c r="C4" s="33">
+        <v>8</v>
+      </c>
+      <c r="D4" s="33">
+        <v>10</v>
+      </c>
+      <c r="E4" s="33">
+        <v>77</v>
+      </c>
+      <c r="F4" s="33">
+        <v>235</v>
+      </c>
+      <c r="G4" s="33">
+        <v>206</v>
+      </c>
+      <c r="H4" s="33">
+        <v>138</v>
+      </c>
+      <c r="I4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B5" s="35">
+        <v>39</v>
+      </c>
+      <c r="C5" s="33">
+        <v>9</v>
+      </c>
+      <c r="D5" s="33">
+        <v>7</v>
+      </c>
+      <c r="E5" s="33">
+        <v>112</v>
+      </c>
+      <c r="F5" s="33">
+        <v>237</v>
+      </c>
+      <c r="G5" s="33">
+        <v>253</v>
+      </c>
+      <c r="H5" s="33">
+        <v>153</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B6" s="35">
+        <v>40</v>
+      </c>
+      <c r="C6" s="33">
+        <v>15</v>
+      </c>
+      <c r="D6" s="33">
+        <v>9</v>
+      </c>
+      <c r="E6" s="33">
+        <v>115</v>
+      </c>
+      <c r="F6" s="33">
+        <v>274</v>
+      </c>
+      <c r="G6" s="33">
+        <v>286</v>
+      </c>
+      <c r="H6" s="33">
+        <v>175</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B7" s="35">
+        <v>41</v>
+      </c>
+      <c r="C7" s="33">
+        <v>21</v>
+      </c>
+      <c r="D7" s="33">
+        <v>17</v>
+      </c>
+      <c r="E7" s="33">
+        <v>207</v>
+      </c>
+      <c r="F7" s="33">
+        <v>488</v>
+      </c>
+      <c r="G7" s="33">
+        <v>502</v>
+      </c>
+      <c r="H7" s="33">
+        <v>351</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B8" s="35">
+        <v>42</v>
+      </c>
+      <c r="C8" s="33">
+        <v>24</v>
+      </c>
+      <c r="D8" s="33">
+        <v>25</v>
+      </c>
+      <c r="E8" s="33">
+        <v>263</v>
+      </c>
+      <c r="F8" s="33">
+        <v>672</v>
+      </c>
+      <c r="G8" s="33">
+        <v>781</v>
+      </c>
+      <c r="H8" s="33">
+        <v>559</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B9" s="35">
+        <v>43</v>
+      </c>
+      <c r="C9" s="33">
+        <v>50</v>
+      </c>
+      <c r="D9" s="33">
+        <v>30</v>
+      </c>
+      <c r="E9" s="33">
+        <v>429</v>
+      </c>
+      <c r="F9" s="33">
+        <v>1050</v>
+      </c>
+      <c r="G9" s="33">
+        <v>1412</v>
+      </c>
+      <c r="H9" s="33">
+        <v>1123</v>
+      </c>
+      <c r="I9" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B10" s="35">
+        <v>44</v>
+      </c>
+      <c r="C10" s="33">
+        <v>64</v>
+      </c>
+      <c r="D10" s="33">
+        <v>49</v>
+      </c>
+      <c r="E10" s="33">
+        <v>544</v>
+      </c>
+      <c r="F10" s="33">
+        <v>1492</v>
+      </c>
+      <c r="G10" s="33">
+        <v>2079</v>
+      </c>
+      <c r="H10" s="33">
+        <v>1682</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B11" s="35">
+        <v>45</v>
+      </c>
+      <c r="C11" s="33">
+        <v>65</v>
+      </c>
+      <c r="D11" s="33">
+        <v>58</v>
+      </c>
+      <c r="E11" s="33">
+        <v>602</v>
+      </c>
+      <c r="F11" s="33">
+        <v>1683</v>
+      </c>
+      <c r="G11" s="33">
+        <v>2380</v>
+      </c>
+      <c r="H11" s="33">
+        <v>2044</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B12" s="35">
+        <v>46</v>
+      </c>
+      <c r="C12" s="33">
+        <v>64</v>
+      </c>
+      <c r="D12" s="33">
+        <v>68</v>
+      </c>
+      <c r="E12" s="33">
+        <v>569</v>
+      </c>
+      <c r="F12" s="33">
+        <v>1707</v>
+      </c>
+      <c r="G12" s="33">
+        <v>2562</v>
+      </c>
+      <c r="H12" s="33">
+        <v>2494</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B13" s="35">
+        <v>47</v>
+      </c>
+      <c r="C13" s="33">
+        <v>54</v>
+      </c>
+      <c r="D13" s="33">
+        <v>54</v>
+      </c>
+      <c r="E13" s="33">
+        <v>601</v>
+      </c>
+      <c r="F13" s="33">
+        <v>1658</v>
+      </c>
+      <c r="G13" s="33">
+        <v>2839</v>
+      </c>
+      <c r="H13" s="33">
+        <v>2807</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B14" s="35">
+        <v>48</v>
+      </c>
+      <c r="C14" s="33">
+        <v>62</v>
+      </c>
+      <c r="D14" s="33">
+        <v>68</v>
+      </c>
+      <c r="E14" s="33">
+        <v>557</v>
+      </c>
+      <c r="F14" s="33">
+        <v>1678</v>
+      </c>
+      <c r="G14" s="33">
+        <v>2843</v>
+      </c>
+      <c r="H14" s="33">
+        <v>3038</v>
+      </c>
+      <c r="I14" s="34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B15" s="35">
+        <v>49</v>
+      </c>
+      <c r="C15" s="33">
+        <v>58</v>
+      </c>
+      <c r="D15" s="33">
+        <v>58</v>
+      </c>
+      <c r="E15" s="33">
+        <v>591</v>
+      </c>
+      <c r="F15" s="33">
+        <v>1653</v>
+      </c>
+      <c r="G15" s="33">
+        <v>3145</v>
+      </c>
+      <c r="H15" s="33">
+        <v>3576</v>
+      </c>
+      <c r="I15" s="34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B16" s="35">
+        <v>50</v>
+      </c>
+      <c r="C16" s="33">
+        <v>70</v>
+      </c>
+      <c r="D16" s="33">
+        <v>66</v>
+      </c>
+      <c r="E16" s="33">
+        <v>670</v>
+      </c>
+      <c r="F16" s="33">
+        <v>1946</v>
+      </c>
+      <c r="G16" s="33">
+        <v>3899</v>
+      </c>
+      <c r="H16" s="33">
+        <v>4498</v>
+      </c>
+      <c r="I16" s="34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B17" s="35">
+        <v>51</v>
+      </c>
+      <c r="C17" s="33">
+        <v>78</v>
+      </c>
+      <c r="D17" s="33">
+        <v>87</v>
+      </c>
+      <c r="E17" s="33">
+        <v>703</v>
+      </c>
+      <c r="F17" s="33">
+        <v>2159</v>
+      </c>
+      <c r="G17" s="33">
+        <v>4325</v>
+      </c>
+      <c r="H17" s="33">
+        <v>5037</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B18" s="35">
+        <v>52</v>
+      </c>
+      <c r="C18" s="33">
+        <v>54</v>
+      </c>
+      <c r="D18" s="33">
+        <v>49</v>
+      </c>
+      <c r="E18" s="33">
+        <v>595</v>
+      </c>
+      <c r="F18" s="33">
+        <v>1828</v>
+      </c>
+      <c r="G18" s="33">
+        <v>3842</v>
+      </c>
+      <c r="H18" s="33">
+        <v>4534</v>
+      </c>
+      <c r="I18" s="34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="35">
+        <v>2020</v>
+      </c>
+      <c r="B19" s="35">
+        <v>53</v>
+      </c>
+      <c r="C19" s="33">
+        <v>74</v>
+      </c>
+      <c r="D19" s="33">
+        <v>51</v>
+      </c>
+      <c r="E19" s="33">
+        <v>604</v>
+      </c>
+      <c r="F19" s="33">
+        <v>1869</v>
+      </c>
+      <c r="G19" s="33">
+        <v>3783</v>
+      </c>
+      <c r="H19" s="33">
+        <v>4395</v>
+      </c>
+      <c r="I19" s="34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B20" s="35">
+        <v>1</v>
+      </c>
+      <c r="C20" s="33">
+        <v>64</v>
+      </c>
+      <c r="D20" s="33">
+        <v>33</v>
+      </c>
+      <c r="E20" s="33">
+        <v>568</v>
+      </c>
+      <c r="F20" s="33">
+        <v>1754</v>
+      </c>
+      <c r="G20" s="33">
+        <v>3851</v>
+      </c>
+      <c r="H20" s="33">
+        <v>4560</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B21" s="35">
+        <v>2</v>
+      </c>
+      <c r="C21" s="33">
+        <v>58</v>
+      </c>
+      <c r="D21" s="33">
+        <v>47</v>
+      </c>
+      <c r="E21" s="33">
+        <v>508</v>
+      </c>
+      <c r="F21" s="33">
+        <v>1546</v>
+      </c>
+      <c r="G21" s="33">
+        <v>3289</v>
+      </c>
+      <c r="H21" s="33">
+        <v>4111</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B22" s="35">
+        <v>3</v>
+      </c>
+      <c r="C22" s="33">
+        <v>39</v>
+      </c>
+      <c r="D22" s="33">
+        <v>36</v>
+      </c>
+      <c r="E22" s="33">
+        <v>388</v>
+      </c>
+      <c r="F22" s="33">
+        <v>1409</v>
+      </c>
+      <c r="G22" s="33">
+        <v>3049</v>
+      </c>
+      <c r="H22" s="33">
+        <v>3585</v>
+      </c>
+      <c r="I22" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B23" s="35">
+        <v>4</v>
+      </c>
+      <c r="C23" s="33">
+        <v>34</v>
+      </c>
+      <c r="D23" s="33">
+        <v>30</v>
+      </c>
+      <c r="E23" s="33">
+        <v>388</v>
+      </c>
+      <c r="F23" s="33">
+        <v>1179</v>
+      </c>
+      <c r="G23" s="33">
+        <v>2693</v>
+      </c>
+      <c r="H23" s="33">
+        <v>2893</v>
+      </c>
+      <c r="I23" s="34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B24" s="35">
+        <v>5</v>
+      </c>
+      <c r="C24" s="33">
+        <v>43</v>
+      </c>
+      <c r="D24" s="33">
+        <v>38</v>
+      </c>
+      <c r="E24" s="33">
+        <v>344</v>
+      </c>
+      <c r="F24" s="33">
+        <v>1080</v>
+      </c>
+      <c r="G24" s="33">
+        <v>2248</v>
+      </c>
+      <c r="H24" s="33">
+        <v>2418</v>
+      </c>
+      <c r="I24" s="34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B25" s="35">
+        <v>6</v>
+      </c>
+      <c r="C25" s="33">
+        <v>38</v>
+      </c>
+      <c r="D25" s="33">
+        <v>23</v>
+      </c>
+      <c r="E25" s="33">
+        <v>284</v>
+      </c>
+      <c r="F25" s="33">
+        <v>934</v>
+      </c>
+      <c r="G25" s="33">
+        <v>1859</v>
+      </c>
+      <c r="H25" s="33">
+        <v>1812</v>
+      </c>
+      <c r="I25" s="34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B26" s="35">
+        <v>7</v>
+      </c>
+      <c r="C26" s="33">
+        <v>35</v>
+      </c>
+      <c r="D26" s="33">
+        <v>22</v>
+      </c>
+      <c r="E26" s="33">
+        <v>298</v>
+      </c>
+      <c r="F26" s="33">
+        <v>992</v>
+      </c>
+      <c r="G26" s="33">
+        <v>1922</v>
+      </c>
+      <c r="H26" s="33">
+        <v>1612</v>
+      </c>
+      <c r="I26" s="34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B27" s="35">
+        <v>8</v>
+      </c>
+      <c r="C27" s="33">
+        <v>43</v>
+      </c>
+      <c r="D27" s="33">
+        <v>31</v>
+      </c>
+      <c r="E27" s="33">
+        <v>303</v>
+      </c>
+      <c r="F27" s="33">
+        <v>1013</v>
+      </c>
+      <c r="G27" s="33">
+        <v>1700</v>
+      </c>
+      <c r="H27" s="33">
+        <v>1426</v>
+      </c>
+      <c r="I27" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B28" s="35">
+        <v>9</v>
+      </c>
+      <c r="C28" s="33">
+        <v>49</v>
+      </c>
+      <c r="D28" s="33">
+        <v>28</v>
+      </c>
+      <c r="E28" s="33">
+        <v>314</v>
+      </c>
+      <c r="F28" s="33">
+        <v>967</v>
+      </c>
+      <c r="G28" s="33">
+        <v>1531</v>
+      </c>
+      <c r="H28" s="33">
+        <v>1187</v>
+      </c>
+      <c r="I28" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B29" s="35">
+        <v>10</v>
+      </c>
+      <c r="C29" s="33">
+        <v>50</v>
+      </c>
+      <c r="D29" s="33">
+        <v>36</v>
+      </c>
+      <c r="E29" s="33">
+        <v>375</v>
+      </c>
+      <c r="F29" s="33">
+        <v>1247</v>
+      </c>
+      <c r="G29" s="33">
+        <v>1604</v>
+      </c>
+      <c r="H29" s="33">
+        <v>1204</v>
+      </c>
+      <c r="I29" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B30" s="35">
+        <v>11</v>
+      </c>
+      <c r="C30" s="33">
+        <v>74</v>
+      </c>
+      <c r="D30" s="33">
+        <v>65</v>
+      </c>
+      <c r="E30" s="33">
+        <v>438</v>
+      </c>
+      <c r="F30" s="33">
+        <v>1460</v>
+      </c>
+      <c r="G30" s="33">
+        <v>1968</v>
+      </c>
+      <c r="H30" s="33">
+        <v>1221</v>
+      </c>
+      <c r="I30" s="34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B31" s="35">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>50</v>
-      </c>
-      <c r="F3">
-        <v>156</v>
-      </c>
-      <c r="G3">
-        <v>138</v>
-      </c>
-      <c r="H3">
-        <v>96</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="C31" s="33">
+        <v>78</v>
+      </c>
+      <c r="D31" s="33">
+        <v>74</v>
+      </c>
+      <c r="E31" s="33">
+        <v>552</v>
+      </c>
+      <c r="F31" s="33">
+        <v>1728</v>
+      </c>
+      <c r="G31" s="33">
+        <v>2244</v>
+      </c>
+      <c r="H31" s="33">
+        <v>1394</v>
+      </c>
+      <c r="I31" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B32" s="35">
+        <v>13</v>
+      </c>
+      <c r="C32" s="33">
+        <v>81</v>
+      </c>
+      <c r="D32" s="33">
+        <v>84</v>
+      </c>
+      <c r="E32" s="33">
+        <v>520</v>
+      </c>
+      <c r="F32" s="33">
+        <v>1695</v>
+      </c>
+      <c r="G32" s="33">
+        <v>2228</v>
+      </c>
+      <c r="H32" s="33">
+        <v>1259</v>
+      </c>
+      <c r="I32" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B33" s="35">
+        <v>14</v>
+      </c>
+      <c r="C33" s="33">
+        <v>87</v>
+      </c>
+      <c r="D33" s="33">
+        <v>58</v>
+      </c>
+      <c r="E33" s="33">
+        <v>629</v>
+      </c>
+      <c r="F33" s="33">
+        <v>1845</v>
+      </c>
+      <c r="G33" s="33">
+        <v>2248</v>
+      </c>
+      <c r="H33" s="33">
+        <v>1201</v>
+      </c>
+      <c r="I33" s="34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B34" s="35">
+        <v>15</v>
+      </c>
+      <c r="C34" s="33">
+        <v>82</v>
+      </c>
+      <c r="D34" s="33">
+        <v>77</v>
+      </c>
+      <c r="E34" s="33">
+        <v>593</v>
+      </c>
+      <c r="F34" s="33">
+        <v>1585</v>
+      </c>
+      <c r="G34" s="33">
+        <v>2098</v>
+      </c>
+      <c r="H34" s="33">
+        <v>1096</v>
+      </c>
+      <c r="I34" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="35">
+        <v>2021</v>
+      </c>
+      <c r="B35" s="35">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>77</v>
-      </c>
-      <c r="F4">
-        <v>235</v>
-      </c>
-      <c r="G4">
-        <v>206</v>
-      </c>
-      <c r="H4">
-        <v>138</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-      <c r="E5">
-        <v>112</v>
-      </c>
-      <c r="F5">
-        <v>237</v>
-      </c>
-      <c r="G5">
-        <v>253</v>
-      </c>
-      <c r="H5">
-        <v>153</v>
-      </c>
-      <c r="I5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>115</v>
-      </c>
-      <c r="F6">
-        <v>274</v>
-      </c>
-      <c r="G6">
-        <v>287</v>
-      </c>
-      <c r="H6">
-        <v>175</v>
-      </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7">
-        <v>21</v>
-      </c>
-      <c r="D7">
-        <v>17</v>
-      </c>
-      <c r="E7">
-        <v>206</v>
-      </c>
-      <c r="F7">
-        <v>488</v>
-      </c>
-      <c r="G7">
-        <v>502</v>
-      </c>
-      <c r="H7">
-        <v>351</v>
-      </c>
-      <c r="I7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8">
-        <v>24</v>
-      </c>
-      <c r="D8">
-        <v>25</v>
-      </c>
-      <c r="E8">
-        <v>262</v>
-      </c>
-      <c r="F8">
-        <v>672</v>
-      </c>
-      <c r="G8">
-        <v>780</v>
-      </c>
-      <c r="H8">
-        <v>559</v>
-      </c>
-      <c r="I8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9">
-        <v>50</v>
-      </c>
-      <c r="D9">
-        <v>30</v>
-      </c>
-      <c r="E9">
-        <v>428</v>
-      </c>
-      <c r="F9">
-        <v>1051</v>
-      </c>
-      <c r="G9">
-        <v>1412</v>
-      </c>
-      <c r="H9">
-        <v>1123</v>
-      </c>
-      <c r="I9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10">
-        <v>64</v>
-      </c>
-      <c r="D10">
-        <v>49</v>
-      </c>
-      <c r="E10">
-        <v>541</v>
-      </c>
-      <c r="F10">
-        <v>1490</v>
-      </c>
-      <c r="G10">
-        <v>2076</v>
-      </c>
-      <c r="H10">
-        <v>1682</v>
-      </c>
-      <c r="I10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11">
-        <v>65</v>
-      </c>
-      <c r="D11">
-        <v>58</v>
-      </c>
-      <c r="E11">
-        <v>601</v>
-      </c>
-      <c r="F11">
-        <v>1680</v>
-      </c>
-      <c r="G11">
-        <v>2378</v>
-      </c>
-      <c r="H11">
-        <v>2044</v>
-      </c>
-      <c r="I11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12">
-        <v>64</v>
-      </c>
-      <c r="D12">
-        <v>68</v>
-      </c>
-      <c r="E12">
-        <v>569</v>
-      </c>
-      <c r="F12">
-        <v>1707</v>
-      </c>
-      <c r="G12">
-        <v>2559</v>
-      </c>
-      <c r="H12">
-        <v>2492</v>
-      </c>
-      <c r="I12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13">
-        <v>54</v>
-      </c>
-      <c r="D13">
-        <v>54</v>
-      </c>
-      <c r="E13">
-        <v>598</v>
-      </c>
-      <c r="F13">
-        <v>1655</v>
-      </c>
-      <c r="G13">
-        <v>2838</v>
-      </c>
-      <c r="H13">
-        <v>2806</v>
-      </c>
-      <c r="I13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14">
+      <c r="C35" s="33">
+        <v>70</v>
+      </c>
+      <c r="D35" s="33">
         <v>63</v>
       </c>
-      <c r="D14">
-        <v>68</v>
-      </c>
-      <c r="E14">
-        <v>555</v>
-      </c>
-      <c r="F14">
-        <v>1675</v>
-      </c>
-      <c r="G14">
-        <v>2844</v>
-      </c>
-      <c r="H14">
-        <v>3040</v>
-      </c>
-      <c r="I14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15">
-        <v>58</v>
-      </c>
-      <c r="D15">
-        <v>58</v>
-      </c>
-      <c r="E15">
-        <v>591</v>
-      </c>
-      <c r="F15">
-        <v>1651</v>
-      </c>
-      <c r="G15">
-        <v>3144</v>
-      </c>
-      <c r="H15">
-        <v>3574</v>
-      </c>
-      <c r="I15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16">
-        <v>70</v>
-      </c>
-      <c r="D16">
-        <v>66</v>
-      </c>
-      <c r="E16">
-        <v>667</v>
-      </c>
-      <c r="F16">
-        <v>1940</v>
-      </c>
-      <c r="G16">
-        <v>3899</v>
-      </c>
-      <c r="H16">
-        <v>4490</v>
-      </c>
-      <c r="I16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17">
-        <v>78</v>
-      </c>
-      <c r="D17">
-        <v>83</v>
-      </c>
-      <c r="E17">
-        <v>694</v>
-      </c>
-      <c r="F17">
-        <v>2147</v>
-      </c>
-      <c r="G17">
-        <v>4311</v>
-      </c>
-      <c r="H17">
-        <v>5024</v>
-      </c>
-      <c r="I17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18">
-        <v>53</v>
-      </c>
-      <c r="D18">
-        <v>49</v>
-      </c>
-      <c r="E18">
-        <v>593</v>
-      </c>
-      <c r="F18">
-        <v>1827</v>
-      </c>
-      <c r="G18">
-        <v>3838</v>
-      </c>
-      <c r="H18">
-        <v>4526</v>
-      </c>
-      <c r="I18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19">
-        <v>74</v>
-      </c>
-      <c r="D19">
-        <v>51</v>
-      </c>
-      <c r="E19">
-        <v>602</v>
-      </c>
-      <c r="F19">
-        <v>1863</v>
-      </c>
-      <c r="G19">
-        <v>3780</v>
-      </c>
-      <c r="H19">
-        <v>4391</v>
-      </c>
-      <c r="I19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20">
-        <v>64</v>
-      </c>
-      <c r="D20">
-        <v>32</v>
-      </c>
-      <c r="E20">
-        <v>563</v>
-      </c>
-      <c r="F20">
-        <v>1748</v>
-      </c>
-      <c r="G20">
-        <v>3847</v>
-      </c>
-      <c r="H20">
-        <v>4555</v>
-      </c>
-      <c r="I20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21">
-        <v>58</v>
-      </c>
-      <c r="D21">
-        <v>46</v>
-      </c>
-      <c r="E21">
-        <v>506</v>
-      </c>
-      <c r="F21">
-        <v>1542</v>
-      </c>
-      <c r="G21">
-        <v>3283</v>
-      </c>
-      <c r="H21">
-        <v>4108</v>
-      </c>
-      <c r="I21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22">
-        <v>39</v>
-      </c>
-      <c r="D22">
-        <v>36</v>
-      </c>
-      <c r="E22">
-        <v>385</v>
-      </c>
-      <c r="F22">
-        <v>1409</v>
-      </c>
-      <c r="G22">
-        <v>3048</v>
-      </c>
-      <c r="H22">
-        <v>3581</v>
-      </c>
-      <c r="I22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23">
-        <v>33</v>
-      </c>
-      <c r="D23">
-        <v>30</v>
-      </c>
-      <c r="E23">
-        <v>388</v>
-      </c>
-      <c r="F23">
-        <v>1174</v>
-      </c>
-      <c r="G23">
-        <v>2678</v>
-      </c>
-      <c r="H23">
-        <v>2876</v>
-      </c>
-      <c r="I23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24">
-        <v>42</v>
-      </c>
-      <c r="D24">
-        <v>37</v>
-      </c>
-      <c r="E24">
-        <v>344</v>
-      </c>
-      <c r="F24">
-        <v>1078</v>
-      </c>
-      <c r="G24">
-        <v>2243</v>
-      </c>
-      <c r="H24">
-        <v>2406</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="E35" s="33">
+        <v>437</v>
+      </c>
+      <c r="F35" s="33">
+        <v>1102</v>
+      </c>
+      <c r="G35" s="33">
+        <v>1522</v>
+      </c>
+      <c r="H35" s="33">
+        <v>807</v>
+      </c>
+      <c r="I35" s="34" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25">
-        <v>38</v>
-      </c>
-      <c r="D25">
-        <v>23</v>
-      </c>
-      <c r="E25">
-        <v>283</v>
-      </c>
-      <c r="F25">
-        <v>933</v>
-      </c>
-      <c r="G25">
-        <v>1857</v>
-      </c>
-      <c r="H25">
-        <v>1808</v>
-      </c>
-      <c r="I25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26">
-        <v>35</v>
-      </c>
-      <c r="D26">
-        <v>22</v>
-      </c>
-      <c r="E26">
-        <v>299</v>
-      </c>
-      <c r="F26">
-        <v>989</v>
-      </c>
-      <c r="G26">
-        <v>1914</v>
-      </c>
-      <c r="H26">
-        <v>1608</v>
-      </c>
-      <c r="I26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27">
-        <v>43</v>
-      </c>
-      <c r="D27">
-        <v>31</v>
-      </c>
-      <c r="E27">
-        <v>302</v>
-      </c>
-      <c r="F27">
-        <v>1014</v>
-      </c>
-      <c r="G27">
-        <v>1704</v>
-      </c>
-      <c r="H27">
-        <v>1425</v>
-      </c>
-      <c r="I27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28">
-        <v>49</v>
-      </c>
-      <c r="D28">
-        <v>28</v>
-      </c>
-      <c r="E28">
-        <v>314</v>
-      </c>
-      <c r="F28">
-        <v>964</v>
-      </c>
-      <c r="G28">
-        <v>1520</v>
-      </c>
-      <c r="H28">
-        <v>1183</v>
-      </c>
-      <c r="I28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29">
-        <v>50</v>
-      </c>
-      <c r="D29">
-        <v>37</v>
-      </c>
-      <c r="E29">
-        <v>374</v>
-      </c>
-      <c r="F29">
-        <v>1241</v>
-      </c>
-      <c r="G29">
-        <v>1591</v>
-      </c>
-      <c r="H29">
-        <v>1199</v>
-      </c>
-      <c r="I29" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30">
-        <v>74</v>
-      </c>
-      <c r="D30">
-        <v>65</v>
-      </c>
-      <c r="E30">
-        <v>430</v>
-      </c>
-      <c r="F30">
-        <v>1429</v>
-      </c>
-      <c r="G30">
-        <v>1927</v>
-      </c>
-      <c r="H30">
-        <v>1208</v>
-      </c>
-      <c r="I30" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31">
-        <v>74</v>
-      </c>
-      <c r="D31">
-        <v>74</v>
-      </c>
-      <c r="E31">
-        <v>546</v>
-      </c>
-      <c r="F31">
-        <v>1674</v>
-      </c>
-      <c r="G31">
-        <v>2179</v>
-      </c>
-      <c r="H31">
-        <v>1358</v>
-      </c>
-      <c r="I31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32">
-        <v>81</v>
-      </c>
-      <c r="D32">
-        <v>84</v>
-      </c>
-      <c r="E32">
-        <v>504</v>
-      </c>
-      <c r="F32">
-        <v>1617</v>
-      </c>
-      <c r="G32">
-        <v>2111</v>
-      </c>
-      <c r="H32">
-        <v>1213</v>
-      </c>
-      <c r="I32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33">
-        <v>86</v>
-      </c>
-      <c r="D33">
-        <v>59</v>
-      </c>
-      <c r="E33">
-        <v>587</v>
-      </c>
-      <c r="F33">
-        <v>1607</v>
-      </c>
-      <c r="G33">
-        <v>1987</v>
-      </c>
-      <c r="H33">
-        <v>1095</v>
-      </c>
-      <c r="I33" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34">
-        <v>69</v>
-      </c>
-      <c r="D34">
-        <v>69</v>
-      </c>
-      <c r="E34">
-        <v>455</v>
-      </c>
-      <c r="F34">
-        <v>1048</v>
-      </c>
-      <c r="G34">
-        <v>1465</v>
-      </c>
-      <c r="H34">
-        <v>852</v>
-      </c>
-      <c r="I34" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
/home/ofenloch/workspaces/COVID19/rki-data-evaluation/getRKIData.sh: add data automatically downloaded at 2021-05-05--05-03-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Klinische-Aspekte.xlsx
+++ b/rki-data/RKI-Klinische-Aspekte.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949AEF4E-AF57-43B6-8A97-49DBCC66A3C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B99830-1146-4F2B-B351-A2F8CCC330C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{3677AF26-2CAB-4FDE-A93C-D8C0E4111944}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="97">
   <si>
     <t>Meldejahr</t>
   </si>
@@ -197,10 +197,121 @@
     <t>Anteil Verstorben</t>
   </si>
   <si>
-    <t>Die dem RKI übermittelten COVID-19-Fälle nach Meldewoche und  Geschlecht sowie Anteile mit für COVID-19 relevanten Symptomen, Anteile Hospitalisierter und Verstorbener für die Meldewochen KW 10 – 53/2020 und KW 01 - 16/2021</t>
-  </si>
-  <si>
     <t>2021-KW16</t>
+  </si>
+  <si>
+    <t>Die dem RKI übermittelten COVID-19-Fälle nach Meldewoche und  Geschlecht sowie Anteile mit für COVID-19 relevanten Symptomen, Anteile Hospitalisierter und Verstorbener für die Meldewochen KW 10 – 53/2020 und KW 01 - 17/2021</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>2021-KW17</t>
   </si>
 </sst>
 </file>
@@ -384,10 +495,12 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -702,17 +815,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872BAA18-906B-41C7-A8B5-537096EA6980}">
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -826,10 +939,10 @@
         <v>5631</v>
       </c>
       <c r="J4" s="13">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="K4" s="14">
-        <v>9.4654590658852775E-2</v>
+        <v>9.4477002308648556E-2</v>
       </c>
       <c r="L4" s="13">
         <v>84</v>
@@ -846,37 +959,37 @@
         <v>12</v>
       </c>
       <c r="C5" s="7">
-        <v>22410</v>
+        <v>22408</v>
       </c>
       <c r="D5" s="5">
         <v>45</v>
       </c>
       <c r="E5" s="6">
-        <v>0.5499151709974105</v>
+        <v>0.54983032684407929</v>
       </c>
       <c r="F5" s="6">
-        <v>0.4500848290025895</v>
+        <v>0.45016967315592071</v>
       </c>
       <c r="G5" s="7">
-        <v>20156</v>
+        <v>20154</v>
       </c>
       <c r="H5" s="8">
-        <v>3.8896606469537603E-2</v>
+        <v>3.890046640865337E-2</v>
       </c>
       <c r="I5" s="7">
-        <v>19377</v>
+        <v>19375</v>
       </c>
       <c r="J5" s="7">
         <v>2230</v>
       </c>
       <c r="K5" s="6">
-        <v>0.1150848944625071</v>
+        <v>0.11509677419354838</v>
       </c>
       <c r="L5" s="5">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="M5" s="10">
-        <v>2.1195894680000001E-2</v>
+        <v>2.1153159580000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -905,19 +1018,19 @@
         <v>3.2961328834674279E-2</v>
       </c>
       <c r="I6" s="12">
-        <v>29519</v>
+        <v>29528</v>
       </c>
       <c r="J6" s="12">
-        <v>5144</v>
+        <v>5145</v>
       </c>
       <c r="K6" s="14">
-        <v>0.17426064568582947</v>
+        <v>0.17424139799512328</v>
       </c>
       <c r="L6" s="12">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="M6" s="16">
-        <v>4.3067412419999999E-2</v>
+        <v>4.2979099200000002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -928,7 +1041,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="7">
-        <v>36053</v>
+        <v>36052</v>
       </c>
       <c r="D7" s="5">
         <v>51</v>
@@ -940,25 +1053,25 @@
         <v>0.54920194309507286</v>
       </c>
       <c r="G7" s="7">
-        <v>32038</v>
+        <v>32035</v>
       </c>
       <c r="H7" s="8">
-        <v>5.5527810724764343E-2</v>
+        <v>5.553301076947089E-2</v>
       </c>
       <c r="I7" s="7">
-        <v>31615</v>
+        <v>31617</v>
       </c>
       <c r="J7" s="7">
-        <v>6092</v>
+        <v>6091</v>
       </c>
       <c r="K7" s="6">
-        <v>0.19269334176814804</v>
+        <v>0.19264952399025839</v>
       </c>
       <c r="L7" s="7">
-        <v>2261</v>
+        <v>2258</v>
       </c>
       <c r="M7" s="10">
-        <v>6.2713227740000002E-2</v>
+        <v>6.2631754129999995E-2</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -969,37 +1082,37 @@
         <v>15</v>
       </c>
       <c r="C8" s="12">
-        <v>27158</v>
+        <v>27156</v>
       </c>
       <c r="D8" s="13">
         <v>52</v>
       </c>
       <c r="E8" s="14">
-        <v>0.43469124423963135</v>
+        <v>0.43468642849242339</v>
       </c>
       <c r="F8" s="14">
-        <v>0.56530875576036865</v>
+        <v>0.56531357150757655</v>
       </c>
       <c r="G8" s="12">
-        <v>23580</v>
+        <v>23579</v>
       </c>
       <c r="H8" s="15">
-        <v>8.4605597964376597E-2</v>
+        <v>8.4609186140209514E-2</v>
       </c>
       <c r="I8" s="12">
-        <v>24151</v>
+        <v>24149</v>
       </c>
       <c r="J8" s="12">
-        <v>4731</v>
+        <v>4730</v>
       </c>
       <c r="K8" s="14">
-        <v>0.19589250962693056</v>
+        <v>0.19586732369870388</v>
       </c>
       <c r="L8" s="12">
         <v>1876</v>
       </c>
       <c r="M8" s="16">
-        <v>6.9077251630000003E-2</v>
+        <v>6.9082339069999998E-2</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1016,10 +1129,10 @@
         <v>51</v>
       </c>
       <c r="E9" s="6">
-        <v>0.44720891300583038</v>
+        <v>0.44709345956243146</v>
       </c>
       <c r="F9" s="6">
-        <v>0.55279108699416957</v>
+        <v>0.55290654043756859</v>
       </c>
       <c r="G9" s="7">
         <v>14877</v>
@@ -1028,13 +1141,13 @@
         <v>0.11474087517644686</v>
       </c>
       <c r="I9" s="7">
-        <v>15528</v>
+        <v>15529</v>
       </c>
       <c r="J9" s="7">
         <v>3378</v>
       </c>
       <c r="K9" s="6">
-        <v>0.21754250386398763</v>
+        <v>0.21752849507373301</v>
       </c>
       <c r="L9" s="7">
         <v>1217</v>
@@ -1051,37 +1164,37 @@
         <v>17</v>
       </c>
       <c r="C10" s="12">
-        <v>12362</v>
+        <v>12359</v>
       </c>
       <c r="D10" s="13">
         <v>50</v>
       </c>
       <c r="E10" s="14">
-        <v>0.44981773997569868</v>
+        <v>0.44976502997893369</v>
       </c>
       <c r="F10" s="14">
-        <v>0.55018226002430137</v>
+        <v>0.55023497002106625</v>
       </c>
       <c r="G10" s="12">
         <v>10270</v>
       </c>
       <c r="H10" s="15">
-        <v>0.139143135345667</v>
+        <v>0.13924050632911392</v>
       </c>
       <c r="I10" s="12">
-        <v>10984</v>
+        <v>10983</v>
       </c>
       <c r="J10" s="12">
         <v>2240</v>
       </c>
       <c r="K10" s="14">
-        <v>0.20393299344501092</v>
+        <v>0.20395156150414276</v>
       </c>
       <c r="L10" s="13">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="M10" s="16">
-        <v>5.8323895799999997E-2</v>
+        <v>5.8499878630000002E-2</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1092,37 +1205,37 @@
         <v>18</v>
       </c>
       <c r="C11" s="7">
-        <v>7437</v>
+        <v>7438</v>
       </c>
       <c r="D11" s="5">
         <v>48</v>
       </c>
       <c r="E11" s="6">
-        <v>0.47806781485468247</v>
+        <v>0.4778689627337549</v>
       </c>
       <c r="F11" s="6">
-        <v>0.52193218514531758</v>
+        <v>0.5221310372662451</v>
       </c>
       <c r="G11" s="7">
-        <v>6257</v>
+        <v>6258</v>
       </c>
       <c r="H11" s="8">
-        <v>0.1758031005274093</v>
+        <v>0.17561521252796419</v>
       </c>
       <c r="I11" s="7">
-        <v>6609</v>
+        <v>6610</v>
       </c>
       <c r="J11" s="7">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="K11" s="6">
-        <v>0.20638523225904071</v>
+        <v>0.20650529500756429</v>
       </c>
       <c r="L11" s="5">
         <v>386</v>
       </c>
       <c r="M11" s="10">
-        <v>5.1902648910000002E-2</v>
+        <v>5.1895670870000001E-2</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1133,16 +1246,16 @@
         <v>19</v>
       </c>
       <c r="C12" s="12">
-        <v>6238</v>
+        <v>6239</v>
       </c>
       <c r="D12" s="13">
         <v>47</v>
       </c>
       <c r="E12" s="14">
-        <v>0.48026315789473684</v>
+        <v>0.48034654259586074</v>
       </c>
       <c r="F12" s="14">
-        <v>0.51973684210526316</v>
+        <v>0.51965345740413926</v>
       </c>
       <c r="G12" s="12">
         <v>5253</v>
@@ -1163,7 +1276,7 @@
         <v>257</v>
       </c>
       <c r="M12" s="16">
-        <v>4.1199102270000003E-2</v>
+        <v>4.1192498789999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1215,37 +1328,37 @@
         <v>21</v>
       </c>
       <c r="C14" s="12">
-        <v>3608</v>
+        <v>3601</v>
       </c>
       <c r="D14" s="13">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E14" s="14">
-        <v>0.50319710870169587</v>
+        <v>0.50306406685236771</v>
       </c>
       <c r="F14" s="14">
-        <v>0.49680289129830413</v>
+        <v>0.49693593314763229</v>
       </c>
       <c r="G14" s="12">
-        <v>2837</v>
+        <v>2836</v>
       </c>
       <c r="H14" s="15">
-        <v>0.26471624955939371</v>
+        <v>0.26480959097320167</v>
       </c>
       <c r="I14" s="12">
-        <v>3120</v>
+        <v>3119</v>
       </c>
       <c r="J14" s="13">
         <v>513</v>
       </c>
       <c r="K14" s="14">
-        <v>0.16442307692307692</v>
+        <v>0.16447579352356526</v>
       </c>
       <c r="L14" s="13">
         <v>113</v>
       </c>
       <c r="M14" s="16">
-        <v>3.1319290460000003E-2</v>
+        <v>3.1380172169999998E-2</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1256,37 +1369,37 @@
         <v>22</v>
       </c>
       <c r="C15" s="7">
-        <v>3205</v>
+        <v>3207</v>
       </c>
       <c r="D15" s="5">
         <v>42</v>
       </c>
       <c r="E15" s="6">
-        <v>0.51581584716567497</v>
+        <v>0.51580594679186231</v>
       </c>
       <c r="F15" s="6">
-        <v>0.48418415283432509</v>
+        <v>0.48419405320813774</v>
       </c>
       <c r="G15" s="7">
-        <v>2548</v>
+        <v>2550</v>
       </c>
       <c r="H15" s="8">
-        <v>0.23233908948194662</v>
+        <v>0.23254901960784313</v>
       </c>
       <c r="I15" s="7">
-        <v>2769</v>
+        <v>2771</v>
       </c>
       <c r="J15" s="5">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="K15" s="6">
-        <v>0.15204044781509571</v>
+        <v>0.15229159148321905</v>
       </c>
       <c r="L15" s="5">
         <v>65</v>
       </c>
       <c r="M15" s="10">
-        <v>2.0280811230000001E-2</v>
+        <v>2.026816339E-2</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1297,16 +1410,16 @@
         <v>23</v>
       </c>
       <c r="C16" s="12">
-        <v>2352</v>
+        <v>2351</v>
       </c>
       <c r="D16" s="13">
         <v>39</v>
       </c>
       <c r="E16" s="14">
-        <v>0.50660417554324666</v>
+        <v>0.50639386189258317</v>
       </c>
       <c r="F16" s="14">
-        <v>0.49339582445675328</v>
+        <v>0.49360613810741688</v>
       </c>
       <c r="G16" s="12">
         <v>1838</v>
@@ -1327,7 +1440,7 @@
         <v>45</v>
       </c>
       <c r="M16" s="16">
-        <v>1.9132653060000001E-2</v>
+        <v>1.9140791149999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1344,16 +1457,16 @@
         <v>37</v>
       </c>
       <c r="E17" s="6">
-        <v>0.5358215358215358</v>
+        <v>0.5353925353925354</v>
       </c>
       <c r="F17" s="6">
-        <v>0.4641784641784642</v>
+        <v>0.4646074646074646</v>
       </c>
       <c r="G17" s="7">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="H17" s="8">
-        <v>0.24440619621342513</v>
+        <v>0.24426605504587157</v>
       </c>
       <c r="I17" s="7">
         <v>2088</v>
@@ -1391,10 +1504,10 @@
         <v>0.41209324915007284</v>
       </c>
       <c r="G18" s="12">
-        <v>2937</v>
+        <v>2939</v>
       </c>
       <c r="H18" s="15">
-        <v>0.2512768130745659</v>
+        <v>0.25110581830554612</v>
       </c>
       <c r="I18" s="12">
         <v>3772</v>
@@ -1420,16 +1533,16 @@
         <v>26</v>
       </c>
       <c r="C19" s="7">
-        <v>3212</v>
+        <v>3211</v>
       </c>
       <c r="D19" s="5">
         <v>37</v>
       </c>
       <c r="E19" s="6">
-        <v>0.55143391521197005</v>
+        <v>0.55129404427814155</v>
       </c>
       <c r="F19" s="6">
-        <v>0.44856608478802995</v>
+        <v>0.44870595572185845</v>
       </c>
       <c r="G19" s="7">
         <v>2330</v>
@@ -1438,19 +1551,19 @@
         <v>0.23261802575107296</v>
       </c>
       <c r="I19" s="7">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="J19" s="5">
         <v>296</v>
       </c>
       <c r="K19" s="6">
-        <v>0.10338805448829899</v>
+        <v>0.103424178895877</v>
       </c>
       <c r="L19" s="5">
         <v>23</v>
       </c>
       <c r="M19" s="10">
-        <v>7.1606475700000003E-3</v>
+        <v>7.1628776E-3</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1476,7 +1589,7 @@
         <v>2066</v>
       </c>
       <c r="H20" s="15">
-        <v>0.26718296224588578</v>
+        <v>0.26669893514036785</v>
       </c>
       <c r="I20" s="12">
         <v>2463</v>
@@ -1520,13 +1633,13 @@
         <v>0.23940020682523269</v>
       </c>
       <c r="I21" s="7">
-        <v>2192</v>
+        <v>2193</v>
       </c>
       <c r="J21" s="5">
         <v>256</v>
       </c>
       <c r="K21" s="6">
-        <v>0.11678832116788321</v>
+        <v>0.11673506611947104</v>
       </c>
       <c r="L21" s="5">
         <v>25</v>
@@ -1543,37 +1656,37 @@
         <v>29</v>
       </c>
       <c r="C22" s="12">
-        <v>3015</v>
+        <v>3016</v>
       </c>
       <c r="D22" s="13">
         <v>36</v>
       </c>
       <c r="E22" s="14">
-        <v>0.52460106382978722</v>
+        <v>0.52475905616483887</v>
       </c>
       <c r="F22" s="14">
-        <v>0.47539893617021278</v>
+        <v>0.47524094383516119</v>
       </c>
       <c r="G22" s="12">
-        <v>2360</v>
+        <v>2361</v>
       </c>
       <c r="H22" s="15">
-        <v>0.22966101694915253</v>
+        <v>0.22956374417619652</v>
       </c>
       <c r="I22" s="12">
-        <v>2646</v>
+        <v>2647</v>
       </c>
       <c r="J22" s="13">
         <v>317</v>
       </c>
       <c r="K22" s="14">
-        <v>0.11980347694633409</v>
+        <v>0.11975821684926331</v>
       </c>
       <c r="L22" s="13">
         <v>30</v>
       </c>
       <c r="M22" s="16">
-        <v>9.9502487499999997E-3</v>
+        <v>9.9469495999999994E-3</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1637,10 +1750,10 @@
         <v>0.49792272538429583</v>
       </c>
       <c r="G24" s="12">
-        <v>3715</v>
+        <v>3716</v>
       </c>
       <c r="H24" s="15">
-        <v>0.24576043068640646</v>
+        <v>0.24569429494079656</v>
       </c>
       <c r="I24" s="12">
         <v>4175</v>
@@ -1666,37 +1779,37 @@
         <v>32</v>
       </c>
       <c r="C25" s="7">
-        <v>6057</v>
+        <v>6054</v>
       </c>
       <c r="D25" s="5">
         <v>34</v>
       </c>
       <c r="E25" s="6">
-        <v>0.53679510501074912</v>
+        <v>0.53689609530112503</v>
       </c>
       <c r="F25" s="6">
-        <v>0.46320489498925088</v>
+        <v>0.46310390469887491</v>
       </c>
       <c r="G25" s="7">
-        <v>4556</v>
+        <v>4553</v>
       </c>
       <c r="H25" s="8">
-        <v>0.30026338893766463</v>
+        <v>0.30046123435097738</v>
       </c>
       <c r="I25" s="7">
-        <v>5287</v>
+        <v>5286</v>
       </c>
       <c r="J25" s="5">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K25" s="6">
-        <v>7.5468129373936071E-2</v>
+        <v>7.5293227393113879E-2</v>
       </c>
       <c r="L25" s="5">
         <v>31</v>
       </c>
       <c r="M25" s="10">
-        <v>5.1180452299999998E-3</v>
+        <v>5.1205814299999999E-3</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1713,25 +1826,25 @@
         <v>32</v>
       </c>
       <c r="E26" s="14">
-        <v>0.53409807134753562</v>
+        <v>0.53422412706416234</v>
       </c>
       <c r="F26" s="14">
-        <v>0.46590192865246438</v>
+        <v>0.46577587293583766</v>
       </c>
       <c r="G26" s="12">
-        <v>5855</v>
+        <v>5856</v>
       </c>
       <c r="H26" s="15">
-        <v>0.33253629376601196</v>
+        <v>0.33247950819672129</v>
       </c>
       <c r="I26" s="12">
         <v>7009</v>
       </c>
       <c r="J26" s="13">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K26" s="14">
-        <v>6.2633756598658871E-2</v>
+        <v>6.2491082893422742E-2</v>
       </c>
       <c r="L26" s="13">
         <v>30</v>
@@ -1748,37 +1861,37 @@
         <v>34</v>
       </c>
       <c r="C27" s="7">
-        <v>9590</v>
+        <v>9591</v>
       </c>
       <c r="D27" s="5">
         <v>32</v>
       </c>
       <c r="E27" s="6">
-        <v>0.54735186156266391</v>
+        <v>0.5473993288590604</v>
       </c>
       <c r="F27" s="6">
-        <v>0.45264813843733614</v>
+        <v>0.4526006711409396</v>
       </c>
       <c r="G27" s="7">
-        <v>7211</v>
+        <v>7213</v>
       </c>
       <c r="H27" s="8">
-        <v>0.34530578283178476</v>
+        <v>0.34521003743241369</v>
       </c>
       <c r="I27" s="7">
-        <v>8309</v>
+        <v>8310</v>
       </c>
       <c r="J27" s="5">
         <v>434</v>
       </c>
       <c r="K27" s="6">
-        <v>5.2232518955349617E-2</v>
+        <v>5.2226233453670279E-2</v>
       </c>
       <c r="L27" s="5">
         <v>30</v>
       </c>
       <c r="M27" s="10">
-        <v>3.1282585999999999E-3</v>
+        <v>3.12793243E-3</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1789,16 +1902,16 @@
         <v>35</v>
       </c>
       <c r="C28" s="12">
-        <v>8821</v>
+        <v>8820</v>
       </c>
       <c r="D28" s="13">
         <v>32</v>
       </c>
       <c r="E28" s="14">
-        <v>0.53119653245123755</v>
+        <v>0.53102897558749718</v>
       </c>
       <c r="F28" s="14">
-        <v>0.4688034675487624</v>
+        <v>0.46897102441250288</v>
       </c>
       <c r="G28" s="12">
         <v>6878</v>
@@ -1807,19 +1920,19 @@
         <v>0.30750218086653097</v>
       </c>
       <c r="I28" s="12">
-        <v>7428</v>
+        <v>7431</v>
       </c>
       <c r="J28" s="13">
         <v>366</v>
       </c>
       <c r="K28" s="14">
-        <v>4.9273021001615507E-2</v>
+        <v>4.9253128784820348E-2</v>
       </c>
       <c r="L28" s="13">
         <v>18</v>
       </c>
       <c r="M28" s="16">
-        <v>2.0405849599999999E-3</v>
+        <v>2.04081632E-3</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1836,25 +1949,25 @@
         <v>33</v>
       </c>
       <c r="E29" s="6">
-        <v>0.53675612602100353</v>
+        <v>0.53663943990665108</v>
       </c>
       <c r="F29" s="6">
-        <v>0.46324387397899652</v>
+        <v>0.46336056009334892</v>
       </c>
       <c r="G29" s="7">
         <v>6656</v>
       </c>
       <c r="H29" s="8">
-        <v>0.27223557692307693</v>
+        <v>0.27208533653846156</v>
       </c>
       <c r="I29" s="7">
-        <v>7081</v>
+        <v>7083</v>
       </c>
       <c r="J29" s="5">
         <v>397</v>
       </c>
       <c r="K29" s="6">
-        <v>5.6065527467871766E-2</v>
+        <v>5.6049696456303824E-2</v>
       </c>
       <c r="L29" s="5">
         <v>36</v>
@@ -1871,37 +1984,37 @@
         <v>37</v>
       </c>
       <c r="C30" s="12">
-        <v>9770</v>
+        <v>9768</v>
       </c>
       <c r="D30" s="13">
         <v>35</v>
       </c>
       <c r="E30" s="14">
-        <v>0.51779835390946505</v>
+        <v>0.51769911504424782</v>
       </c>
       <c r="F30" s="14">
-        <v>0.48220164609053495</v>
+        <v>0.48230088495575218</v>
       </c>
       <c r="G30" s="12">
-        <v>7613</v>
+        <v>7612</v>
       </c>
       <c r="H30" s="15">
-        <v>0.20517535794036518</v>
+        <v>0.20520231213872833</v>
       </c>
       <c r="I30" s="12">
-        <v>8038</v>
+        <v>8039</v>
       </c>
       <c r="J30" s="13">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="K30" s="14">
-        <v>5.7974620552376212E-2</v>
+        <v>5.8091802462992913E-2</v>
       </c>
       <c r="L30" s="13">
         <v>66</v>
       </c>
       <c r="M30" s="16">
-        <v>6.7553735899999997E-3</v>
+        <v>6.7567567499999997E-3</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1912,37 +2025,37 @@
         <v>38</v>
       </c>
       <c r="C31" s="7">
-        <v>12296</v>
+        <v>12294</v>
       </c>
       <c r="D31" s="5">
         <v>36</v>
       </c>
       <c r="E31" s="6">
-        <v>0.51205754925202318</v>
+        <v>0.51230479928051675</v>
       </c>
       <c r="F31" s="6">
-        <v>0.48794245074797676</v>
+        <v>0.4876952007194833</v>
       </c>
       <c r="G31" s="7">
-        <v>9770</v>
+        <v>9768</v>
       </c>
       <c r="H31" s="8">
-        <v>0.18669396110542477</v>
+        <v>0.18673218673218672</v>
       </c>
       <c r="I31" s="7">
-        <v>10068</v>
+        <v>10067</v>
       </c>
       <c r="J31" s="5">
         <v>674</v>
       </c>
       <c r="K31" s="6">
-        <v>6.6944775526420336E-2</v>
+        <v>6.6951425449488428E-2</v>
       </c>
       <c r="L31" s="5">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M31" s="10">
-        <v>6.4248536099999996E-3</v>
+        <v>6.5072393000000003E-3</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1953,16 +2066,16 @@
         <v>39</v>
       </c>
       <c r="C32" s="12">
-        <v>13063</v>
+        <v>13064</v>
       </c>
       <c r="D32" s="13">
         <v>37</v>
       </c>
       <c r="E32" s="14">
-        <v>0.51634741133933382</v>
+        <v>0.51630769230769236</v>
       </c>
       <c r="F32" s="14">
-        <v>0.48365258866066618</v>
+        <v>0.4836923076923077</v>
       </c>
       <c r="G32" s="12">
         <v>10369</v>
@@ -1971,19 +2084,19 @@
         <v>0.18188832095669785</v>
       </c>
       <c r="I32" s="12">
-        <v>10856</v>
+        <v>10858</v>
       </c>
       <c r="J32" s="13">
         <v>771</v>
       </c>
       <c r="K32" s="14">
-        <v>7.1020633750921144E-2</v>
+        <v>7.1007552035365629E-2</v>
       </c>
       <c r="L32" s="13">
         <v>107</v>
       </c>
       <c r="M32" s="16">
-        <v>8.1910740199999995E-3</v>
+        <v>8.1904470300000008E-3</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2000,25 +2113,25 @@
         <v>38</v>
       </c>
       <c r="E33" s="6">
-        <v>0.51923924680395495</v>
+        <v>0.51917627054600413</v>
       </c>
       <c r="F33" s="6">
-        <v>0.48076075319604511</v>
+        <v>0.48082372945399582</v>
       </c>
       <c r="G33" s="7">
-        <v>12616</v>
+        <v>12618</v>
       </c>
       <c r="H33" s="8">
-        <v>0.17541217501585288</v>
+        <v>0.17530511967031226</v>
       </c>
       <c r="I33" s="7">
-        <v>13481</v>
+        <v>13486</v>
       </c>
       <c r="J33" s="5">
         <v>874</v>
       </c>
       <c r="K33" s="6">
-        <v>6.4831985757733107E-2</v>
+        <v>6.4807948984131697E-2</v>
       </c>
       <c r="L33" s="5">
         <v>121</v>
@@ -2035,37 +2148,37 @@
         <v>41</v>
       </c>
       <c r="C34" s="19">
-        <v>26127</v>
+        <v>26126</v>
       </c>
       <c r="D34" s="20">
         <v>39</v>
       </c>
       <c r="E34" s="21">
-        <v>0.51029502151198525</v>
+        <v>0.510179778733866</v>
       </c>
       <c r="F34" s="21">
-        <v>0.48970497848801475</v>
+        <v>0.489820221266134</v>
       </c>
       <c r="G34" s="19">
-        <v>20102</v>
+        <v>20117</v>
       </c>
       <c r="H34" s="22">
-        <v>0.16625211421749081</v>
+        <v>0.16632698712531691</v>
       </c>
       <c r="I34" s="19">
-        <v>21549</v>
+        <v>21559</v>
       </c>
       <c r="J34" s="20">
         <v>1587</v>
       </c>
       <c r="K34" s="21">
-        <v>7.3646108868160934E-2</v>
+        <v>7.3611948606150557E-2</v>
       </c>
       <c r="L34" s="20">
         <v>239</v>
       </c>
       <c r="M34" s="23">
-        <v>9.1476250599999993E-3</v>
+        <v>9.1479751899999993E-3</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2082,31 +2195,31 @@
         <v>39</v>
       </c>
       <c r="E35" s="6">
-        <v>0.50857456768892706</v>
+        <v>0.50850291391993885</v>
       </c>
       <c r="F35" s="6">
-        <v>0.49142543231107289</v>
+        <v>0.49149708608006115</v>
       </c>
       <c r="G35" s="7">
-        <v>30890</v>
+        <v>30902</v>
       </c>
       <c r="H35" s="8">
-        <v>0.15995467788928455</v>
+        <v>0.15995728431816711</v>
       </c>
       <c r="I35" s="7">
-        <v>33713</v>
+        <v>33724</v>
       </c>
       <c r="J35" s="5">
-        <v>2327</v>
+        <v>2329</v>
       </c>
       <c r="K35" s="6">
-        <v>6.9023818704950612E-2</v>
+        <v>6.9060609654845215E-2</v>
       </c>
       <c r="L35" s="5">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="M35" s="10">
-        <v>1.0930000469999999E-2</v>
+        <v>1.0906239599999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2117,37 +2230,37 @@
         <v>43</v>
       </c>
       <c r="C36" s="12">
-        <v>74817</v>
+        <v>74811</v>
       </c>
       <c r="D36" s="13">
         <v>40</v>
       </c>
       <c r="E36" s="14">
-        <v>0.50149750862914166</v>
+        <v>0.5014774619889325</v>
       </c>
       <c r="F36" s="14">
-        <v>0.49850249137085834</v>
+        <v>0.49852253801106755</v>
       </c>
       <c r="G36" s="12">
-        <v>52413</v>
+        <v>52419</v>
       </c>
       <c r="H36" s="15">
-        <v>0.15486615915898727</v>
+        <v>0.15471489345466338</v>
       </c>
       <c r="I36" s="12">
-        <v>58145</v>
+        <v>58160</v>
       </c>
       <c r="J36" s="13">
-        <v>4101</v>
+        <v>4102</v>
       </c>
       <c r="K36" s="14">
-        <v>7.0530570126408121E-2</v>
+        <v>7.0529573590096289E-2</v>
       </c>
       <c r="L36" s="13">
         <v>991</v>
       </c>
       <c r="M36" s="16">
-        <v>1.3245652720000001E-2</v>
+        <v>1.324671505E-2</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2158,37 +2271,37 @@
         <v>44</v>
       </c>
       <c r="C37" s="7">
-        <v>111077</v>
+        <v>111078</v>
       </c>
       <c r="D37" s="5">
         <v>41</v>
       </c>
       <c r="E37" s="6">
-        <v>0.49726078255593892</v>
+        <v>0.49723821942120322</v>
       </c>
       <c r="F37" s="6">
-        <v>0.50273921744406114</v>
+        <v>0.50276178057879672</v>
       </c>
       <c r="G37" s="7">
-        <v>75643</v>
+        <v>75661</v>
       </c>
       <c r="H37" s="8">
-        <v>0.15774096743915497</v>
+        <v>0.15769022349691386</v>
       </c>
       <c r="I37" s="7">
-        <v>83954</v>
+        <v>84005</v>
       </c>
       <c r="J37" s="5">
-        <v>5915</v>
+        <v>5920</v>
       </c>
       <c r="K37" s="6">
-        <v>7.0455249303189846E-2</v>
+        <v>7.0471995714540797E-2</v>
       </c>
       <c r="L37" s="5">
         <v>1592</v>
       </c>
       <c r="M37" s="10">
-        <v>1.433240004E-2</v>
+        <v>1.433227101E-2</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2199,37 +2312,37 @@
         <v>45</v>
       </c>
       <c r="C38" s="19">
-        <v>125799</v>
+        <v>125794</v>
       </c>
       <c r="D38" s="20">
         <v>41</v>
       </c>
       <c r="E38" s="21">
-        <v>0.49125266345183355</v>
+        <v>0.49126840444109776</v>
       </c>
       <c r="F38" s="21">
-        <v>0.5087473365481664</v>
+        <v>0.50873159555890224</v>
       </c>
       <c r="G38" s="19">
-        <v>85229</v>
+        <v>85257</v>
       </c>
       <c r="H38" s="22">
-        <v>0.15217824918748313</v>
+        <v>0.15221037568762683</v>
       </c>
       <c r="I38" s="19">
-        <v>92757</v>
+        <v>92804</v>
       </c>
       <c r="J38" s="20">
-        <v>6834</v>
+        <v>6835</v>
       </c>
       <c r="K38" s="21">
-        <v>7.3676380219282647E-2</v>
+        <v>7.364984267919486E-2</v>
       </c>
       <c r="L38" s="20">
-        <v>1856</v>
+        <v>1858</v>
       </c>
       <c r="M38" s="23">
-        <v>1.475369438E-2</v>
+        <v>1.4770179810000001E-2</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2240,37 +2353,37 @@
         <v>46</v>
       </c>
       <c r="C39" s="7">
-        <v>127846</v>
+        <v>127839</v>
       </c>
       <c r="D39" s="5">
         <v>42</v>
       </c>
       <c r="E39" s="6">
-        <v>0.48458181071972595</v>
+        <v>0.48455740163384509</v>
       </c>
       <c r="F39" s="6">
-        <v>0.51541818928027405</v>
+        <v>0.51544259836615491</v>
       </c>
       <c r="G39" s="7">
-        <v>85802</v>
+        <v>85820</v>
       </c>
       <c r="H39" s="8">
-        <v>0.14842311368033378</v>
+        <v>0.14838033092519226</v>
       </c>
       <c r="I39" s="7">
-        <v>94482</v>
+        <v>94573</v>
       </c>
       <c r="J39" s="5">
-        <v>7475</v>
+        <v>7479</v>
       </c>
       <c r="K39" s="6">
-        <v>7.911559873838403E-2</v>
+        <v>7.9081767523500365E-2</v>
       </c>
       <c r="L39" s="5">
-        <v>2468</v>
+        <v>2469</v>
       </c>
       <c r="M39" s="10">
-        <v>1.930447569E-2</v>
+        <v>1.931335507E-2</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2281,37 +2394,37 @@
         <v>47</v>
       </c>
       <c r="C40" s="19">
-        <v>128456</v>
+        <v>128445</v>
       </c>
       <c r="D40" s="20">
         <v>43</v>
       </c>
       <c r="E40" s="21">
-        <v>0.47442268800852838</v>
+        <v>0.47441736499251375</v>
       </c>
       <c r="F40" s="21">
-        <v>0.52557731199147162</v>
+        <v>0.52558263500748625</v>
       </c>
       <c r="G40" s="19">
-        <v>86420</v>
+        <v>86453</v>
       </c>
       <c r="H40" s="22">
-        <v>0.14810229113631104</v>
+        <v>0.14810359386024777</v>
       </c>
       <c r="I40" s="19">
-        <v>93995</v>
+        <v>94072</v>
       </c>
       <c r="J40" s="20">
-        <v>8019</v>
+        <v>8024</v>
       </c>
       <c r="K40" s="21">
-        <v>8.5313048566413113E-2</v>
+        <v>8.5296368738838335E-2</v>
       </c>
       <c r="L40" s="20">
-        <v>3149</v>
+        <v>3150</v>
       </c>
       <c r="M40" s="23">
-        <v>2.4514230549999998E-2</v>
+        <v>2.4524115379999999E-2</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2322,37 +2435,37 @@
         <v>48</v>
       </c>
       <c r="C41" s="7">
-        <v>123290</v>
+        <v>123288</v>
       </c>
       <c r="D41" s="5">
         <v>44</v>
       </c>
       <c r="E41" s="6">
-        <v>0.46549936737276032</v>
+        <v>0.4654667156442594</v>
       </c>
       <c r="F41" s="6">
-        <v>0.53450063262723968</v>
+        <v>0.53453328435574055</v>
       </c>
       <c r="G41" s="7">
-        <v>82441</v>
+        <v>82508</v>
       </c>
       <c r="H41" s="8">
-        <v>0.15459540762484686</v>
+        <v>0.15460318999369757</v>
       </c>
       <c r="I41" s="7">
-        <v>89846</v>
+        <v>89976</v>
       </c>
       <c r="J41" s="5">
-        <v>8251</v>
+        <v>8258</v>
       </c>
       <c r="K41" s="6">
-        <v>9.1834917525543708E-2</v>
+        <v>9.1780030230283638E-2</v>
       </c>
       <c r="L41" s="5">
-        <v>3505</v>
+        <v>3510</v>
       </c>
       <c r="M41" s="10">
-        <v>2.8428907449999999E-2</v>
+        <v>2.846992408E-2</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2363,37 +2476,37 @@
         <v>49</v>
       </c>
       <c r="C42" s="19">
-        <v>128506</v>
+        <v>128489</v>
       </c>
       <c r="D42" s="20">
         <v>45</v>
       </c>
       <c r="E42" s="21">
-        <v>0.45916687570550607</v>
+        <v>0.45914247410880182</v>
       </c>
       <c r="F42" s="21">
-        <v>0.54083312429449393</v>
+        <v>0.54085752589119818</v>
       </c>
       <c r="G42" s="19">
-        <v>87469</v>
+        <v>87636</v>
       </c>
       <c r="H42" s="22">
-        <v>0.14207319164503995</v>
+        <v>0.14193938564060432</v>
       </c>
       <c r="I42" s="19">
-        <v>94164</v>
+        <v>94308</v>
       </c>
       <c r="J42" s="20">
-        <v>9088</v>
+        <v>9090</v>
       </c>
       <c r="K42" s="21">
-        <v>9.6512467609702224E-2</v>
+        <v>9.638630869067312E-2</v>
       </c>
       <c r="L42" s="20">
-        <v>4370</v>
+        <v>4372</v>
       </c>
       <c r="M42" s="23">
-        <v>3.4006194259999997E-2</v>
+        <v>3.402625905E-2</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2404,37 +2517,37 @@
         <v>50</v>
       </c>
       <c r="C43" s="7">
-        <v>156512</v>
+        <v>156489</v>
       </c>
       <c r="D43" s="5">
         <v>46</v>
       </c>
       <c r="E43" s="6">
-        <v>0.45384491686231626</v>
+        <v>0.45385125094085937</v>
       </c>
       <c r="F43" s="6">
-        <v>0.54615508313768368</v>
+        <v>0.54614874905914068</v>
       </c>
       <c r="G43" s="7">
-        <v>107365</v>
+        <v>107606</v>
       </c>
       <c r="H43" s="8">
-        <v>0.14663065244725934</v>
+        <v>0.14682266788097317</v>
       </c>
       <c r="I43" s="7">
-        <v>114700</v>
+        <v>114817</v>
       </c>
       <c r="J43" s="5">
-        <v>11157</v>
+        <v>11162</v>
       </c>
       <c r="K43" s="6">
-        <v>9.7271142109851785E-2</v>
+        <v>9.7215569123039275E-2</v>
       </c>
       <c r="L43" s="5">
-        <v>5598</v>
+        <v>5604</v>
       </c>
       <c r="M43" s="10">
-        <v>3.576722551E-2</v>
+        <v>3.5810823759999999E-2</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2445,37 +2558,37 @@
         <v>51</v>
       </c>
       <c r="C44" s="19">
-        <v>174930</v>
+        <v>174879</v>
       </c>
       <c r="D44" s="20">
         <v>46</v>
       </c>
       <c r="E44" s="21">
-        <v>0.45178930160539238</v>
+        <v>0.45180067363330167</v>
       </c>
       <c r="F44" s="21">
-        <v>0.54821069839460768</v>
+        <v>0.54819932636669833</v>
       </c>
       <c r="G44" s="19">
-        <v>118103</v>
+        <v>118376</v>
       </c>
       <c r="H44" s="22">
-        <v>0.1444586504999873</v>
+        <v>0.14488578765966073</v>
       </c>
       <c r="I44" s="19">
-        <v>126478</v>
+        <v>126789</v>
       </c>
       <c r="J44" s="20">
-        <v>12395</v>
+        <v>12425</v>
       </c>
       <c r="K44" s="21">
-        <v>9.8001233416088171E-2</v>
+        <v>9.799746034750649E-2</v>
       </c>
       <c r="L44" s="20">
-        <v>6265</v>
+        <v>6278</v>
       </c>
       <c r="M44" s="23">
-        <v>3.5814325729999999E-2</v>
+        <v>3.5899107380000003E-2</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2486,37 +2599,37 @@
         <v>52</v>
       </c>
       <c r="C45" s="7">
-        <v>139212</v>
+        <v>139154</v>
       </c>
       <c r="D45" s="5">
         <v>48</v>
       </c>
       <c r="E45" s="6">
-        <v>0.44487921307681183</v>
+        <v>0.44490430881661303</v>
       </c>
       <c r="F45" s="6">
-        <v>0.55512078692318823</v>
+        <v>0.55509569118338697</v>
       </c>
       <c r="G45" s="7">
-        <v>91379</v>
+        <v>91500</v>
       </c>
       <c r="H45" s="8">
-        <v>0.15780430952407007</v>
+        <v>0.1578360655737705</v>
       </c>
       <c r="I45" s="7">
-        <v>99948</v>
+        <v>100129</v>
       </c>
       <c r="J45" s="5">
-        <v>10916</v>
+        <v>10918</v>
       </c>
       <c r="K45" s="6">
-        <v>0.10921679273222075</v>
+        <v>0.10903933925236445</v>
       </c>
       <c r="L45" s="5">
-        <v>5559</v>
+        <v>5567</v>
       </c>
       <c r="M45" s="10">
-        <v>3.9931902419999998E-2</v>
+        <v>4.0006036469999999E-2</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2527,37 +2640,37 @@
         <v>53</v>
       </c>
       <c r="C46" s="19">
-        <v>123193</v>
+        <v>123151</v>
       </c>
       <c r="D46" s="20">
         <v>49</v>
       </c>
       <c r="E46" s="21">
-        <v>0.44119814008317232</v>
+        <v>0.44123981492855097</v>
       </c>
       <c r="F46" s="21">
-        <v>0.55880185991682763</v>
+        <v>0.55876018507144909</v>
       </c>
       <c r="G46" s="19">
-        <v>84273</v>
+        <v>84388</v>
       </c>
       <c r="H46" s="22">
-        <v>0.13417108682496173</v>
+        <v>0.13408304498269896</v>
       </c>
       <c r="I46" s="19">
-        <v>90311</v>
+        <v>90417</v>
       </c>
       <c r="J46" s="20">
-        <v>10790</v>
+        <v>10796</v>
       </c>
       <c r="K46" s="21">
-        <v>0.11947603281992226</v>
+        <v>0.1194023247840561</v>
       </c>
       <c r="L46" s="20">
-        <v>5541</v>
+        <v>5549</v>
       </c>
       <c r="M46" s="23">
-        <v>4.4978204930000001E-2</v>
+        <v>4.5058505409999998E-2</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2568,37 +2681,37 @@
         <v>1</v>
       </c>
       <c r="C47" s="27">
-        <v>145482</v>
+        <v>145533</v>
       </c>
       <c r="D47" s="28">
         <v>48</v>
       </c>
       <c r="E47" s="29">
-        <v>0.45082876759830781</v>
+        <v>0.45075187709288056</v>
       </c>
       <c r="F47" s="29">
-        <v>0.54917123240169219</v>
+        <v>0.54924812290711944</v>
       </c>
       <c r="G47" s="27">
-        <v>101571</v>
+        <v>101868</v>
       </c>
       <c r="H47" s="30">
-        <v>0.13187819357887587</v>
+        <v>0.13163113048258532</v>
       </c>
       <c r="I47" s="27">
-        <v>106772</v>
+        <v>107114</v>
       </c>
       <c r="J47" s="28">
-        <v>10832</v>
+        <v>10870</v>
       </c>
       <c r="K47" s="29">
-        <v>0.10144981830442439</v>
+        <v>0.10148066545923035</v>
       </c>
       <c r="L47" s="28">
-        <v>5534</v>
+        <v>5540</v>
       </c>
       <c r="M47" s="31">
-        <v>3.8039070119999997E-2</v>
+        <v>3.8066967620000003E-2</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2609,37 +2722,37 @@
         <v>2</v>
       </c>
       <c r="C48" s="19">
-        <v>119004</v>
+        <v>119049</v>
       </c>
       <c r="D48" s="20">
         <v>48</v>
       </c>
       <c r="E48" s="21">
-        <v>0.45425150005516468</v>
+        <v>0.45421304465861273</v>
       </c>
       <c r="F48" s="21">
-        <v>0.54574849994483532</v>
+        <v>0.54578695534138721</v>
       </c>
       <c r="G48" s="19">
-        <v>81142</v>
+        <v>81219</v>
       </c>
       <c r="H48" s="22">
-        <v>0.15761258041458184</v>
+        <v>0.15754934190275674</v>
       </c>
       <c r="I48" s="19">
-        <v>87319</v>
+        <v>87471</v>
       </c>
       <c r="J48" s="20">
-        <v>9563</v>
+        <v>9577</v>
       </c>
       <c r="K48" s="21">
-        <v>0.10951797432403028</v>
+        <v>0.1094877159287078</v>
       </c>
       <c r="L48" s="20">
-        <v>4921</v>
+        <v>4936</v>
       </c>
       <c r="M48" s="23">
-        <v>4.1351551200000003E-2</v>
+        <v>4.1461919040000003E-2</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2650,37 +2763,37 @@
         <v>3</v>
       </c>
       <c r="C49" s="7">
-        <v>95576</v>
+        <v>95602</v>
       </c>
       <c r="D49" s="5">
         <v>48</v>
       </c>
       <c r="E49" s="6">
-        <v>0.45815396302861483</v>
+        <v>0.45801293208020843</v>
       </c>
       <c r="F49" s="6">
-        <v>0.54184603697138511</v>
+        <v>0.54198706791979157</v>
       </c>
       <c r="G49" s="7">
-        <v>66808</v>
+        <v>66919</v>
       </c>
       <c r="H49" s="8">
-        <v>0.15670279008501975</v>
+        <v>0.15674173254232729</v>
       </c>
       <c r="I49" s="7">
-        <v>72476</v>
+        <v>72567</v>
       </c>
       <c r="J49" s="5">
-        <v>8509</v>
+        <v>8521</v>
       </c>
       <c r="K49" s="6">
-        <v>0.11740438214029472</v>
+        <v>0.11742251987818154</v>
       </c>
       <c r="L49" s="5">
-        <v>3923</v>
+        <v>3928</v>
       </c>
       <c r="M49" s="10">
-        <v>4.1045869249999999E-2</v>
+        <v>4.1087006539999998E-2</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2691,37 +2804,37 @@
         <v>4</v>
       </c>
       <c r="C50" s="19">
-        <v>78244</v>
+        <v>78250</v>
       </c>
       <c r="D50" s="20">
         <v>48</v>
       </c>
       <c r="E50" s="21">
-        <v>0.46313334364208031</v>
+        <v>0.46314311115692364</v>
       </c>
       <c r="F50" s="21">
-        <v>0.53686665635791975</v>
+        <v>0.53685688884307636</v>
       </c>
       <c r="G50" s="19">
-        <v>55387</v>
+        <v>55437</v>
       </c>
       <c r="H50" s="22">
-        <v>0.15942369147995017</v>
+        <v>0.15958655771416203</v>
       </c>
       <c r="I50" s="19">
-        <v>61176</v>
+        <v>61286</v>
       </c>
       <c r="J50" s="20">
-        <v>7219</v>
+        <v>7235</v>
       </c>
       <c r="K50" s="21">
-        <v>0.11800379233686413</v>
+        <v>0.11805306268968443</v>
       </c>
       <c r="L50" s="20">
-        <v>2974</v>
+        <v>2989</v>
       </c>
       <c r="M50" s="23">
-        <v>3.8009304219999998E-2</v>
+        <v>3.8198083059999999E-2</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2738,31 +2851,31 @@
         <v>46</v>
       </c>
       <c r="E51" s="6">
-        <v>0.47373841400617922</v>
+        <v>0.4736061915833164</v>
       </c>
       <c r="F51" s="6">
-        <v>0.52626158599382078</v>
+        <v>0.5263938084166836</v>
       </c>
       <c r="G51" s="7">
-        <v>46542</v>
+        <v>46708</v>
       </c>
       <c r="H51" s="8">
-        <v>0.15979115637488719</v>
+        <v>0.16003682452684764</v>
       </c>
       <c r="I51" s="7">
-        <v>51107</v>
+        <v>51280</v>
       </c>
       <c r="J51" s="5">
-        <v>6173</v>
+        <v>6189</v>
       </c>
       <c r="K51" s="6">
-        <v>0.12078580233627488</v>
+        <v>0.12069032761310453</v>
       </c>
       <c r="L51" s="5">
-        <v>2130</v>
+        <v>2143</v>
       </c>
       <c r="M51" s="10">
-        <v>3.293695588E-2</v>
+        <v>3.3137979550000002E-2</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2773,37 +2886,37 @@
         <v>6</v>
       </c>
       <c r="C52" s="19">
-        <v>50848</v>
+        <v>50861</v>
       </c>
       <c r="D52" s="20">
         <v>45</v>
       </c>
       <c r="E52" s="21">
-        <v>0.48375394009079553</v>
+        <v>0.48369899122024695</v>
       </c>
       <c r="F52" s="21">
-        <v>0.51624605990920447</v>
+        <v>0.51630100877975305</v>
       </c>
       <c r="G52" s="19">
-        <v>37393</v>
+        <v>37430</v>
       </c>
       <c r="H52" s="22">
-        <v>0.16337282379054904</v>
+        <v>0.16334491049959926</v>
       </c>
       <c r="I52" s="19">
-        <v>40456</v>
+        <v>40510</v>
       </c>
       <c r="J52" s="20">
-        <v>4950</v>
+        <v>4967</v>
       </c>
       <c r="K52" s="21">
-        <v>0.12235515127545976</v>
+        <v>0.12261170081461367</v>
       </c>
       <c r="L52" s="20">
-        <v>1598</v>
+        <v>1612</v>
       </c>
       <c r="M52" s="23">
-        <v>3.142699811E-2</v>
+        <v>3.169422543E-2</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2814,37 +2927,37 @@
         <v>7</v>
       </c>
       <c r="C53" s="7">
-        <v>52492</v>
+        <v>52491</v>
       </c>
       <c r="D53" s="5">
         <v>44</v>
       </c>
       <c r="E53" s="6">
-        <v>0.49179919046979609</v>
+        <v>0.49175107427869857</v>
       </c>
       <c r="F53" s="6">
-        <v>0.50820080953020397</v>
+        <v>0.50824892572130143</v>
       </c>
       <c r="G53" s="7">
-        <v>38691</v>
+        <v>38866</v>
       </c>
       <c r="H53" s="8">
-        <v>0.16233749450776666</v>
+        <v>0.16235269901713581</v>
       </c>
       <c r="I53" s="7">
-        <v>42067</v>
+        <v>42093</v>
       </c>
       <c r="J53" s="5">
-        <v>4882</v>
+        <v>4896</v>
       </c>
       <c r="K53" s="6">
-        <v>0.11605296313024462</v>
+        <v>0.11631387641650631</v>
       </c>
       <c r="L53" s="5">
-        <v>1387</v>
+        <v>1399</v>
       </c>
       <c r="M53" s="10">
-        <v>2.642307399E-2</v>
+        <v>2.6652187989999999E-2</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2855,37 +2968,37 @@
         <v>8</v>
       </c>
       <c r="C54" s="19">
-        <v>56460</v>
+        <v>56450</v>
       </c>
       <c r="D54" s="20">
         <v>42</v>
       </c>
       <c r="E54" s="21">
-        <v>0.49708779366973621</v>
+        <v>0.4971050896976823</v>
       </c>
       <c r="F54" s="21">
-        <v>0.50291220633026379</v>
+        <v>0.5028949103023177</v>
       </c>
       <c r="G54" s="19">
-        <v>41547</v>
+        <v>41792</v>
       </c>
       <c r="H54" s="22">
-        <v>0.15738801838881267</v>
+        <v>0.15715926493108728</v>
       </c>
       <c r="I54" s="19">
-        <v>44892</v>
+        <v>44959</v>
       </c>
       <c r="J54" s="20">
-        <v>4516</v>
+        <v>4538</v>
       </c>
       <c r="K54" s="21">
-        <v>0.10059698832754166</v>
+        <v>0.10093640872795213</v>
       </c>
       <c r="L54" s="20">
-        <v>1127</v>
+        <v>1146</v>
       </c>
       <c r="M54" s="23">
-        <v>1.9961034360000001E-2</v>
+        <v>2.030115146E-2</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2896,37 +3009,37 @@
         <v>9</v>
       </c>
       <c r="C55" s="7">
-        <v>58502</v>
+        <v>58500</v>
       </c>
       <c r="D55" s="5">
         <v>40</v>
       </c>
       <c r="E55" s="6">
-        <v>0.50705097337827609</v>
+        <v>0.50700810015993947</v>
       </c>
       <c r="F55" s="6">
-        <v>0.49294902662172385</v>
+        <v>0.49299189984006053</v>
       </c>
       <c r="G55" s="7">
-        <v>43205</v>
+        <v>43481</v>
       </c>
       <c r="H55" s="8">
-        <v>0.15470431663001968</v>
+        <v>0.15432027782249719</v>
       </c>
       <c r="I55" s="7">
-        <v>46193</v>
+        <v>46285</v>
       </c>
       <c r="J55" s="5">
-        <v>4076</v>
+        <v>4097</v>
       </c>
       <c r="K55" s="6">
-        <v>8.8238477691425107E-2</v>
+        <v>8.8516798098736096E-2</v>
       </c>
       <c r="L55" s="5">
-        <v>939</v>
+        <v>954</v>
       </c>
       <c r="M55" s="10">
-        <v>1.6050733300000002E-2</v>
+        <v>1.6307692299999999E-2</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2937,37 +3050,37 @@
         <v>10</v>
       </c>
       <c r="C56" s="19">
-        <v>71452</v>
+        <v>71456</v>
       </c>
       <c r="D56" s="20">
         <v>39</v>
       </c>
       <c r="E56" s="21">
-        <v>0.50269904582035485</v>
+        <v>0.50264251990698328</v>
       </c>
       <c r="F56" s="21">
-        <v>0.49730095417964509</v>
+        <v>0.49735748009301672</v>
       </c>
       <c r="G56" s="19">
-        <v>52136</v>
+        <v>52352</v>
       </c>
       <c r="H56" s="22">
-        <v>0.15597667638483964</v>
+        <v>0.15577246332518338</v>
       </c>
       <c r="I56" s="19">
-        <v>55073</v>
+        <v>55244</v>
       </c>
       <c r="J56" s="32">
-        <v>4516</v>
+        <v>4543</v>
       </c>
       <c r="K56" s="21">
-        <v>8.2000254208051127E-2</v>
+        <v>8.2235174860618349E-2</v>
       </c>
       <c r="L56" s="32">
-        <v>970</v>
+        <v>995</v>
       </c>
       <c r="M56" s="23">
-        <v>1.3575547219999999E-2</v>
+        <v>1.392465293E-2</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2978,37 +3091,37 @@
         <v>11</v>
       </c>
       <c r="C57" s="7">
-        <v>92789</v>
+        <v>92775</v>
       </c>
       <c r="D57" s="5">
         <v>39</v>
       </c>
       <c r="E57" s="6">
-        <v>0.50402246508803883</v>
+        <v>0.50399566278124153</v>
       </c>
       <c r="F57" s="6">
-        <v>0.49597753491196112</v>
+        <v>0.49600433721875847</v>
       </c>
       <c r="G57" s="7">
-        <v>66913</v>
+        <v>67329</v>
       </c>
       <c r="H57" s="8">
-        <v>0.15363232854602243</v>
+        <v>0.15394555095129886</v>
       </c>
       <c r="I57" s="7">
-        <v>70649</v>
+        <v>70998</v>
       </c>
       <c r="J57" s="5">
-        <v>5228</v>
+        <v>5286</v>
       </c>
       <c r="K57" s="6">
-        <v>7.3999631983467568E-2</v>
+        <v>7.4452801487365841E-2</v>
       </c>
       <c r="L57" s="5">
-        <v>1092</v>
+        <v>1132</v>
       </c>
       <c r="M57" s="10">
-        <v>1.1768636359999999E-2</v>
+        <v>1.2201562920000001E-2</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3019,37 +3132,37 @@
         <v>12</v>
       </c>
       <c r="C58" s="19">
-        <v>116631</v>
+        <v>116596</v>
       </c>
       <c r="D58" s="20">
         <v>38</v>
       </c>
       <c r="E58" s="21">
-        <v>0.50801229472811726</v>
+        <v>0.50803533648241384</v>
       </c>
       <c r="F58" s="21">
-        <v>0.49198770527188274</v>
+        <v>0.49196466351758622</v>
       </c>
       <c r="G58" s="19">
-        <v>80233</v>
+        <v>81523</v>
       </c>
       <c r="H58" s="22">
-        <v>0.15568407014570065</v>
+        <v>0.15692503955938814</v>
       </c>
       <c r="I58" s="19">
-        <v>87289</v>
+        <v>88163</v>
       </c>
       <c r="J58" s="32">
-        <v>6071</v>
+        <v>6211</v>
       </c>
       <c r="K58" s="21">
-        <v>6.9550573382671357E-2</v>
+        <v>7.0449054592062424E-2</v>
       </c>
       <c r="L58" s="32">
-        <v>1213</v>
+        <v>1309</v>
       </c>
       <c r="M58" s="23">
-        <v>1.040032238E-2</v>
+        <v>1.122680023E-2</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3060,37 +3173,37 @@
         <v>13</v>
       </c>
       <c r="C59" s="7">
-        <v>110441</v>
+        <v>110406</v>
       </c>
       <c r="D59" s="5">
         <v>39</v>
       </c>
       <c r="E59" s="6">
-        <v>0.51235389580788093</v>
+        <v>0.51229676372158339</v>
       </c>
       <c r="F59" s="6">
-        <v>0.48764610419211901</v>
+        <v>0.48770323627841661</v>
       </c>
       <c r="G59" s="7">
-        <v>73414</v>
+        <v>74931</v>
       </c>
       <c r="H59" s="8">
-        <v>0.15215081592066909</v>
+        <v>0.15314088961844896</v>
       </c>
       <c r="I59" s="7">
-        <v>80286</v>
+        <v>81602</v>
       </c>
       <c r="J59" s="5">
-        <v>5868</v>
+        <v>6057</v>
       </c>
       <c r="K59" s="6">
-        <v>7.3088707869367012E-2</v>
+        <v>7.422612190877674E-2</v>
       </c>
       <c r="L59" s="5">
-        <v>1113</v>
+        <v>1247</v>
       </c>
       <c r="M59" s="10">
-        <v>1.007777908E-2</v>
+        <v>1.1294676010000001E-2</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3101,37 +3214,37 @@
         <v>14</v>
       </c>
       <c r="C60" s="19">
-        <v>118588</v>
+        <v>118519</v>
       </c>
       <c r="D60" s="20">
         <v>39</v>
       </c>
       <c r="E60" s="21">
-        <v>0.50755633288617952</v>
+        <v>0.50745685555102593</v>
       </c>
       <c r="F60" s="21">
-        <v>0.49244366711382043</v>
+        <v>0.49254314444897407</v>
       </c>
       <c r="G60" s="19">
-        <v>77964</v>
+        <v>79809</v>
       </c>
       <c r="H60" s="22">
-        <v>0.1378071930634652</v>
+        <v>0.13860592163791052</v>
       </c>
       <c r="I60" s="19">
-        <v>85169</v>
+        <v>86806</v>
       </c>
       <c r="J60" s="32">
-        <v>6070</v>
+        <v>6415</v>
       </c>
       <c r="K60" s="21">
-        <v>7.1270063051110152E-2</v>
+        <v>7.3900421629841256E-2</v>
       </c>
       <c r="L60" s="32">
-        <v>849</v>
+        <v>1092</v>
       </c>
       <c r="M60" s="23">
-        <v>7.1592403900000001E-3</v>
+        <v>9.2137125600000001E-3</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3142,37 +3255,37 @@
         <v>15</v>
       </c>
       <c r="C61" s="7">
-        <v>142522</v>
+        <v>142548</v>
       </c>
       <c r="D61" s="5">
         <v>38</v>
       </c>
       <c r="E61" s="6">
-        <v>0.51026303678266716</v>
+        <v>0.51020350420518767</v>
       </c>
       <c r="F61" s="6">
-        <v>0.48973696321733279</v>
+        <v>0.48979649579481233</v>
       </c>
       <c r="G61" s="7">
-        <v>87364</v>
+        <v>91504</v>
       </c>
       <c r="H61" s="8">
-        <v>0.15506387070189093</v>
+        <v>0.15574182549396748</v>
       </c>
       <c r="I61" s="7">
-        <v>99114</v>
+        <v>102046</v>
       </c>
       <c r="J61" s="5">
-        <v>5536</v>
+        <v>6382</v>
       </c>
       <c r="K61" s="6">
-        <v>5.5854874185281594E-2</v>
+        <v>6.2540422946514324E-2</v>
       </c>
       <c r="L61" s="5">
-        <v>535</v>
+        <v>936</v>
       </c>
       <c r="M61" s="10">
-        <v>3.7538064200000002E-3</v>
+        <v>6.5662092699999997E-3</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3183,37 +3296,78 @@
         <v>16</v>
       </c>
       <c r="C62" s="19">
-        <v>144068</v>
+        <v>145336</v>
       </c>
       <c r="D62" s="20">
         <v>37</v>
       </c>
       <c r="E62" s="21">
-        <v>0.51943199853926425</v>
+        <v>0.51936001779272867</v>
       </c>
       <c r="F62" s="21">
-        <v>0.48056800146073569</v>
+        <v>0.48063998220727139</v>
       </c>
       <c r="G62" s="19">
-        <v>75752</v>
+        <v>89223</v>
       </c>
       <c r="H62" s="22">
-        <v>0.16787675572922167</v>
+        <v>0.16311937504903445</v>
       </c>
       <c r="I62" s="19">
-        <v>92276</v>
+        <v>102023</v>
       </c>
       <c r="J62" s="32">
-        <v>4004</v>
+        <v>5759</v>
       </c>
       <c r="K62" s="21">
-        <v>4.3391564437123414E-2</v>
+        <v>5.6448055830548016E-2</v>
       </c>
       <c r="L62" s="32">
-        <v>161</v>
+        <v>530</v>
       </c>
       <c r="M62" s="23">
-        <v>1.11752783E-3</v>
+        <v>3.64672207E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="25">
+        <v>2021</v>
+      </c>
+      <c r="B63" s="25">
+        <v>17</v>
+      </c>
+      <c r="C63" s="27">
+        <v>124151</v>
+      </c>
+      <c r="D63" s="28">
+        <v>37</v>
+      </c>
+      <c r="E63" s="29">
+        <v>0.52079548324548042</v>
+      </c>
+      <c r="F63" s="29">
+        <v>0.47920451675451958</v>
+      </c>
+      <c r="G63" s="27">
+        <v>67889</v>
+      </c>
+      <c r="H63" s="30">
+        <v>0.16970348657367174</v>
+      </c>
+      <c r="I63" s="27">
+        <v>81126</v>
+      </c>
+      <c r="J63" s="34">
+        <v>3655</v>
+      </c>
+      <c r="K63" s="29">
+        <v>4.5053373764267927E-2</v>
+      </c>
+      <c r="L63" s="34">
+        <v>163</v>
+      </c>
+      <c r="M63" s="31">
+        <v>1.31291733E-3</v>
       </c>
     </row>
   </sheetData>
@@ -3224,13 +3378,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EE44EF-F204-44BC-9DFD-46318AB81991}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="33"/>
     <col min="2" max="2" width="13.85546875" style="33" customWidth="1"/>
@@ -3285,960 +3439,989 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B3" s="35">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>158</v>
+      </c>
+      <c r="G3">
+        <v>138</v>
+      </c>
+      <c r="H3">
+        <v>96</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>77</v>
+      </c>
+      <c r="F4">
+        <v>235</v>
+      </c>
+      <c r="G4">
+        <v>206</v>
+      </c>
+      <c r="H4">
+        <v>138</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>112</v>
+      </c>
+      <c r="F5">
+        <v>237</v>
+      </c>
+      <c r="G5">
+        <v>253</v>
+      </c>
+      <c r="H5">
+        <v>153</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>115</v>
+      </c>
+      <c r="F6">
+        <v>274</v>
+      </c>
+      <c r="G6">
+        <v>286</v>
+      </c>
+      <c r="H6">
+        <v>175</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>207</v>
+      </c>
+      <c r="F7">
+        <v>487</v>
+      </c>
+      <c r="G7">
+        <v>502</v>
+      </c>
+      <c r="H7">
+        <v>352</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>263</v>
+      </c>
+      <c r="F8">
+        <v>674</v>
+      </c>
+      <c r="G8">
+        <v>781</v>
+      </c>
+      <c r="H8">
+        <v>559</v>
+      </c>
+      <c r="I8" s="35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9">
+        <v>430</v>
+      </c>
+      <c r="F9">
+        <v>1050</v>
+      </c>
+      <c r="G9">
+        <v>1412</v>
+      </c>
+      <c r="H9">
+        <v>1123</v>
+      </c>
+      <c r="I9" s="35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10">
+        <v>64</v>
+      </c>
+      <c r="D10">
+        <v>49</v>
+      </c>
+      <c r="E10">
+        <v>544</v>
+      </c>
+      <c r="F10">
+        <v>1492</v>
+      </c>
+      <c r="G10">
+        <v>2083</v>
+      </c>
+      <c r="H10">
+        <v>1683</v>
+      </c>
+      <c r="I10" s="35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11">
+        <v>65</v>
+      </c>
+      <c r="D11">
+        <v>58</v>
+      </c>
+      <c r="E11">
+        <v>602</v>
+      </c>
+      <c r="F11">
+        <v>1685</v>
+      </c>
+      <c r="G11">
+        <v>2380</v>
+      </c>
+      <c r="H11">
+        <v>2043</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <v>68</v>
+      </c>
+      <c r="E12">
+        <v>569</v>
+      </c>
+      <c r="F12">
+        <v>1711</v>
+      </c>
+      <c r="G12">
+        <v>2562</v>
+      </c>
+      <c r="H12">
+        <v>2494</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13">
+        <v>54</v>
+      </c>
+      <c r="D13">
+        <v>54</v>
+      </c>
+      <c r="E13">
+        <v>602</v>
+      </c>
+      <c r="F13">
+        <v>1660</v>
+      </c>
+      <c r="G13">
+        <v>2840</v>
+      </c>
+      <c r="H13">
+        <v>2808</v>
+      </c>
+      <c r="I13" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14">
+        <v>62</v>
+      </c>
+      <c r="D14">
+        <v>68</v>
+      </c>
+      <c r="E14">
+        <v>557</v>
+      </c>
+      <c r="F14">
+        <v>1682</v>
+      </c>
+      <c r="G14">
+        <v>2845</v>
+      </c>
+      <c r="H14">
+        <v>3039</v>
+      </c>
+      <c r="I14" s="35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15">
+        <v>58</v>
+      </c>
+      <c r="D15">
+        <v>58</v>
+      </c>
+      <c r="E15">
+        <v>591</v>
+      </c>
+      <c r="F15">
+        <v>1656</v>
+      </c>
+      <c r="G15">
+        <v>3147</v>
+      </c>
+      <c r="H15">
+        <v>3573</v>
+      </c>
+      <c r="I15" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16">
+        <v>70</v>
+      </c>
+      <c r="D16">
+        <v>66</v>
+      </c>
+      <c r="E16">
+        <v>670</v>
+      </c>
+      <c r="F16">
+        <v>1949</v>
+      </c>
+      <c r="G16">
+        <v>3899</v>
+      </c>
+      <c r="H16">
+        <v>4500</v>
+      </c>
+      <c r="I16" s="35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17">
+        <v>79</v>
+      </c>
+      <c r="D17">
+        <v>87</v>
+      </c>
+      <c r="E17">
+        <v>705</v>
+      </c>
+      <c r="F17">
+        <v>2166</v>
+      </c>
+      <c r="G17">
+        <v>4338</v>
+      </c>
+      <c r="H17">
+        <v>5044</v>
+      </c>
+      <c r="I17" s="35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18">
+        <v>54</v>
+      </c>
+      <c r="D18">
+        <v>49</v>
+      </c>
+      <c r="E18">
+        <v>593</v>
+      </c>
+      <c r="F18">
+        <v>1830</v>
+      </c>
+      <c r="G18">
+        <v>3846</v>
+      </c>
+      <c r="H18">
+        <v>4532</v>
+      </c>
+      <c r="I18" s="35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19">
+        <v>74</v>
+      </c>
+      <c r="D19">
+        <v>51</v>
+      </c>
+      <c r="E19">
+        <v>605</v>
+      </c>
+      <c r="F19">
+        <v>1869</v>
+      </c>
+      <c r="G19">
+        <v>3784</v>
+      </c>
+      <c r="H19">
+        <v>4399</v>
+      </c>
+      <c r="I19" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20">
+        <v>64</v>
+      </c>
+      <c r="D20">
+        <v>33</v>
+      </c>
+      <c r="E20">
+        <v>567</v>
+      </c>
+      <c r="F20">
+        <v>1770</v>
+      </c>
+      <c r="G20">
+        <v>3862</v>
+      </c>
+      <c r="H20">
+        <v>4573</v>
+      </c>
+      <c r="I20" s="35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21">
+        <v>58</v>
+      </c>
+      <c r="D21">
+        <v>47</v>
+      </c>
+      <c r="E21">
+        <v>508</v>
+      </c>
+      <c r="F21">
+        <v>1547</v>
+      </c>
+      <c r="G21">
+        <v>3295</v>
+      </c>
+      <c r="H21">
+        <v>4118</v>
+      </c>
+      <c r="I21" s="35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22">
+        <v>39</v>
+      </c>
+      <c r="D22">
+        <v>36</v>
+      </c>
+      <c r="E22">
+        <v>388</v>
+      </c>
+      <c r="F22">
+        <v>1411</v>
+      </c>
+      <c r="G22">
+        <v>3052</v>
+      </c>
+      <c r="H22">
+        <v>3592</v>
+      </c>
+      <c r="I22" s="35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23">
+        <v>34</v>
+      </c>
+      <c r="D23">
+        <v>30</v>
+      </c>
+      <c r="E23">
+        <v>389</v>
+      </c>
+      <c r="F23">
+        <v>1182</v>
+      </c>
+      <c r="G23">
+        <v>2697</v>
+      </c>
+      <c r="H23">
+        <v>2901</v>
+      </c>
+      <c r="I23" s="35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24">
+        <v>43</v>
+      </c>
+      <c r="D24">
+        <v>38</v>
+      </c>
+      <c r="E24">
+        <v>346</v>
+      </c>
+      <c r="F24">
+        <v>1079</v>
+      </c>
+      <c r="G24">
+        <v>2255</v>
+      </c>
+      <c r="H24">
+        <v>2427</v>
+      </c>
+      <c r="I24" s="35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25">
+        <v>38</v>
+      </c>
+      <c r="D25">
+        <v>23</v>
+      </c>
+      <c r="E25">
+        <v>286</v>
+      </c>
+      <c r="F25">
+        <v>934</v>
+      </c>
+      <c r="G25">
+        <v>1865</v>
+      </c>
+      <c r="H25">
+        <v>1821</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26">
+        <v>35</v>
+      </c>
+      <c r="D26">
+        <v>22</v>
+      </c>
+      <c r="E26">
+        <v>298</v>
+      </c>
+      <c r="F26">
+        <v>998</v>
+      </c>
+      <c r="G26">
+        <v>1927</v>
+      </c>
+      <c r="H26">
+        <v>1615</v>
+      </c>
+      <c r="I26" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="33">
-        <v>12</v>
-      </c>
-      <c r="D3" s="33">
-        <v>12</v>
-      </c>
-      <c r="E3" s="33">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27">
+        <v>44</v>
+      </c>
+      <c r="D27">
+        <v>31</v>
+      </c>
+      <c r="E27">
+        <v>305</v>
+      </c>
+      <c r="F27">
+        <v>1019</v>
+      </c>
+      <c r="G27">
+        <v>1706</v>
+      </c>
+      <c r="H27">
+        <v>1433</v>
+      </c>
+      <c r="I27" s="35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28">
+        <v>49</v>
+      </c>
+      <c r="D28">
+        <v>28</v>
+      </c>
+      <c r="E28">
+        <v>314</v>
+      </c>
+      <c r="F28">
+        <v>971</v>
+      </c>
+      <c r="G28">
+        <v>1539</v>
+      </c>
+      <c r="H28">
+        <v>1196</v>
+      </c>
+      <c r="I28" s="35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29">
         <v>50</v>
       </c>
-      <c r="F3" s="33">
-        <v>157</v>
-      </c>
-      <c r="G3" s="33">
-        <v>138</v>
-      </c>
-      <c r="H3" s="33">
+      <c r="D29">
+        <v>36</v>
+      </c>
+      <c r="E29">
+        <v>376</v>
+      </c>
+      <c r="F29">
+        <v>1259</v>
+      </c>
+      <c r="G29">
+        <v>1614</v>
+      </c>
+      <c r="H29">
+        <v>1208</v>
+      </c>
+      <c r="I29" s="35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30">
+        <v>75</v>
+      </c>
+      <c r="D30">
+        <v>67</v>
+      </c>
+      <c r="E30">
+        <v>444</v>
+      </c>
+      <c r="F30">
+        <v>1479</v>
+      </c>
+      <c r="G30">
+        <v>1989</v>
+      </c>
+      <c r="H30">
+        <v>1230</v>
+      </c>
+      <c r="I30" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31">
+        <v>80</v>
+      </c>
+      <c r="D31">
+        <v>76</v>
+      </c>
+      <c r="E31">
+        <v>569</v>
+      </c>
+      <c r="F31">
+        <v>1764</v>
+      </c>
+      <c r="G31">
+        <v>2297</v>
+      </c>
+      <c r="H31">
+        <v>1424</v>
+      </c>
+      <c r="I31" s="35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32">
+        <v>82</v>
+      </c>
+      <c r="D32">
+        <v>86</v>
+      </c>
+      <c r="E32">
+        <v>529</v>
+      </c>
+      <c r="F32">
+        <v>1757</v>
+      </c>
+      <c r="G32">
+        <v>2315</v>
+      </c>
+      <c r="H32">
+        <v>1288</v>
+      </c>
+      <c r="I32" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33">
+        <v>90</v>
+      </c>
+      <c r="D33">
+        <v>63</v>
+      </c>
+      <c r="E33">
+        <v>646</v>
+      </c>
+      <c r="F33">
+        <v>1965</v>
+      </c>
+      <c r="G33">
+        <v>2397</v>
+      </c>
+      <c r="H33">
+        <v>1252</v>
+      </c>
+      <c r="I33" s="35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34">
+        <v>85</v>
+      </c>
+      <c r="D34">
+        <v>78</v>
+      </c>
+      <c r="E34">
+        <v>657</v>
+      </c>
+      <c r="F34">
+        <v>1883</v>
+      </c>
+      <c r="G34">
+        <v>2462</v>
+      </c>
+      <c r="H34">
+        <v>1214</v>
+      </c>
+      <c r="I34" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35">
+        <v>77</v>
+      </c>
+      <c r="D35">
+        <v>71</v>
+      </c>
+      <c r="E35">
+        <v>596</v>
+      </c>
+      <c r="F35">
+        <v>1758</v>
+      </c>
+      <c r="G35">
+        <v>2160</v>
+      </c>
+      <c r="H35">
+        <v>1094</v>
+      </c>
+      <c r="I35" s="35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36">
+        <v>50</v>
+      </c>
+      <c r="D36">
+        <v>74</v>
+      </c>
+      <c r="E36">
+        <v>388</v>
+      </c>
+      <c r="F36">
+        <v>1002</v>
+      </c>
+      <c r="G36">
+        <v>1420</v>
+      </c>
+      <c r="H36">
+        <v>718</v>
+      </c>
+      <c r="I36" s="35" t="s">
         <v>96</v>
-      </c>
-      <c r="I3" s="34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B4" s="35">
-        <v>38</v>
-      </c>
-      <c r="C4" s="33">
-        <v>8</v>
-      </c>
-      <c r="D4" s="33">
-        <v>10</v>
-      </c>
-      <c r="E4" s="33">
-        <v>77</v>
-      </c>
-      <c r="F4" s="33">
-        <v>235</v>
-      </c>
-      <c r="G4" s="33">
-        <v>206</v>
-      </c>
-      <c r="H4" s="33">
-        <v>138</v>
-      </c>
-      <c r="I4" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B5" s="35">
-        <v>39</v>
-      </c>
-      <c r="C5" s="33">
-        <v>9</v>
-      </c>
-      <c r="D5" s="33">
-        <v>7</v>
-      </c>
-      <c r="E5" s="33">
-        <v>112</v>
-      </c>
-      <c r="F5" s="33">
-        <v>237</v>
-      </c>
-      <c r="G5" s="33">
-        <v>253</v>
-      </c>
-      <c r="H5" s="33">
-        <v>153</v>
-      </c>
-      <c r="I5" s="34" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B6" s="35">
-        <v>40</v>
-      </c>
-      <c r="C6" s="33">
-        <v>15</v>
-      </c>
-      <c r="D6" s="33">
-        <v>9</v>
-      </c>
-      <c r="E6" s="33">
-        <v>115</v>
-      </c>
-      <c r="F6" s="33">
-        <v>274</v>
-      </c>
-      <c r="G6" s="33">
-        <v>286</v>
-      </c>
-      <c r="H6" s="33">
-        <v>175</v>
-      </c>
-      <c r="I6" s="34" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B7" s="35">
-        <v>41</v>
-      </c>
-      <c r="C7" s="33">
-        <v>21</v>
-      </c>
-      <c r="D7" s="33">
-        <v>17</v>
-      </c>
-      <c r="E7" s="33">
-        <v>207</v>
-      </c>
-      <c r="F7" s="33">
-        <v>488</v>
-      </c>
-      <c r="G7" s="33">
-        <v>502</v>
-      </c>
-      <c r="H7" s="33">
-        <v>351</v>
-      </c>
-      <c r="I7" s="34" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B8" s="35">
-        <v>42</v>
-      </c>
-      <c r="C8" s="33">
-        <v>24</v>
-      </c>
-      <c r="D8" s="33">
-        <v>25</v>
-      </c>
-      <c r="E8" s="33">
-        <v>263</v>
-      </c>
-      <c r="F8" s="33">
-        <v>672</v>
-      </c>
-      <c r="G8" s="33">
-        <v>781</v>
-      </c>
-      <c r="H8" s="33">
-        <v>559</v>
-      </c>
-      <c r="I8" s="34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B9" s="35">
-        <v>43</v>
-      </c>
-      <c r="C9" s="33">
-        <v>50</v>
-      </c>
-      <c r="D9" s="33">
-        <v>30</v>
-      </c>
-      <c r="E9" s="33">
-        <v>429</v>
-      </c>
-      <c r="F9" s="33">
-        <v>1050</v>
-      </c>
-      <c r="G9" s="33">
-        <v>1412</v>
-      </c>
-      <c r="H9" s="33">
-        <v>1123</v>
-      </c>
-      <c r="I9" s="34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B10" s="35">
-        <v>44</v>
-      </c>
-      <c r="C10" s="33">
-        <v>64</v>
-      </c>
-      <c r="D10" s="33">
-        <v>49</v>
-      </c>
-      <c r="E10" s="33">
-        <v>544</v>
-      </c>
-      <c r="F10" s="33">
-        <v>1492</v>
-      </c>
-      <c r="G10" s="33">
-        <v>2079</v>
-      </c>
-      <c r="H10" s="33">
-        <v>1682</v>
-      </c>
-      <c r="I10" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B11" s="35">
-        <v>45</v>
-      </c>
-      <c r="C11" s="33">
-        <v>65</v>
-      </c>
-      <c r="D11" s="33">
-        <v>58</v>
-      </c>
-      <c r="E11" s="33">
-        <v>602</v>
-      </c>
-      <c r="F11" s="33">
-        <v>1683</v>
-      </c>
-      <c r="G11" s="33">
-        <v>2380</v>
-      </c>
-      <c r="H11" s="33">
-        <v>2044</v>
-      </c>
-      <c r="I11" s="34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B12" s="35">
-        <v>46</v>
-      </c>
-      <c r="C12" s="33">
-        <v>64</v>
-      </c>
-      <c r="D12" s="33">
-        <v>68</v>
-      </c>
-      <c r="E12" s="33">
-        <v>569</v>
-      </c>
-      <c r="F12" s="33">
-        <v>1707</v>
-      </c>
-      <c r="G12" s="33">
-        <v>2562</v>
-      </c>
-      <c r="H12" s="33">
-        <v>2494</v>
-      </c>
-      <c r="I12" s="34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B13" s="35">
-        <v>47</v>
-      </c>
-      <c r="C13" s="33">
-        <v>54</v>
-      </c>
-      <c r="D13" s="33">
-        <v>54</v>
-      </c>
-      <c r="E13" s="33">
-        <v>601</v>
-      </c>
-      <c r="F13" s="33">
-        <v>1658</v>
-      </c>
-      <c r="G13" s="33">
-        <v>2839</v>
-      </c>
-      <c r="H13" s="33">
-        <v>2807</v>
-      </c>
-      <c r="I13" s="34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B14" s="35">
-        <v>48</v>
-      </c>
-      <c r="C14" s="33">
-        <v>62</v>
-      </c>
-      <c r="D14" s="33">
-        <v>68</v>
-      </c>
-      <c r="E14" s="33">
-        <v>557</v>
-      </c>
-      <c r="F14" s="33">
-        <v>1678</v>
-      </c>
-      <c r="G14" s="33">
-        <v>2843</v>
-      </c>
-      <c r="H14" s="33">
-        <v>3038</v>
-      </c>
-      <c r="I14" s="34" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B15" s="35">
-        <v>49</v>
-      </c>
-      <c r="C15" s="33">
-        <v>58</v>
-      </c>
-      <c r="D15" s="33">
-        <v>58</v>
-      </c>
-      <c r="E15" s="33">
-        <v>591</v>
-      </c>
-      <c r="F15" s="33">
-        <v>1653</v>
-      </c>
-      <c r="G15" s="33">
-        <v>3145</v>
-      </c>
-      <c r="H15" s="33">
-        <v>3576</v>
-      </c>
-      <c r="I15" s="34" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B16" s="35">
-        <v>50</v>
-      </c>
-      <c r="C16" s="33">
-        <v>70</v>
-      </c>
-      <c r="D16" s="33">
-        <v>66</v>
-      </c>
-      <c r="E16" s="33">
-        <v>670</v>
-      </c>
-      <c r="F16" s="33">
-        <v>1946</v>
-      </c>
-      <c r="G16" s="33">
-        <v>3899</v>
-      </c>
-      <c r="H16" s="33">
-        <v>4498</v>
-      </c>
-      <c r="I16" s="34" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B17" s="35">
-        <v>51</v>
-      </c>
-      <c r="C17" s="33">
-        <v>78</v>
-      </c>
-      <c r="D17" s="33">
-        <v>87</v>
-      </c>
-      <c r="E17" s="33">
-        <v>703</v>
-      </c>
-      <c r="F17" s="33">
-        <v>2159</v>
-      </c>
-      <c r="G17" s="33">
-        <v>4325</v>
-      </c>
-      <c r="H17" s="33">
-        <v>5037</v>
-      </c>
-      <c r="I17" s="34" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B18" s="35">
-        <v>52</v>
-      </c>
-      <c r="C18" s="33">
-        <v>54</v>
-      </c>
-      <c r="D18" s="33">
-        <v>49</v>
-      </c>
-      <c r="E18" s="33">
-        <v>595</v>
-      </c>
-      <c r="F18" s="33">
-        <v>1828</v>
-      </c>
-      <c r="G18" s="33">
-        <v>3842</v>
-      </c>
-      <c r="H18" s="33">
-        <v>4534</v>
-      </c>
-      <c r="I18" s="34" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="35">
-        <v>2020</v>
-      </c>
-      <c r="B19" s="35">
-        <v>53</v>
-      </c>
-      <c r="C19" s="33">
-        <v>74</v>
-      </c>
-      <c r="D19" s="33">
-        <v>51</v>
-      </c>
-      <c r="E19" s="33">
-        <v>604</v>
-      </c>
-      <c r="F19" s="33">
-        <v>1869</v>
-      </c>
-      <c r="G19" s="33">
-        <v>3783</v>
-      </c>
-      <c r="H19" s="33">
-        <v>4395</v>
-      </c>
-      <c r="I19" s="34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B20" s="35">
-        <v>1</v>
-      </c>
-      <c r="C20" s="33">
-        <v>64</v>
-      </c>
-      <c r="D20" s="33">
-        <v>33</v>
-      </c>
-      <c r="E20" s="33">
-        <v>568</v>
-      </c>
-      <c r="F20" s="33">
-        <v>1754</v>
-      </c>
-      <c r="G20" s="33">
-        <v>3851</v>
-      </c>
-      <c r="H20" s="33">
-        <v>4560</v>
-      </c>
-      <c r="I20" s="34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B21" s="35">
-        <v>2</v>
-      </c>
-      <c r="C21" s="33">
-        <v>58</v>
-      </c>
-      <c r="D21" s="33">
-        <v>47</v>
-      </c>
-      <c r="E21" s="33">
-        <v>508</v>
-      </c>
-      <c r="F21" s="33">
-        <v>1546</v>
-      </c>
-      <c r="G21" s="33">
-        <v>3289</v>
-      </c>
-      <c r="H21" s="33">
-        <v>4111</v>
-      </c>
-      <c r="I21" s="34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B22" s="35">
-        <v>3</v>
-      </c>
-      <c r="C22" s="33">
-        <v>39</v>
-      </c>
-      <c r="D22" s="33">
-        <v>36</v>
-      </c>
-      <c r="E22" s="33">
-        <v>388</v>
-      </c>
-      <c r="F22" s="33">
-        <v>1409</v>
-      </c>
-      <c r="G22" s="33">
-        <v>3049</v>
-      </c>
-      <c r="H22" s="33">
-        <v>3585</v>
-      </c>
-      <c r="I22" s="34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B23" s="35">
-        <v>4</v>
-      </c>
-      <c r="C23" s="33">
-        <v>34</v>
-      </c>
-      <c r="D23" s="33">
-        <v>30</v>
-      </c>
-      <c r="E23" s="33">
-        <v>388</v>
-      </c>
-      <c r="F23" s="33">
-        <v>1179</v>
-      </c>
-      <c r="G23" s="33">
-        <v>2693</v>
-      </c>
-      <c r="H23" s="33">
-        <v>2893</v>
-      </c>
-      <c r="I23" s="34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B24" s="35">
-        <v>5</v>
-      </c>
-      <c r="C24" s="33">
-        <v>43</v>
-      </c>
-      <c r="D24" s="33">
-        <v>38</v>
-      </c>
-      <c r="E24" s="33">
-        <v>344</v>
-      </c>
-      <c r="F24" s="33">
-        <v>1080</v>
-      </c>
-      <c r="G24" s="33">
-        <v>2248</v>
-      </c>
-      <c r="H24" s="33">
-        <v>2418</v>
-      </c>
-      <c r="I24" s="34" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B25" s="35">
-        <v>6</v>
-      </c>
-      <c r="C25" s="33">
-        <v>38</v>
-      </c>
-      <c r="D25" s="33">
-        <v>23</v>
-      </c>
-      <c r="E25" s="33">
-        <v>284</v>
-      </c>
-      <c r="F25" s="33">
-        <v>934</v>
-      </c>
-      <c r="G25" s="33">
-        <v>1859</v>
-      </c>
-      <c r="H25" s="33">
-        <v>1812</v>
-      </c>
-      <c r="I25" s="34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B26" s="35">
-        <v>7</v>
-      </c>
-      <c r="C26" s="33">
-        <v>35</v>
-      </c>
-      <c r="D26" s="33">
-        <v>22</v>
-      </c>
-      <c r="E26" s="33">
-        <v>298</v>
-      </c>
-      <c r="F26" s="33">
-        <v>992</v>
-      </c>
-      <c r="G26" s="33">
-        <v>1922</v>
-      </c>
-      <c r="H26" s="33">
-        <v>1612</v>
-      </c>
-      <c r="I26" s="34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B27" s="35">
-        <v>8</v>
-      </c>
-      <c r="C27" s="33">
-        <v>43</v>
-      </c>
-      <c r="D27" s="33">
-        <v>31</v>
-      </c>
-      <c r="E27" s="33">
-        <v>303</v>
-      </c>
-      <c r="F27" s="33">
-        <v>1013</v>
-      </c>
-      <c r="G27" s="33">
-        <v>1700</v>
-      </c>
-      <c r="H27" s="33">
-        <v>1426</v>
-      </c>
-      <c r="I27" s="34" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B28" s="35">
-        <v>9</v>
-      </c>
-      <c r="C28" s="33">
-        <v>49</v>
-      </c>
-      <c r="D28" s="33">
-        <v>28</v>
-      </c>
-      <c r="E28" s="33">
-        <v>314</v>
-      </c>
-      <c r="F28" s="33">
-        <v>967</v>
-      </c>
-      <c r="G28" s="33">
-        <v>1531</v>
-      </c>
-      <c r="H28" s="33">
-        <v>1187</v>
-      </c>
-      <c r="I28" s="34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B29" s="35">
-        <v>10</v>
-      </c>
-      <c r="C29" s="33">
-        <v>50</v>
-      </c>
-      <c r="D29" s="33">
-        <v>36</v>
-      </c>
-      <c r="E29" s="33">
-        <v>375</v>
-      </c>
-      <c r="F29" s="33">
-        <v>1247</v>
-      </c>
-      <c r="G29" s="33">
-        <v>1604</v>
-      </c>
-      <c r="H29" s="33">
-        <v>1204</v>
-      </c>
-      <c r="I29" s="34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B30" s="35">
-        <v>11</v>
-      </c>
-      <c r="C30" s="33">
-        <v>74</v>
-      </c>
-      <c r="D30" s="33">
-        <v>65</v>
-      </c>
-      <c r="E30" s="33">
-        <v>438</v>
-      </c>
-      <c r="F30" s="33">
-        <v>1460</v>
-      </c>
-      <c r="G30" s="33">
-        <v>1968</v>
-      </c>
-      <c r="H30" s="33">
-        <v>1221</v>
-      </c>
-      <c r="I30" s="34" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B31" s="35">
-        <v>12</v>
-      </c>
-      <c r="C31" s="33">
-        <v>78</v>
-      </c>
-      <c r="D31" s="33">
-        <v>74</v>
-      </c>
-      <c r="E31" s="33">
-        <v>552</v>
-      </c>
-      <c r="F31" s="33">
-        <v>1728</v>
-      </c>
-      <c r="G31" s="33">
-        <v>2244</v>
-      </c>
-      <c r="H31" s="33">
-        <v>1394</v>
-      </c>
-      <c r="I31" s="34" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B32" s="35">
-        <v>13</v>
-      </c>
-      <c r="C32" s="33">
-        <v>81</v>
-      </c>
-      <c r="D32" s="33">
-        <v>84</v>
-      </c>
-      <c r="E32" s="33">
-        <v>520</v>
-      </c>
-      <c r="F32" s="33">
-        <v>1695</v>
-      </c>
-      <c r="G32" s="33">
-        <v>2228</v>
-      </c>
-      <c r="H32" s="33">
-        <v>1259</v>
-      </c>
-      <c r="I32" s="34" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B33" s="35">
-        <v>14</v>
-      </c>
-      <c r="C33" s="33">
-        <v>87</v>
-      </c>
-      <c r="D33" s="33">
-        <v>58</v>
-      </c>
-      <c r="E33" s="33">
-        <v>629</v>
-      </c>
-      <c r="F33" s="33">
-        <v>1845</v>
-      </c>
-      <c r="G33" s="33">
-        <v>2248</v>
-      </c>
-      <c r="H33" s="33">
-        <v>1201</v>
-      </c>
-      <c r="I33" s="34" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B34" s="35">
-        <v>15</v>
-      </c>
-      <c r="C34" s="33">
-        <v>82</v>
-      </c>
-      <c r="D34" s="33">
-        <v>77</v>
-      </c>
-      <c r="E34" s="33">
-        <v>593</v>
-      </c>
-      <c r="F34" s="33">
-        <v>1585</v>
-      </c>
-      <c r="G34" s="33">
-        <v>2098</v>
-      </c>
-      <c r="H34" s="33">
-        <v>1096</v>
-      </c>
-      <c r="I34" s="34" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="35">
-        <v>2021</v>
-      </c>
-      <c r="B35" s="35">
-        <v>16</v>
-      </c>
-      <c r="C35" s="33">
-        <v>70</v>
-      </c>
-      <c r="D35" s="33">
-        <v>63</v>
-      </c>
-      <c r="E35" s="33">
-        <v>437</v>
-      </c>
-      <c r="F35" s="33">
-        <v>1102</v>
-      </c>
-      <c r="G35" s="33">
-        <v>1522</v>
-      </c>
-      <c r="H35" s="33">
-        <v>807</v>
-      </c>
-      <c r="I35" s="34" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>